<commit_message>
RTAC: updated the model to accomodate for 2x UDP frames (Banshee & PHIL) Problems with RTAC real time communication started. Seems to work as HMI shows something changing.
</commit_message>
<xml_diff>
--- a/SimulationTools/RTAC/MGC_SEL_programming.xlsx
+++ b/SimulationTools/RTAC/MGC_SEL_programming.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H48" sqref="H2:H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +407,7 @@
         <v>,IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",D2,")",G2,"),")</f>
+        <f t="shared" ref="H2:H48" si="1">CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",D2,")",G2,"),")</f>
         <v>(ID:=1,CBID:=301,Flow:=ADR(HMI1.Flow_301),Status:=ADR(HMI1.CB301_Closed),IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)),</v>
       </c>
     </row>
@@ -419,11 +419,11 @@
         <v>302</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C48" si="1">CONCATENATE("HMI1.Flow_",B3)</f>
+        <f t="shared" ref="C3:C48" si="2">CONCATENATE("HMI1.Flow_",B3)</f>
         <v>HMI1.Flow_302</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D48" si="2">CONCATENATE("HMI1.CB",B3,"_Closed")</f>
+        <f t="shared" ref="D3:D48" si="3">CONCATENATE("HMI1.CB",B3,"_Closed")</f>
         <v>HMI1.CB302_Closed</v>
       </c>
       <c r="E3" t="str">
@@ -431,15 +431,15 @@
         <v>HMI1.CB302_Cmd</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F48" si="3">CONCATENATE("CB", B3, "_MODBUS")</f>
+        <f t="shared" ref="F3:F48" si="4">CONCATENATE("CB", B3, "_MODBUS")</f>
         <v>CB302_MODBUS</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G48" si="4">IF(E3="","",CONCATENATE(",IOCCmd:=ADR(",E3,"),MBCmd:=ADR(",F3,".CMD),MBRst:=ADR(",F3,".RST)"))</f>
+        <f t="shared" ref="G3:G48" si="5">IF(E3="","",CONCATENATE(",IOCCmd:=ADR(",E3,"),MBCmd:=ADR(",F3,".CMD),MBRst:=ADR(",F3,".RST)"))</f>
         <v>,IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)</v>
       </c>
       <c r="H3" t="str">
-        <f>CONCATENATE("(ID:=",A3,",CBID:=",B3,",Flow:=ADR(HMI1.Flow_",B3,"),Status:=ADR(",D3,")",G3,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=2,CBID:=302,Flow:=ADR(HMI1.Flow_302),Status:=ADR(HMI1.CB302_Closed),IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)),</v>
       </c>
     </row>
@@ -451,11 +451,11 @@
         <v>303</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_303</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB303_Closed</v>
       </c>
       <c r="E4" t="str">
@@ -463,15 +463,15 @@
         <v>HMI1.CB303_Cmd</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB303_MODBUS</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)</v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE("(ID:=",A4,",CBID:=",B4,",Flow:=ADR(HMI1.Flow_",B4,"),Status:=ADR(",D4,")",G4,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=3,CBID:=303,Flow:=ADR(HMI1.Flow_303),Status:=ADR(HMI1.CB303_Closed),IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)),</v>
       </c>
     </row>
@@ -483,11 +483,11 @@
         <v>304</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_304</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB304_Closed</v>
       </c>
       <c r="E5" t="str">
@@ -495,15 +495,15 @@
         <v>HMI1.CB304_Cmd</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB304_MODBUS</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)</v>
       </c>
       <c r="H5" t="str">
-        <f>CONCATENATE("(ID:=",A5,",CBID:=",B5,",Flow:=ADR(HMI1.Flow_",B5,"),Status:=ADR(",D5,")",G5,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=4,CBID:=304,Flow:=ADR(HMI1.Flow_304),Status:=ADR(HMI1.CB304_Closed),IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)),</v>
       </c>
     </row>
@@ -515,11 +515,11 @@
         <v>305</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_305</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB305_Closed</v>
       </c>
       <c r="E6" t="str">
@@ -527,15 +527,15 @@
         <v>HMI1.CB305_Cmd</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB305_MODBUS</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("(ID:=",A6,",CBID:=",B6,",Flow:=ADR(HMI1.Flow_",B6,"),Status:=ADR(",D6,")",G6,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=5,CBID:=305,Flow:=ADR(HMI1.Flow_305),Status:=ADR(HMI1.CB305_Closed),IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)),</v>
       </c>
     </row>
@@ -547,23 +547,23 @@
         <v>306</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_306</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB306_Closed</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB306_MODBUS</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H7" t="str">
-        <f>CONCATENATE("(ID:=",A7,",CBID:=",B7,",Flow:=ADR(HMI1.Flow_",B7,"),Status:=ADR(",D7,")",G7,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=6,CBID:=306,Flow:=ADR(HMI1.Flow_306),Status:=ADR(HMI1.CB306_Closed)),</v>
       </c>
     </row>
@@ -575,23 +575,23 @@
         <v>307</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_307</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB307_Closed</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB307_MODBUS</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H8" t="str">
-        <f>CONCATENATE("(ID:=",A8,",CBID:=",B8,",Flow:=ADR(HMI1.Flow_",B8,"),Status:=ADR(",D8,")",G8,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=7,CBID:=307,Flow:=ADR(HMI1.Flow_307),Status:=ADR(HMI1.CB307_Closed)),</v>
       </c>
     </row>
@@ -603,23 +603,23 @@
         <v>308</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_308</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB308_Closed</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB308_MODBUS</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H9" t="str">
-        <f>CONCATENATE("(ID:=",A9,",CBID:=",B9,",Flow:=ADR(HMI1.Flow_",B9,"),Status:=ADR(",D9,")",G9,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=8,CBID:=308,Flow:=ADR(HMI1.Flow_308),Status:=ADR(HMI1.CB308_Closed)),</v>
       </c>
     </row>
@@ -631,23 +631,23 @@
         <v>309</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_309</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB309_Closed</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB309_MODBUS</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H10" t="str">
-        <f>CONCATENATE("(ID:=",A10,",CBID:=",B10,",Flow:=ADR(HMI1.Flow_",B10,"),Status:=ADR(",D10,")",G10,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=9,CBID:=309,Flow:=ADR(HMI1.Flow_309),Status:=ADR(HMI1.CB309_Closed)),</v>
       </c>
     </row>
@@ -659,11 +659,11 @@
         <v>201</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_201</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB201_Closed</v>
       </c>
       <c r="E11" t="str">
@@ -671,15 +671,15 @@
         <v>HMI1.CB201_Cmd</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB201_MODBUS</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)</v>
       </c>
       <c r="H11" t="str">
-        <f>CONCATENATE("(ID:=",A11,",CBID:=",B11,",Flow:=ADR(HMI1.Flow_",B11,"),Status:=ADR(",D11,")",G11,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=10,CBID:=201,Flow:=ADR(HMI1.Flow_201),Status:=ADR(HMI1.CB201_Closed),IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)),</v>
       </c>
     </row>
@@ -691,11 +691,11 @@
         <v>202</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_202</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB202_Closed</v>
       </c>
       <c r="E12" t="str">
@@ -703,15 +703,15 @@
         <v>HMI1.CB202_Cmd</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB202_MODBUS</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)</v>
       </c>
       <c r="H12" t="str">
-        <f>CONCATENATE("(ID:=",A12,",CBID:=",B12,",Flow:=ADR(HMI1.Flow_",B12,"),Status:=ADR(",D12,")",G12,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=11,CBID:=202,Flow:=ADR(HMI1.Flow_202),Status:=ADR(HMI1.CB202_Closed),IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)),</v>
       </c>
     </row>
@@ -723,11 +723,11 @@
         <v>203</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_203</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB203_Closed</v>
       </c>
       <c r="E13" t="str">
@@ -735,15 +735,15 @@
         <v>HMI1.CB203_Cmd</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB203_MODBUS</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)</v>
       </c>
       <c r="H13" t="str">
-        <f>CONCATENATE("(ID:=",A13,",CBID:=",B13,",Flow:=ADR(HMI1.Flow_",B13,"),Status:=ADR(",D13,")",G13,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=12,CBID:=203,Flow:=ADR(HMI1.Flow_203),Status:=ADR(HMI1.CB203_Closed),IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)),</v>
       </c>
     </row>
@@ -755,23 +755,23 @@
         <v>204</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_204</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB204_Closed</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB204_MODBUS</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H14" t="str">
-        <f>CONCATENATE("(ID:=",A14,",CBID:=",B14,",Flow:=ADR(HMI1.Flow_",B14,"),Status:=ADR(",D14,")",G14,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=13,CBID:=204,Flow:=ADR(HMI1.Flow_204),Status:=ADR(HMI1.CB204_Closed)),</v>
       </c>
     </row>
@@ -783,23 +783,23 @@
         <v>205</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_205</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB205_Closed</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB205_MODBUS</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H15" t="str">
-        <f>CONCATENATE("(ID:=",A15,",CBID:=",B15,",Flow:=ADR(HMI1.Flow_",B15,"),Status:=ADR(",D15,")",G15,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=14,CBID:=205,Flow:=ADR(HMI1.Flow_205),Status:=ADR(HMI1.CB205_Closed)),</v>
       </c>
     </row>
@@ -811,23 +811,23 @@
         <v>206</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_206</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB206_Closed</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB206_MODBUS</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H16" t="str">
-        <f>CONCATENATE("(ID:=",A16,",CBID:=",B16,",Flow:=ADR(HMI1.Flow_",B16,"),Status:=ADR(",D16,")",G16,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=15,CBID:=206,Flow:=ADR(HMI1.Flow_206),Status:=ADR(HMI1.CB206_Closed)),</v>
       </c>
     </row>
@@ -839,23 +839,23 @@
         <v>207</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_207</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB207_Closed</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB207_MODBUS</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H17" t="str">
-        <f>CONCATENATE("(ID:=",A17,",CBID:=",B17,",Flow:=ADR(HMI1.Flow_",B17,"),Status:=ADR(",D17,")",G17,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=16,CBID:=207,Flow:=ADR(HMI1.Flow_207),Status:=ADR(HMI1.CB207_Closed)),</v>
       </c>
     </row>
@@ -867,23 +867,23 @@
         <v>208</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_208</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB208_Closed</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB208_MODBUS</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H18" t="str">
-        <f>CONCATENATE("(ID:=",A18,",CBID:=",B18,",Flow:=ADR(HMI1.Flow_",B18,"),Status:=ADR(",D18,")",G18,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=17,CBID:=208,Flow:=ADR(HMI1.Flow_208),Status:=ADR(HMI1.CB208_Closed)),</v>
       </c>
     </row>
@@ -895,23 +895,23 @@
         <v>209</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_209</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB209_Closed</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB209_MODBUS</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H19" t="str">
-        <f>CONCATENATE("(ID:=",A19,",CBID:=",B19,",Flow:=ADR(HMI1.Flow_",B19,"),Status:=ADR(",D19,")",G19,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=18,CBID:=209,Flow:=ADR(HMI1.Flow_209),Status:=ADR(HMI1.CB209_Closed)),</v>
       </c>
     </row>
@@ -923,23 +923,23 @@
         <v>210</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_210</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB210_Closed</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB210_MODBUS</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H20" t="str">
-        <f>CONCATENATE("(ID:=",A20,",CBID:=",B20,",Flow:=ADR(HMI1.Flow_",B20,"),Status:=ADR(",D20,")",G20,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=19,CBID:=210,Flow:=ADR(HMI1.Flow_210),Status:=ADR(HMI1.CB210_Closed)),</v>
       </c>
     </row>
@@ -951,23 +951,23 @@
         <v>211</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_211</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB211_Closed</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB211_MODBUS</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H21" t="str">
-        <f>CONCATENATE("(ID:=",A21,",CBID:=",B21,",Flow:=ADR(HMI1.Flow_",B21,"),Status:=ADR(",D21,")",G21,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=20,CBID:=211,Flow:=ADR(HMI1.Flow_211),Status:=ADR(HMI1.CB211_Closed)),</v>
       </c>
     </row>
@@ -979,23 +979,23 @@
         <v>212</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_212</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB212_Closed</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB212_MODBUS</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H22" t="str">
-        <f>CONCATENATE("(ID:=",A22,",CBID:=",B22,",Flow:=ADR(HMI1.Flow_",B22,"),Status:=ADR(",D22,")",G22,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=21,CBID:=212,Flow:=ADR(HMI1.Flow_212),Status:=ADR(HMI1.CB212_Closed)),</v>
       </c>
     </row>
@@ -1007,11 +1007,11 @@
         <v>213</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_213</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB213_Closed</v>
       </c>
       <c r="E23" t="str">
@@ -1019,15 +1019,15 @@
         <v>HMI1.CB213_Cmd</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB213_MODBUS</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)</v>
       </c>
       <c r="H23" t="str">
-        <f>CONCATENATE("(ID:=",A23,",CBID:=",B23,",Flow:=ADR(HMI1.Flow_",B23,"),Status:=ADR(",D23,")",G23,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=22,CBID:=213,Flow:=ADR(HMI1.Flow_213),Status:=ADR(HMI1.CB213_Closed),IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1039,23 +1039,23 @@
         <v>214</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_214</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB214_Closed</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB214_MODBUS</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H24" t="str">
-        <f>CONCATENATE("(ID:=",A24,",CBID:=",B24,",Flow:=ADR(HMI1.Flow_",B24,"),Status:=ADR(",D24,")",G24,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=23,CBID:=214,Flow:=ADR(HMI1.Flow_214),Status:=ADR(HMI1.CB214_Closed)),</v>
       </c>
     </row>
@@ -1067,23 +1067,23 @@
         <v>215</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_215</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB215_Closed</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB215_MODBUS</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H25" t="str">
-        <f>CONCATENATE("(ID:=",A25,",CBID:=",B25,",Flow:=ADR(HMI1.Flow_",B25,"),Status:=ADR(",D25,")",G25,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=24,CBID:=215,Flow:=ADR(HMI1.Flow_215),Status:=ADR(HMI1.CB215_Closed)),</v>
       </c>
     </row>
@@ -1095,11 +1095,11 @@
         <v>216</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_216</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB216_Closed</v>
       </c>
       <c r="E26" t="str">
@@ -1107,15 +1107,15 @@
         <v>HMI1.CB216_Cmd</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB216_MODBUS</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)</v>
       </c>
       <c r="H26" t="str">
-        <f>CONCATENATE("(ID:=",A26,",CBID:=",B26,",Flow:=ADR(HMI1.Flow_",B26,"),Status:=ADR(",D26,")",G26,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=25,CBID:=216,Flow:=ADR(HMI1.Flow_216),Status:=ADR(HMI1.CB216_Closed),IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1127,11 +1127,11 @@
         <v>217</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_217</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB217_Closed</v>
       </c>
       <c r="E27" t="str">
@@ -1139,15 +1139,15 @@
         <v>HMI1.CB217_Cmd</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB217_MODBUS</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)</v>
       </c>
       <c r="H27" t="str">
-        <f>CONCATENATE("(ID:=",A27,",CBID:=",B27,",Flow:=ADR(HMI1.Flow_",B27,"),Status:=ADR(",D27,")",G27,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=26,CBID:=217,Flow:=ADR(HMI1.Flow_217),Status:=ADR(HMI1.CB217_Closed),IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1159,23 +1159,23 @@
         <v>218</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_218</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB218_Closed</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB218_MODBUS</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H28" t="str">
-        <f>CONCATENATE("(ID:=",A28,",CBID:=",B28,",Flow:=ADR(HMI1.Flow_",B28,"),Status:=ADR(",D28,")",G28,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=27,CBID:=218,Flow:=ADR(HMI1.Flow_218),Status:=ADR(HMI1.CB218_Closed)),</v>
       </c>
     </row>
@@ -1187,23 +1187,23 @@
         <v>219</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_219</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB219_Closed</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB219_MODBUS</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H29" t="str">
-        <f>CONCATENATE("(ID:=",A29,",CBID:=",B29,",Flow:=ADR(HMI1.Flow_",B29,"),Status:=ADR(",D29,")",G29,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=28,CBID:=219,Flow:=ADR(HMI1.Flow_219),Status:=ADR(HMI1.CB219_Closed)),</v>
       </c>
     </row>
@@ -1215,11 +1215,11 @@
         <v>101</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_101</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB101_Closed</v>
       </c>
       <c r="E30" t="str">
@@ -1227,15 +1227,15 @@
         <v>HMI1.CB101_Cmd</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB101_MODBUS</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)</v>
       </c>
       <c r="H30" t="str">
-        <f>CONCATENATE("(ID:=",A30,",CBID:=",B30,",Flow:=ADR(HMI1.Flow_",B30,"),Status:=ADR(",D30,")",G30,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=29,CBID:=101,Flow:=ADR(HMI1.Flow_101),Status:=ADR(HMI1.CB101_Closed),IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1247,11 +1247,11 @@
         <v>102</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_102</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB102_Closed</v>
       </c>
       <c r="E31" t="str">
@@ -1259,15 +1259,15 @@
         <v>HMI1.CB102_Cmd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB102_MODBUS</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)</v>
       </c>
       <c r="H31" t="str">
-        <f>CONCATENATE("(ID:=",A31,",CBID:=",B31,",Flow:=ADR(HMI1.Flow_",B31,"),Status:=ADR(",D31,")",G31,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=30,CBID:=102,Flow:=ADR(HMI1.Flow_102),Status:=ADR(HMI1.CB102_Closed),IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1279,11 +1279,11 @@
         <v>103</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_103</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB103_Closed</v>
       </c>
       <c r="E32" t="str">
@@ -1291,15 +1291,15 @@
         <v>HMI1.CB103_Cmd</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB103_MODBUS</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)</v>
       </c>
       <c r="H32" t="str">
-        <f>CONCATENATE("(ID:=",A32,",CBID:=",B32,",Flow:=ADR(HMI1.Flow_",B32,"),Status:=ADR(",D32,")",G32,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=31,CBID:=103,Flow:=ADR(HMI1.Flow_103),Status:=ADR(HMI1.CB103_Closed),IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1311,23 +1311,23 @@
         <v>104</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_104</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB104_Closed</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB104_MODBUS</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H33" t="str">
-        <f>CONCATENATE("(ID:=",A33,",CBID:=",B33,",Flow:=ADR(HMI1.Flow_",B33,"),Status:=ADR(",D33,")",G33,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=32,CBID:=104,Flow:=ADR(HMI1.Flow_104),Status:=ADR(HMI1.CB104_Closed)),</v>
       </c>
     </row>
@@ -1339,23 +1339,23 @@
         <v>105</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_105</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB105_Closed</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB105_MODBUS</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H34" t="str">
-        <f>CONCATENATE("(ID:=",A34,",CBID:=",B34,",Flow:=ADR(HMI1.Flow_",B34,"),Status:=ADR(",D34,")",G34,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=33,CBID:=105,Flow:=ADR(HMI1.Flow_105),Status:=ADR(HMI1.CB105_Closed)),</v>
       </c>
     </row>
@@ -1367,23 +1367,23 @@
         <v>106</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_106</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB106_Closed</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB106_MODBUS</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H35" t="str">
-        <f>CONCATENATE("(ID:=",A35,",CBID:=",B35,",Flow:=ADR(HMI1.Flow_",B35,"),Status:=ADR(",D35,")",G35,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=34,CBID:=106,Flow:=ADR(HMI1.Flow_106),Status:=ADR(HMI1.CB106_Closed)),</v>
       </c>
     </row>
@@ -1395,23 +1395,23 @@
         <v>107</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_107</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB107_Closed</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB107_MODBUS</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H36" t="str">
-        <f>CONCATENATE("(ID:=",A36,",CBID:=",B36,",Flow:=ADR(HMI1.Flow_",B36,"),Status:=ADR(",D36,")",G36,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=35,CBID:=107,Flow:=ADR(HMI1.Flow_107),Status:=ADR(HMI1.CB107_Closed)),</v>
       </c>
     </row>
@@ -1423,11 +1423,11 @@
         <v>108</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_108</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB108_Closed</v>
       </c>
       <c r="E37" t="str">
@@ -1435,15 +1435,15 @@
         <v>HMI1.CB108_Cmd</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB108_MODBUS</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)</v>
       </c>
       <c r="H37" t="str">
-        <f>CONCATENATE("(ID:=",A37,",CBID:=",B37,",Flow:=ADR(HMI1.Flow_",B37,"),Status:=ADR(",D37,")",G37,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=36,CBID:=108,Flow:=ADR(HMI1.Flow_108),Status:=ADR(HMI1.CB108_Closed),IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1455,11 +1455,11 @@
         <v>109</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_109</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB109_Closed</v>
       </c>
       <c r="E38" t="str">
@@ -1467,15 +1467,15 @@
         <v>HMI1.CB109_Cmd</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB109_MODBUS</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)</v>
       </c>
       <c r="H38" t="str">
-        <f>CONCATENATE("(ID:=",A38,",CBID:=",B38,",Flow:=ADR(HMI1.Flow_",B38,"),Status:=ADR(",D38,")",G38,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=37,CBID:=109,Flow:=ADR(HMI1.Flow_109),Status:=ADR(HMI1.CB109_Closed),IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1487,23 +1487,23 @@
         <v>110</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_110</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB110_Closed</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB110_MODBUS</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H39" t="str">
-        <f>CONCATENATE("(ID:=",A39,",CBID:=",B39,",Flow:=ADR(HMI1.Flow_",B39,"),Status:=ADR(",D39,")",G39,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=38,CBID:=110,Flow:=ADR(HMI1.Flow_110),Status:=ADR(HMI1.CB110_Closed)),</v>
       </c>
     </row>
@@ -1515,11 +1515,11 @@
         <v>111</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_111</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB111_Closed</v>
       </c>
       <c r="E40" t="str">
@@ -1527,15 +1527,15 @@
         <v>HMI1.CB111_Cmd</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB111_MODBUS</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)</v>
       </c>
       <c r="H40" t="str">
-        <f>CONCATENATE("(ID:=",A40,",CBID:=",B40,",Flow:=ADR(HMI1.Flow_",B40,"),Status:=ADR(",D40,")",G40,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=39,CBID:=111,Flow:=ADR(HMI1.Flow_111),Status:=ADR(HMI1.CB111_Closed),IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1547,23 +1547,23 @@
         <v>112</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_112</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB112_Closed</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB112_MODBUS</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H41" t="str">
-        <f>CONCATENATE("(ID:=",A41,",CBID:=",B41,",Flow:=ADR(HMI1.Flow_",B41,"),Status:=ADR(",D41,")",G41,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=40,CBID:=112,Flow:=ADR(HMI1.Flow_112),Status:=ADR(HMI1.CB112_Closed)),</v>
       </c>
     </row>
@@ -1575,11 +1575,11 @@
         <v>113</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_113</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB113_Closed</v>
       </c>
       <c r="E42" t="str">
@@ -1587,15 +1587,15 @@
         <v>HMI1.CB113_Cmd</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB113_MODBUS</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)</v>
       </c>
       <c r="H42" t="str">
-        <f>CONCATENATE("(ID:=",A42,",CBID:=",B42,",Flow:=ADR(HMI1.Flow_",B42,"),Status:=ADR(",D42,")",G42,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=41,CBID:=113,Flow:=ADR(HMI1.Flow_113),Status:=ADR(HMI1.CB113_Closed),IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1607,23 +1607,23 @@
         <v>114</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_114</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB114_Closed</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB114_MODBUS</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H43" t="str">
-        <f>CONCATENATE("(ID:=",A43,",CBID:=",B43,",Flow:=ADR(HMI1.Flow_",B43,"),Status:=ADR(",D43,")",G43,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=42,CBID:=114,Flow:=ADR(HMI1.Flow_114),Status:=ADR(HMI1.CB114_Closed)),</v>
       </c>
     </row>
@@ -1635,23 +1635,23 @@
         <v>300</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_300</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB300_Closed</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB300_MODBUS</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H44" t="str">
-        <f>CONCATENATE("(ID:=",A44,",CBID:=",B44,",Flow:=ADR(HMI1.Flow_",B44,"),Status:=ADR(",D44,")",G44,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=43,CBID:=300,Flow:=ADR(HMI1.Flow_300),Status:=ADR(HMI1.CB300_Closed)),</v>
       </c>
     </row>
@@ -1663,23 +1663,23 @@
         <v>200</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_200</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB200_Closed</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB200_MODBUS</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H45" t="str">
-        <f>CONCATENATE("(ID:=",A45,",CBID:=",B45,",Flow:=ADR(HMI1.Flow_",B45,"),Status:=ADR(",D45,")",G45,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=44,CBID:=200,Flow:=ADR(HMI1.Flow_200),Status:=ADR(HMI1.CB200_Closed)),</v>
       </c>
     </row>
@@ -1691,23 +1691,23 @@
         <v>100</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_100</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB100_Closed</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB100_MODBUS</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H46" t="str">
-        <f>CONCATENATE("(ID:=",A46,",CBID:=",B46,",Flow:=ADR(HMI1.Flow_",B46,"),Status:=ADR(",D46,")",G46,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=45,CBID:=100,Flow:=ADR(HMI1.Flow_100),Status:=ADR(HMI1.CB100_Closed)),</v>
       </c>
     </row>
@@ -1719,23 +1719,23 @@
         <v>351</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_351</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB351_Closed</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB351_MODBUS</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H47" t="str">
-        <f>CONCATENATE("(ID:=",A47,",CBID:=",B47,",Flow:=ADR(HMI1.Flow_",B47,"),Status:=ADR(",D47,")",G47,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=46,CBID:=351,Flow:=ADR(HMI1.Flow_351),Status:=ADR(HMI1.CB351_Closed)),</v>
       </c>
     </row>
@@ -1747,24 +1747,388 @@
         <v>151</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>HMI1.Flow_151</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>HMI1.CB151_Closed</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>CB151_MODBUS</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H48" t="str">
-        <f>CONCATENATE("(ID:=",A48,",CBID:=",B48,",Flow:=ADR(HMI1.Flow_",B48,"),Status:=ADR(",D48,")",G48,"),")</f>
+        <f t="shared" si="1"/>
         <v>(ID:=47,CBID:=151,Flow:=ADR(HMI1.Flow_151),Status:=ADR(HMI1.CB151_Closed)),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>401</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" ref="C49:C55" si="6">CONCATENATE("HMI1.Flow_",B49)</f>
+        <v>HMI1.Flow_401</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" ref="D49:D55" si="7">CONCATENATE("HMI1.CB",B49,"_Closed")</f>
+        <v>HMI1.CB401_Closed</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" ref="F49:F55" si="8">CONCATENATE("CB", B49, "_MODBUS")</f>
+        <v>CB401_MODBUS</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" ref="G49:G55" si="9">IF(E49="","",CONCATENATE(",IOCCmd:=ADR(",E49,"),MBCmd:=ADR(",F49,".CMD),MBRst:=ADR(",F49,".RST)"))</f>
+        <v/>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" ref="H49:H55" si="10">CONCATENATE("(ID:=",A49,",CBID:=",B49,",Flow:=ADR(HMI1.Flow_",B49,"),Status:=ADR(",D49,")",G49,"),")</f>
+        <v>(ID:=48,CBID:=401,Flow:=ADR(HMI1.Flow_401),Status:=ADR(HMI1.CB401_Closed)),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>402</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_402</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB402_Closed</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="8"/>
+        <v>CB402_MODBUS</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=49,CBID:=402,Flow:=ADR(HMI1.Flow_402),Status:=ADR(HMI1.CB402_Closed)),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>403</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_403</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB403_Closed</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="8"/>
+        <v>CB403_MODBUS</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=50,CBID:=403,Flow:=ADR(HMI1.Flow_403),Status:=ADR(HMI1.CB403_Closed)),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>404</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_404</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB404_Closed</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="8"/>
+        <v>CB404_MODBUS</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=51,CBID:=404,Flow:=ADR(HMI1.Flow_404),Status:=ADR(HMI1.CB404_Closed)),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>405</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_405</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB405_Closed</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="8"/>
+        <v>CB405_MODBUS</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=52,CBID:=405,Flow:=ADR(HMI1.Flow_405),Status:=ADR(HMI1.CB405_Closed)),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>406</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_406</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB406_Closed</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="8"/>
+        <v>CB406_MODBUS</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=53,CBID:=406,Flow:=ADR(HMI1.Flow_406),Status:=ADR(HMI1.CB406_Closed)),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>407</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.Flow_407</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="7"/>
+        <v>HMI1.CB407_Closed</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="8"/>
+        <v>CB407_MODBUS</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="10"/>
+        <v>(ID:=54,CBID:=407,Flow:=ADR(HMI1.Flow_407),Status:=ADR(HMI1.CB407_Closed)),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>408</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" ref="C56:C61" si="11">CONCATENATE("HMI1.Flow_",B56)</f>
+        <v>HMI1.Flow_408</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" ref="D56:D61" si="12">CONCATENATE("HMI1.CB",B56,"_Closed")</f>
+        <v>HMI1.CB408_Closed</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" ref="F56:F61" si="13">CONCATENATE("CB", B56, "_MODBUS")</f>
+        <v>CB408_MODBUS</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" ref="G56:G61" si="14">IF(E56="","",CONCATENATE(",IOCCmd:=ADR(",E56,"),MBCmd:=ADR(",F56,".CMD),MBRst:=ADR(",F56,".RST)"))</f>
+        <v/>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" ref="H56:H61" si="15">CONCATENATE("(ID:=",A56,",CBID:=",B56,",Flow:=ADR(HMI1.Flow_",B56,"),Status:=ADR(",D56,")",G56,"),")</f>
+        <v>(ID:=55,CBID:=408,Flow:=ADR(HMI1.Flow_408),Status:=ADR(HMI1.CB408_Closed)),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>409</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="11"/>
+        <v>HMI1.Flow_409</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="12"/>
+        <v>HMI1.CB409_Closed</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="13"/>
+        <v>CB409_MODBUS</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="15"/>
+        <v>(ID:=56,CBID:=409,Flow:=ADR(HMI1.Flow_409),Status:=ADR(HMI1.CB409_Closed)),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>410</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="11"/>
+        <v>HMI1.Flow_410</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="12"/>
+        <v>HMI1.CB410_Closed</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="13"/>
+        <v>CB410_MODBUS</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="15"/>
+        <v>(ID:=57,CBID:=410,Flow:=ADR(HMI1.Flow_410),Status:=ADR(HMI1.CB410_Closed)),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>411</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="11"/>
+        <v>HMI1.Flow_411</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="12"/>
+        <v>HMI1.CB411_Closed</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="13"/>
+        <v>CB411_MODBUS</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="15"/>
+        <v>(ID:=58,CBID:=411,Flow:=ADR(HMI1.Flow_411),Status:=ADR(HMI1.CB411_Closed)),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>412</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="11"/>
+        <v>HMI1.Flow_412</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="12"/>
+        <v>HMI1.CB412_Closed</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="13"/>
+        <v>CB412_MODBUS</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="15"/>
+        <v>(ID:=59,CBID:=412,Flow:=ADR(HMI1.Flow_412),Status:=ADR(HMI1.CB412_Closed)),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>413</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="11"/>
+        <v>HMI1.Flow_413</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="12"/>
+        <v>HMI1.CB413_Closed</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="13"/>
+        <v>CB413_MODBUS</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="15"/>
+        <v>(ID:=60,CBID:=413,Flow:=ADR(HMI1.Flow_413),Status:=ADR(HMI1.CB413_Closed)),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates in RTAC code and diagram builder to accomodate for: - new PV and ESS data in UDP stream from banshee - New ip ranges in 10.79.112.xx subnet
</commit_message>
<xml_diff>
--- a/SimulationTools/RTAC/MGC_SEL_programming.xlsx
+++ b/SimulationTools/RTAC/MGC_SEL_programming.xlsx
@@ -373,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI61"/>
+  <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L61" sqref="L2:L61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,11 +408,11 @@
         <v>301</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B2)</f>
+        <f t="shared" ref="D2:D33" si="0">CONCATENATE("HMI1.Flow_",B2)</f>
         <v>HMI1.Flow_301</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("HMI1.CB",B2,"_Closed")</f>
+        <f t="shared" ref="E2:E33" si="1">CONCATENATE("HMI1.CB",B2,"_Closed")</f>
         <v>HMI1.CB301_Closed</v>
       </c>
       <c r="F2" t="str">
@@ -428,11 +428,11 @@
         <v>HMI1.CB301_Cmd</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("CB", B2, "_MODBUS")</f>
+        <f t="shared" ref="I2:I33" si="2">CONCATENATE("CB", B2, "_MODBUS")</f>
         <v>CB301_MODBUS</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J48" si="0">IF(C2="","",CONCATENATE("HMI1.BUS",C2,"_Stat"))</f>
+        <f t="shared" ref="J2:J48" si="3">IF(C2="","",CONCATENATE("HMI1.BUS",C2,"_Stat"))</f>
         <v/>
       </c>
       <c r="K2" t="str">
@@ -440,7 +440,7 @@
         <v>,IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L60" si="1">CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",E2,"),Vpu:=ADR(",F2,"),VLgood:=ADR(",G2,")",K2,"),")</f>
+        <f t="shared" ref="L2:L62" si="4">CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",E2,"),Vpu:=ADR(",F2,"),VLgood:=ADR(",G2,")",K2,"),")</f>
         <v>(ID:=1,CBID:=301,Flow:=ADR(HMI1.Flow_301),Status:=ADR(HMI1.CB301_Closed),Vpu:=ADR(HMI1.CB301_Vpu),VLgood:=ADR(HMI1.CB301_VLgood),IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)),</v>
       </c>
       <c r="AI2" t="s">
@@ -455,19 +455,19 @@
         <v>302</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B3)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_302</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE("HMI1.CB",B3,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB302_Closed</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F61" si="2">CONCATENATE("HMI1.CB",B3,"_Vpu")</f>
+        <f t="shared" ref="F3:F63" si="5">CONCATENATE("HMI1.CB",B3,"_Vpu")</f>
         <v>HMI1.CB302_Vpu</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G61" si="3">CONCATENATE("HMI1.CB",B3,"_VLgood")</f>
+        <f t="shared" ref="G3:G63" si="6">CONCATENATE("HMI1.CB",B3,"_VLgood")</f>
         <v>HMI1.CB302_VLgood</v>
       </c>
       <c r="H3" t="str">
@@ -475,19 +475,19 @@
         <v>HMI1.CB302_Cmd</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("CB", B3, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB302_MODBUS</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K48" si="4">IF(H3="","",CONCATENATE(",IOCCmd:=ADR(",H3,"),MBCmd:=ADR(",I3,".CMD),MBRst:=ADR(",I3,".RST)"))</f>
+        <f t="shared" ref="K3:K50" si="7">IF(H3="","",CONCATENATE(",IOCCmd:=ADR(",H3,"),MBCmd:=ADR(",I3,".CMD),MBRst:=ADR(",I3,".RST)"))</f>
         <v>,IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=2,CBID:=302,Flow:=ADR(HMI1.Flow_302),Status:=ADR(HMI1.CB302_Closed),Vpu:=ADR(HMI1.CB302_Vpu),VLgood:=ADR(HMI1.CB302_VLgood),IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)),</v>
       </c>
     </row>
@@ -499,19 +499,19 @@
         <v>303</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B4)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_303</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE("HMI1.CB",B4,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB303_Closed</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB303_Vpu</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB303_VLgood</v>
       </c>
       <c r="H4" t="str">
@@ -519,19 +519,19 @@
         <v>HMI1.CB303_Cmd</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("CB", B4, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB303_MODBUS</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=3,CBID:=303,Flow:=ADR(HMI1.Flow_303),Status:=ADR(HMI1.CB303_Closed),Vpu:=ADR(HMI1.CB303_Vpu),VLgood:=ADR(HMI1.CB303_VLgood),IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)),</v>
       </c>
     </row>
@@ -543,19 +543,19 @@
         <v>304</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B5)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_304</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE("HMI1.CB",B5,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB304_Closed</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB304_Vpu</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB304_VLgood</v>
       </c>
       <c r="H5" t="str">
@@ -563,19 +563,19 @@
         <v>HMI1.CB304_Cmd</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("CB", B5, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB304_MODBUS</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=4,CBID:=304,Flow:=ADR(HMI1.Flow_304),Status:=ADR(HMI1.CB304_Closed),Vpu:=ADR(HMI1.CB304_Vpu),VLgood:=ADR(HMI1.CB304_VLgood),IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)),</v>
       </c>
     </row>
@@ -587,19 +587,19 @@
         <v>305</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B6)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_305</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE("HMI1.CB",B6,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB305_Closed</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB305_Vpu</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB305_VLgood</v>
       </c>
       <c r="H6" t="str">
@@ -607,19 +607,19 @@
         <v>HMI1.CB305_Cmd</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("CB", B6, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB305_MODBUS</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=5,CBID:=305,Flow:=ADR(HMI1.Flow_305),Status:=ADR(HMI1.CB305_Closed),Vpu:=ADR(HMI1.CB305_Vpu),VLgood:=ADR(HMI1.CB305_VLgood),IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)),</v>
       </c>
     </row>
@@ -631,35 +631,35 @@
         <v>306</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B7)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_306</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE("HMI1.CB",B7,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB306_Closed</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB306_Vpu</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB306_VLgood</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("CB", B7, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB306_MODBUS</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=6,CBID:=306,Flow:=ADR(HMI1.Flow_306),Status:=ADR(HMI1.CB306_Closed),Vpu:=ADR(HMI1.CB306_Vpu),VLgood:=ADR(HMI1.CB306_VLgood)),</v>
       </c>
     </row>
@@ -671,35 +671,35 @@
         <v>307</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B8)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_307</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE("HMI1.CB",B8,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB307_Closed</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB307_Vpu</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB307_VLgood</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("CB", B8, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB307_MODBUS</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=7,CBID:=307,Flow:=ADR(HMI1.Flow_307),Status:=ADR(HMI1.CB307_Closed),Vpu:=ADR(HMI1.CB307_Vpu),VLgood:=ADR(HMI1.CB307_VLgood)),</v>
       </c>
     </row>
@@ -711,35 +711,35 @@
         <v>308</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B9)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_308</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE("HMI1.CB",B9,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB308_Closed</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB308_Vpu</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB308_VLgood</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("CB", B9, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB308_MODBUS</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=8,CBID:=308,Flow:=ADR(HMI1.Flow_308),Status:=ADR(HMI1.CB308_Closed),Vpu:=ADR(HMI1.CB308_Vpu),VLgood:=ADR(HMI1.CB308_VLgood)),</v>
       </c>
     </row>
@@ -751,35 +751,35 @@
         <v>309</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B10)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_309</v>
       </c>
       <c r="E10" t="str">
-        <f>CONCATENATE("HMI1.CB",B10,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB309_Closed</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB309_Vpu</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB309_VLgood</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("CB", B10, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB309_MODBUS</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=9,CBID:=309,Flow:=ADR(HMI1.Flow_309),Status:=ADR(HMI1.CB309_Closed),Vpu:=ADR(HMI1.CB309_Vpu),VLgood:=ADR(HMI1.CB309_VLgood)),</v>
       </c>
     </row>
@@ -791,19 +791,19 @@
         <v>201</v>
       </c>
       <c r="D11" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B11)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_201</v>
       </c>
       <c r="E11" t="str">
-        <f>CONCATENATE("HMI1.CB",B11,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB201_Closed</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB201_Vpu</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB201_VLgood</v>
       </c>
       <c r="H11" t="str">
@@ -811,19 +811,19 @@
         <v>HMI1.CB201_Cmd</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("CB", B11, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB201_MODBUS</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=10,CBID:=201,Flow:=ADR(HMI1.Flow_201),Status:=ADR(HMI1.CB201_Closed),Vpu:=ADR(HMI1.CB201_Vpu),VLgood:=ADR(HMI1.CB201_VLgood),IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)),</v>
       </c>
     </row>
@@ -835,19 +835,19 @@
         <v>202</v>
       </c>
       <c r="D12" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B12)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_202</v>
       </c>
       <c r="E12" t="str">
-        <f>CONCATENATE("HMI1.CB",B12,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB202_Closed</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB202_Vpu</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB202_VLgood</v>
       </c>
       <c r="H12" t="str">
@@ -855,19 +855,19 @@
         <v>HMI1.CB202_Cmd</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("CB", B12, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB202_MODBUS</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=11,CBID:=202,Flow:=ADR(HMI1.Flow_202),Status:=ADR(HMI1.CB202_Closed),Vpu:=ADR(HMI1.CB202_Vpu),VLgood:=ADR(HMI1.CB202_VLgood),IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)),</v>
       </c>
     </row>
@@ -879,19 +879,19 @@
         <v>203</v>
       </c>
       <c r="D13" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B13)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_203</v>
       </c>
       <c r="E13" t="str">
-        <f>CONCATENATE("HMI1.CB",B13,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB203_Closed</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB203_Vpu</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB203_VLgood</v>
       </c>
       <c r="H13" t="str">
@@ -899,19 +899,19 @@
         <v>HMI1.CB203_Cmd</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("CB", B13, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB203_MODBUS</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=12,CBID:=203,Flow:=ADR(HMI1.Flow_203),Status:=ADR(HMI1.CB203_Closed),Vpu:=ADR(HMI1.CB203_Vpu),VLgood:=ADR(HMI1.CB203_VLgood),IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)),</v>
       </c>
     </row>
@@ -923,35 +923,35 @@
         <v>204</v>
       </c>
       <c r="D14" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B14)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_204</v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE("HMI1.CB",B14,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB204_Closed</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB204_Vpu</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB204_VLgood</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("CB", B14, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB204_MODBUS</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=13,CBID:=204,Flow:=ADR(HMI1.Flow_204),Status:=ADR(HMI1.CB204_Closed),Vpu:=ADR(HMI1.CB204_Vpu),VLgood:=ADR(HMI1.CB204_VLgood)),</v>
       </c>
     </row>
@@ -963,35 +963,35 @@
         <v>205</v>
       </c>
       <c r="D15" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B15)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_205</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE("HMI1.CB",B15,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB205_Closed</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB205_Vpu</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB205_VLgood</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("CB", B15, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB205_MODBUS</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=14,CBID:=205,Flow:=ADR(HMI1.Flow_205),Status:=ADR(HMI1.CB205_Closed),Vpu:=ADR(HMI1.CB205_Vpu),VLgood:=ADR(HMI1.CB205_VLgood)),</v>
       </c>
     </row>
@@ -1003,35 +1003,35 @@
         <v>206</v>
       </c>
       <c r="D16" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B16)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_206</v>
       </c>
       <c r="E16" t="str">
-        <f>CONCATENATE("HMI1.CB",B16,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB206_Closed</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB206_Vpu</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB206_VLgood</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("CB", B16, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB206_MODBUS</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=15,CBID:=206,Flow:=ADR(HMI1.Flow_206),Status:=ADR(HMI1.CB206_Closed),Vpu:=ADR(HMI1.CB206_Vpu),VLgood:=ADR(HMI1.CB206_VLgood)),</v>
       </c>
     </row>
@@ -1043,35 +1043,35 @@
         <v>207</v>
       </c>
       <c r="D17" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B17)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_207</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE("HMI1.CB",B17,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB207_Closed</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB207_Vpu</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB207_VLgood</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("CB", B17, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB207_MODBUS</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=16,CBID:=207,Flow:=ADR(HMI1.Flow_207),Status:=ADR(HMI1.CB207_Closed),Vpu:=ADR(HMI1.CB207_Vpu),VLgood:=ADR(HMI1.CB207_VLgood)),</v>
       </c>
     </row>
@@ -1083,35 +1083,35 @@
         <v>208</v>
       </c>
       <c r="D18" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B18)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_208</v>
       </c>
       <c r="E18" t="str">
-        <f>CONCATENATE("HMI1.CB",B18,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB208_Closed</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB208_Vpu</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB208_VLgood</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("CB", B18, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB208_MODBUS</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=17,CBID:=208,Flow:=ADR(HMI1.Flow_208),Status:=ADR(HMI1.CB208_Closed),Vpu:=ADR(HMI1.CB208_Vpu),VLgood:=ADR(HMI1.CB208_VLgood)),</v>
       </c>
     </row>
@@ -1123,35 +1123,35 @@
         <v>209</v>
       </c>
       <c r="D19" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B19)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_209</v>
       </c>
       <c r="E19" t="str">
-        <f>CONCATENATE("HMI1.CB",B19,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB209_Closed</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB209_Vpu</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB209_VLgood</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("CB", B19, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB209_MODBUS</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=18,CBID:=209,Flow:=ADR(HMI1.Flow_209),Status:=ADR(HMI1.CB209_Closed),Vpu:=ADR(HMI1.CB209_Vpu),VLgood:=ADR(HMI1.CB209_VLgood)),</v>
       </c>
     </row>
@@ -1163,35 +1163,35 @@
         <v>210</v>
       </c>
       <c r="D20" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B20)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_210</v>
       </c>
       <c r="E20" t="str">
-        <f>CONCATENATE("HMI1.CB",B20,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB210_Closed</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB210_Vpu</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB210_VLgood</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("CB", B20, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB210_MODBUS</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=19,CBID:=210,Flow:=ADR(HMI1.Flow_210),Status:=ADR(HMI1.CB210_Closed),Vpu:=ADR(HMI1.CB210_Vpu),VLgood:=ADR(HMI1.CB210_VLgood)),</v>
       </c>
     </row>
@@ -1203,35 +1203,35 @@
         <v>211</v>
       </c>
       <c r="D21" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B21)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_211</v>
       </c>
       <c r="E21" t="str">
-        <f>CONCATENATE("HMI1.CB",B21,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB211_Closed</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB211_Vpu</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB211_VLgood</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("CB", B21, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB211_MODBUS</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=20,CBID:=211,Flow:=ADR(HMI1.Flow_211),Status:=ADR(HMI1.CB211_Closed),Vpu:=ADR(HMI1.CB211_Vpu),VLgood:=ADR(HMI1.CB211_VLgood)),</v>
       </c>
     </row>
@@ -1243,35 +1243,35 @@
         <v>212</v>
       </c>
       <c r="D22" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B22)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_212</v>
       </c>
       <c r="E22" t="str">
-        <f>CONCATENATE("HMI1.CB",B22,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB212_Closed</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB212_Vpu</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB212_VLgood</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("CB", B22, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB212_MODBUS</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=21,CBID:=212,Flow:=ADR(HMI1.Flow_212),Status:=ADR(HMI1.CB212_Closed),Vpu:=ADR(HMI1.CB212_Vpu),VLgood:=ADR(HMI1.CB212_VLgood)),</v>
       </c>
     </row>
@@ -1283,19 +1283,19 @@
         <v>213</v>
       </c>
       <c r="D23" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B23)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_213</v>
       </c>
       <c r="E23" t="str">
-        <f>CONCATENATE("HMI1.CB",B23,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB213_Closed</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB213_Vpu</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB213_VLgood</v>
       </c>
       <c r="H23" t="str">
@@ -1303,19 +1303,19 @@
         <v>HMI1.CB213_Cmd</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("CB", B23, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB213_MODBUS</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=22,CBID:=213,Flow:=ADR(HMI1.Flow_213),Status:=ADR(HMI1.CB213_Closed),Vpu:=ADR(HMI1.CB213_Vpu),VLgood:=ADR(HMI1.CB213_VLgood),IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1327,35 +1327,35 @@
         <v>214</v>
       </c>
       <c r="D24" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B24)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_214</v>
       </c>
       <c r="E24" t="str">
-        <f>CONCATENATE("HMI1.CB",B24,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB214_Closed</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB214_Vpu</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB214_VLgood</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("CB", B24, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB214_MODBUS</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=23,CBID:=214,Flow:=ADR(HMI1.Flow_214),Status:=ADR(HMI1.CB214_Closed),Vpu:=ADR(HMI1.CB214_Vpu),VLgood:=ADR(HMI1.CB214_VLgood)),</v>
       </c>
     </row>
@@ -1367,35 +1367,35 @@
         <v>215</v>
       </c>
       <c r="D25" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B25)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_215</v>
       </c>
       <c r="E25" t="str">
-        <f>CONCATENATE("HMI1.CB",B25,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB215_Closed</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB215_Vpu</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB215_VLgood</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("CB", B25, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB215_MODBUS</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=24,CBID:=215,Flow:=ADR(HMI1.Flow_215),Status:=ADR(HMI1.CB215_Closed),Vpu:=ADR(HMI1.CB215_Vpu),VLgood:=ADR(HMI1.CB215_VLgood)),</v>
       </c>
     </row>
@@ -1407,19 +1407,19 @@
         <v>216</v>
       </c>
       <c r="D26" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B26)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_216</v>
       </c>
       <c r="E26" t="str">
-        <f>CONCATENATE("HMI1.CB",B26,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB216_Closed</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB216_Vpu</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB216_VLgood</v>
       </c>
       <c r="H26" t="str">
@@ -1427,19 +1427,19 @@
         <v>HMI1.CB216_Cmd</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE("CB", B26, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB216_MODBUS</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=25,CBID:=216,Flow:=ADR(HMI1.Flow_216),Status:=ADR(HMI1.CB216_Closed),Vpu:=ADR(HMI1.CB216_Vpu),VLgood:=ADR(HMI1.CB216_VLgood),IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1451,19 +1451,19 @@
         <v>217</v>
       </c>
       <c r="D27" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B27)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_217</v>
       </c>
       <c r="E27" t="str">
-        <f>CONCATENATE("HMI1.CB",B27,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB217_Closed</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB217_Vpu</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB217_VLgood</v>
       </c>
       <c r="H27" t="str">
@@ -1471,19 +1471,19 @@
         <v>HMI1.CB217_Cmd</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE("CB", B27, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB217_MODBUS</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=26,CBID:=217,Flow:=ADR(HMI1.Flow_217),Status:=ADR(HMI1.CB217_Closed),Vpu:=ADR(HMI1.CB217_Vpu),VLgood:=ADR(HMI1.CB217_VLgood),IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1495,35 +1495,35 @@
         <v>218</v>
       </c>
       <c r="D28" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B28)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_218</v>
       </c>
       <c r="E28" t="str">
-        <f>CONCATENATE("HMI1.CB",B28,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB218_Closed</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB218_Vpu</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB218_VLgood</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE("CB", B28, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB218_MODBUS</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=27,CBID:=218,Flow:=ADR(HMI1.Flow_218),Status:=ADR(HMI1.CB218_Closed),Vpu:=ADR(HMI1.CB218_Vpu),VLgood:=ADR(HMI1.CB218_VLgood)),</v>
       </c>
     </row>
@@ -1535,35 +1535,35 @@
         <v>219</v>
       </c>
       <c r="D29" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B29)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_219</v>
       </c>
       <c r="E29" t="str">
-        <f>CONCATENATE("HMI1.CB",B29,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB219_Closed</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB219_Vpu</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB219_VLgood</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE("CB", B29, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB219_MODBUS</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=28,CBID:=219,Flow:=ADR(HMI1.Flow_219),Status:=ADR(HMI1.CB219_Closed),Vpu:=ADR(HMI1.CB219_Vpu),VLgood:=ADR(HMI1.CB219_VLgood)),</v>
       </c>
     </row>
@@ -1575,19 +1575,19 @@
         <v>101</v>
       </c>
       <c r="D30" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B30)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_101</v>
       </c>
       <c r="E30" t="str">
-        <f>CONCATENATE("HMI1.CB",B30,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB101_Closed</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB101_Vpu</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB101_VLgood</v>
       </c>
       <c r="H30" t="str">
@@ -1595,19 +1595,19 @@
         <v>HMI1.CB101_Cmd</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE("CB", B30, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB101_MODBUS</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=29,CBID:=101,Flow:=ADR(HMI1.Flow_101),Status:=ADR(HMI1.CB101_Closed),Vpu:=ADR(HMI1.CB101_Vpu),VLgood:=ADR(HMI1.CB101_VLgood),IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1619,19 +1619,19 @@
         <v>102</v>
       </c>
       <c r="D31" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B31)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_102</v>
       </c>
       <c r="E31" t="str">
-        <f>CONCATENATE("HMI1.CB",B31,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB102_Closed</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB102_Vpu</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB102_VLgood</v>
       </c>
       <c r="H31" t="str">
@@ -1639,19 +1639,19 @@
         <v>HMI1.CB102_Cmd</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE("CB", B31, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB102_MODBUS</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=30,CBID:=102,Flow:=ADR(HMI1.Flow_102),Status:=ADR(HMI1.CB102_Closed),Vpu:=ADR(HMI1.CB102_Vpu),VLgood:=ADR(HMI1.CB102_VLgood),IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1663,19 +1663,19 @@
         <v>103</v>
       </c>
       <c r="D32" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B32)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_103</v>
       </c>
       <c r="E32" t="str">
-        <f>CONCATENATE("HMI1.CB",B32,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB103_Closed</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB103_Vpu</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB103_VLgood</v>
       </c>
       <c r="H32" t="str">
@@ -1683,19 +1683,19 @@
         <v>HMI1.CB103_Cmd</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE("CB", B32, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB103_MODBUS</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=31,CBID:=103,Flow:=ADR(HMI1.Flow_103),Status:=ADR(HMI1.CB103_Closed),Vpu:=ADR(HMI1.CB103_Vpu),VLgood:=ADR(HMI1.CB103_VLgood),IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1707,35 +1707,35 @@
         <v>104</v>
       </c>
       <c r="D33" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B33)</f>
+        <f t="shared" si="0"/>
         <v>HMI1.Flow_104</v>
       </c>
       <c r="E33" t="str">
-        <f>CONCATENATE("HMI1.CB",B33,"_Closed")</f>
+        <f t="shared" si="1"/>
         <v>HMI1.CB104_Closed</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB104_Vpu</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB104_VLgood</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("CB", B33, "_MODBUS")</f>
+        <f t="shared" si="2"/>
         <v>CB104_MODBUS</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=32,CBID:=104,Flow:=ADR(HMI1.Flow_104),Status:=ADR(HMI1.CB104_Closed),Vpu:=ADR(HMI1.CB104_Vpu),VLgood:=ADR(HMI1.CB104_VLgood)),</v>
       </c>
     </row>
@@ -1747,35 +1747,35 @@
         <v>105</v>
       </c>
       <c r="D34" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B34)</f>
+        <f t="shared" ref="D34:D63" si="8">CONCATENATE("HMI1.Flow_",B34)</f>
         <v>HMI1.Flow_105</v>
       </c>
       <c r="E34" t="str">
-        <f>CONCATENATE("HMI1.CB",B34,"_Closed")</f>
+        <f t="shared" ref="E34:E63" si="9">CONCATENATE("HMI1.CB",B34,"_Closed")</f>
         <v>HMI1.CB105_Closed</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB105_Vpu</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB105_VLgood</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("CB", B34, "_MODBUS")</f>
+        <f t="shared" ref="I34:I63" si="10">CONCATENATE("CB", B34, "_MODBUS")</f>
         <v>CB105_MODBUS</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=33,CBID:=105,Flow:=ADR(HMI1.Flow_105),Status:=ADR(HMI1.CB105_Closed),Vpu:=ADR(HMI1.CB105_Vpu),VLgood:=ADR(HMI1.CB105_VLgood)),</v>
       </c>
     </row>
@@ -1787,35 +1787,35 @@
         <v>106</v>
       </c>
       <c r="D35" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B35)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_106</v>
       </c>
       <c r="E35" t="str">
-        <f>CONCATENATE("HMI1.CB",B35,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB106_Closed</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB106_Vpu</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB106_VLgood</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE("CB", B35, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB106_MODBUS</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=34,CBID:=106,Flow:=ADR(HMI1.Flow_106),Status:=ADR(HMI1.CB106_Closed),Vpu:=ADR(HMI1.CB106_Vpu),VLgood:=ADR(HMI1.CB106_VLgood)),</v>
       </c>
     </row>
@@ -1827,35 +1827,35 @@
         <v>107</v>
       </c>
       <c r="D36" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B36)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_107</v>
       </c>
       <c r="E36" t="str">
-        <f>CONCATENATE("HMI1.CB",B36,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB107_Closed</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB107_Vpu</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB107_VLgood</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE("CB", B36, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB107_MODBUS</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=35,CBID:=107,Flow:=ADR(HMI1.Flow_107),Status:=ADR(HMI1.CB107_Closed),Vpu:=ADR(HMI1.CB107_Vpu),VLgood:=ADR(HMI1.CB107_VLgood)),</v>
       </c>
     </row>
@@ -1867,19 +1867,19 @@
         <v>108</v>
       </c>
       <c r="D37" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B37)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_108</v>
       </c>
       <c r="E37" t="str">
-        <f>CONCATENATE("HMI1.CB",B37,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB108_Closed</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB108_Vpu</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB108_VLgood</v>
       </c>
       <c r="H37" t="str">
@@ -1887,19 +1887,19 @@
         <v>HMI1.CB108_Cmd</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE("CB", B37, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB108_MODBUS</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=36,CBID:=108,Flow:=ADR(HMI1.Flow_108),Status:=ADR(HMI1.CB108_Closed),Vpu:=ADR(HMI1.CB108_Vpu),VLgood:=ADR(HMI1.CB108_VLgood),IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1911,19 +1911,19 @@
         <v>109</v>
       </c>
       <c r="D38" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B38)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_109</v>
       </c>
       <c r="E38" t="str">
-        <f>CONCATENATE("HMI1.CB",B38,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB109_Closed</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB109_Vpu</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB109_VLgood</v>
       </c>
       <c r="H38" t="str">
@@ -1931,19 +1931,19 @@
         <v>HMI1.CB109_Cmd</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE("CB", B38, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB109_MODBUS</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=37,CBID:=109,Flow:=ADR(HMI1.Flow_109),Status:=ADR(HMI1.CB109_Closed),Vpu:=ADR(HMI1.CB109_Vpu),VLgood:=ADR(HMI1.CB109_VLgood),IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)),</v>
       </c>
     </row>
@@ -1955,35 +1955,35 @@
         <v>110</v>
       </c>
       <c r="D39" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B39)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_110</v>
       </c>
       <c r="E39" t="str">
-        <f>CONCATENATE("HMI1.CB",B39,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB110_Closed</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB110_Vpu</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB110_VLgood</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE("CB", B39, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB110_MODBUS</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=38,CBID:=110,Flow:=ADR(HMI1.Flow_110),Status:=ADR(HMI1.CB110_Closed),Vpu:=ADR(HMI1.CB110_Vpu),VLgood:=ADR(HMI1.CB110_VLgood)),</v>
       </c>
     </row>
@@ -1995,19 +1995,19 @@
         <v>111</v>
       </c>
       <c r="D40" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B40)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_111</v>
       </c>
       <c r="E40" t="str">
-        <f>CONCATENATE("HMI1.CB",B40,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB111_Closed</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB111_Vpu</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB111_VLgood</v>
       </c>
       <c r="H40" t="str">
@@ -2015,19 +2015,19 @@
         <v>HMI1.CB111_Cmd</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE("CB", B40, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB111_MODBUS</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=39,CBID:=111,Flow:=ADR(HMI1.Flow_111),Status:=ADR(HMI1.CB111_Closed),Vpu:=ADR(HMI1.CB111_Vpu),VLgood:=ADR(HMI1.CB111_VLgood),IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)),</v>
       </c>
     </row>
@@ -2039,35 +2039,35 @@
         <v>112</v>
       </c>
       <c r="D41" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B41)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_112</v>
       </c>
       <c r="E41" t="str">
-        <f>CONCATENATE("HMI1.CB",B41,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB112_Closed</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB112_Vpu</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB112_VLgood</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE("CB", B41, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB112_MODBUS</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=40,CBID:=112,Flow:=ADR(HMI1.Flow_112),Status:=ADR(HMI1.CB112_Closed),Vpu:=ADR(HMI1.CB112_Vpu),VLgood:=ADR(HMI1.CB112_VLgood)),</v>
       </c>
     </row>
@@ -2079,19 +2079,19 @@
         <v>113</v>
       </c>
       <c r="D42" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B42)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_113</v>
       </c>
       <c r="E42" t="str">
-        <f>CONCATENATE("HMI1.CB",B42,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB113_Closed</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB113_Vpu</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB113_VLgood</v>
       </c>
       <c r="H42" t="str">
@@ -2099,19 +2099,19 @@
         <v>HMI1.CB113_Cmd</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("CB", B42, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB113_MODBUS</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>,IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)</v>
       </c>
       <c r="L42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=41,CBID:=113,Flow:=ADR(HMI1.Flow_113),Status:=ADR(HMI1.CB113_Closed),Vpu:=ADR(HMI1.CB113_Vpu),VLgood:=ADR(HMI1.CB113_VLgood),IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)),</v>
       </c>
     </row>
@@ -2123,35 +2123,35 @@
         <v>114</v>
       </c>
       <c r="D43" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B43)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_114</v>
       </c>
       <c r="E43" t="str">
-        <f>CONCATENATE("HMI1.CB",B43,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB114_Closed</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB114_Vpu</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB114_VLgood</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("CB", B43, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB114_MODBUS</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=42,CBID:=114,Flow:=ADR(HMI1.Flow_114),Status:=ADR(HMI1.CB114_Closed),Vpu:=ADR(HMI1.CB114_Vpu),VLgood:=ADR(HMI1.CB114_VLgood)),</v>
       </c>
     </row>
@@ -2163,35 +2163,35 @@
         <v>300</v>
       </c>
       <c r="D44" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B44)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_300</v>
       </c>
       <c r="E44" t="str">
-        <f>CONCATENATE("HMI1.CB",B44,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB300_Closed</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB300_Vpu</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB300_VLgood</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE("CB", B44, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB300_MODBUS</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=43,CBID:=300,Flow:=ADR(HMI1.Flow_300),Status:=ADR(HMI1.CB300_Closed),Vpu:=ADR(HMI1.CB300_Vpu),VLgood:=ADR(HMI1.CB300_VLgood)),</v>
       </c>
     </row>
@@ -2203,35 +2203,35 @@
         <v>200</v>
       </c>
       <c r="D45" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B45)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_200</v>
       </c>
       <c r="E45" t="str">
-        <f>CONCATENATE("HMI1.CB",B45,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB200_Closed</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB200_Vpu</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB200_VLgood</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE("CB", B45, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB200_MODBUS</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=44,CBID:=200,Flow:=ADR(HMI1.Flow_200),Status:=ADR(HMI1.CB200_Closed),Vpu:=ADR(HMI1.CB200_Vpu),VLgood:=ADR(HMI1.CB200_VLgood)),</v>
       </c>
     </row>
@@ -2243,35 +2243,35 @@
         <v>100</v>
       </c>
       <c r="D46" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B46)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_100</v>
       </c>
       <c r="E46" t="str">
-        <f>CONCATENATE("HMI1.CB",B46,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB100_Closed</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB100_Vpu</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB100_VLgood</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE("CB", B46, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB100_MODBUS</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=45,CBID:=100,Flow:=ADR(HMI1.Flow_100),Status:=ADR(HMI1.CB100_Closed),Vpu:=ADR(HMI1.CB100_Vpu),VLgood:=ADR(HMI1.CB100_VLgood)),</v>
       </c>
     </row>
@@ -2283,35 +2283,35 @@
         <v>351</v>
       </c>
       <c r="D47" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B47)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_351</v>
       </c>
       <c r="E47" t="str">
-        <f>CONCATENATE("HMI1.CB",B47,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB351_Closed</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB351_Vpu</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB351_VLgood</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE("CB", B47, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB351_MODBUS</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=46,CBID:=351,Flow:=ADR(HMI1.Flow_351),Status:=ADR(HMI1.CB351_Closed),Vpu:=ADR(HMI1.CB351_Vpu),VLgood:=ADR(HMI1.CB351_VLgood)),</v>
       </c>
     </row>
@@ -2323,35 +2323,35 @@
         <v>151</v>
       </c>
       <c r="D48" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B48)</f>
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_151</v>
       </c>
       <c r="E48" t="str">
-        <f>CONCATENATE("HMI1.CB",B48,"_Closed")</f>
+        <f t="shared" si="9"/>
         <v>HMI1.CB151_Closed</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>HMI1.CB151_Vpu</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>HMI1.CB151_VLgood</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE("CB", B48, "_MODBUS")</f>
+        <f t="shared" si="10"/>
         <v>CB151_MODBUS</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>(ID:=47,CBID:=151,Flow:=ADR(HMI1.Flow_151),Status:=ADR(HMI1.CB151_Closed),Vpu:=ADR(HMI1.CB151_Vpu),VLgood:=ADR(HMI1.CB151_VLgood)),</v>
       </c>
     </row>
@@ -2360,39 +2360,35 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>401</v>
+        <v>261</v>
       </c>
       <c r="D49" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B49)</f>
-        <v>HMI1.Flow_401</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_261</v>
       </c>
       <c r="E49" t="str">
-        <f>CONCATENATE("HMI1.CB",B49,"_Closed")</f>
-        <v>HMI1.CB401_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB261_Closed</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB401_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB261_Vpu</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB401_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB261_VLgood</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE("CB", B49, "_MODBUS")</f>
-        <v>CB401_MODBUS</v>
-      </c>
-      <c r="J49" t="str">
-        <f>IF(C49="","",CONCATENATE("HMI1.BUS",C49,"_Stat"))</f>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>CB261_MODBUS</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" ref="K49:K55" si="5">IF(H49="","",CONCATENATE(",IOCCmd:=ADR(",H49,"),MBCmd:=ADR(",I49,".CMD),MBRst:=ADR(",I49,".RST)"))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L49" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=48,CBID:=401,Flow:=ADR(HMI1.Flow_401),Status:=ADR(HMI1.CB401_Closed),Vpu:=ADR(HMI1.CB401_Vpu),VLgood:=ADR(HMI1.CB401_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=48,CBID:=261,Flow:=ADR(HMI1.Flow_261),Status:=ADR(HMI1.CB261_Closed),Vpu:=ADR(HMI1.CB261_Vpu),VLgood:=ADR(HMI1.CB261_VLgood)),</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -2400,39 +2396,35 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>402</v>
+        <v>271</v>
       </c>
       <c r="D50" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B50)</f>
-        <v>HMI1.Flow_402</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_271</v>
       </c>
       <c r="E50" t="str">
-        <f>CONCATENATE("HMI1.CB",B50,"_Closed")</f>
-        <v>HMI1.CB402_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB271_Closed</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB402_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB271_Vpu</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB402_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB271_VLgood</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE("CB", B50, "_MODBUS")</f>
-        <v>CB402_MODBUS</v>
-      </c>
-      <c r="J50" t="str">
-        <f t="shared" ref="J50:J61" si="6">IF(C50="","",CONCATENATE("HMI1.BUS",C50,"_Stat"))</f>
-        <v/>
+        <f t="shared" si="10"/>
+        <v>CB271_MODBUS</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L50" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=49,CBID:=402,Flow:=ADR(HMI1.Flow_402),Status:=ADR(HMI1.CB402_Closed),Vpu:=ADR(HMI1.CB402_Vpu),VLgood:=ADR(HMI1.CB402_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=49,CBID:=271,Flow:=ADR(HMI1.Flow_271),Status:=ADR(HMI1.CB271_Closed),Vpu:=ADR(HMI1.CB271_Vpu),VLgood:=ADR(HMI1.CB271_VLgood)),</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -2440,39 +2432,39 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D51" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B51)</f>
-        <v>HMI1.Flow_403</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_401</v>
       </c>
       <c r="E51" t="str">
-        <f>CONCATENATE("HMI1.CB",B51,"_Closed")</f>
-        <v>HMI1.CB403_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB401_Closed</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB403_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB401_Vpu</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB403_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB401_VLgood</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE("CB", B51, "_MODBUS")</f>
-        <v>CB403_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB401_MODBUS</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(C51="","",CONCATENATE("HMI1.BUS",C51,"_Stat"))</f>
         <v/>
       </c>
       <c r="K51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K51:K57" si="11">IF(H51="","",CONCATENATE(",IOCCmd:=ADR(",H51,"),MBCmd:=ADR(",I51,".CMD),MBRst:=ADR(",I51,".RST)"))</f>
         <v/>
       </c>
       <c r="L51" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=50,CBID:=403,Flow:=ADR(HMI1.Flow_403),Status:=ADR(HMI1.CB403_Closed),Vpu:=ADR(HMI1.CB403_Vpu),VLgood:=ADR(HMI1.CB403_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=50,CBID:=401,Flow:=ADR(HMI1.Flow_401),Status:=ADR(HMI1.CB401_Closed),Vpu:=ADR(HMI1.CB401_Vpu),VLgood:=ADR(HMI1.CB401_VLgood)),</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -2480,39 +2472,39 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D52" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B52)</f>
-        <v>HMI1.Flow_404</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_402</v>
       </c>
       <c r="E52" t="str">
-        <f>CONCATENATE("HMI1.CB",B52,"_Closed")</f>
-        <v>HMI1.CB404_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB402_Closed</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB404_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB402_Vpu</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB404_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB402_VLgood</v>
       </c>
       <c r="I52" t="str">
-        <f>CONCATENATE("CB", B52, "_MODBUS")</f>
-        <v>CB404_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB402_MODBUS</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J52:J63" si="12">IF(C52="","",CONCATENATE("HMI1.BUS",C52,"_Stat"))</f>
         <v/>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L52" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=51,CBID:=404,Flow:=ADR(HMI1.Flow_404),Status:=ADR(HMI1.CB404_Closed),Vpu:=ADR(HMI1.CB404_Vpu),VLgood:=ADR(HMI1.CB404_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=51,CBID:=402,Flow:=ADR(HMI1.Flow_402),Status:=ADR(HMI1.CB402_Closed),Vpu:=ADR(HMI1.CB402_Vpu),VLgood:=ADR(HMI1.CB402_VLgood)),</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -2520,39 +2512,39 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D53" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B53)</f>
-        <v>HMI1.Flow_405</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_403</v>
       </c>
       <c r="E53" t="str">
-        <f>CONCATENATE("HMI1.CB",B53,"_Closed")</f>
-        <v>HMI1.CB405_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB403_Closed</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB405_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB403_Vpu</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB405_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB403_VLgood</v>
       </c>
       <c r="I53" t="str">
-        <f>CONCATENATE("CB", B53, "_MODBUS")</f>
-        <v>CB405_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB403_MODBUS</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L53" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=52,CBID:=405,Flow:=ADR(HMI1.Flow_405),Status:=ADR(HMI1.CB405_Closed),Vpu:=ADR(HMI1.CB405_Vpu),VLgood:=ADR(HMI1.CB405_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=52,CBID:=403,Flow:=ADR(HMI1.Flow_403),Status:=ADR(HMI1.CB403_Closed),Vpu:=ADR(HMI1.CB403_Vpu),VLgood:=ADR(HMI1.CB403_VLgood)),</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -2560,39 +2552,39 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D54" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B54)</f>
-        <v>HMI1.Flow_406</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_404</v>
       </c>
       <c r="E54" t="str">
-        <f>CONCATENATE("HMI1.CB",B54,"_Closed")</f>
-        <v>HMI1.CB406_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB404_Closed</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB406_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB404_Vpu</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB406_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB404_VLgood</v>
       </c>
       <c r="I54" t="str">
-        <f>CONCATENATE("CB", B54, "_MODBUS")</f>
-        <v>CB406_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB404_MODBUS</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L54" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=53,CBID:=406,Flow:=ADR(HMI1.Flow_406),Status:=ADR(HMI1.CB406_Closed),Vpu:=ADR(HMI1.CB406_Vpu),VLgood:=ADR(HMI1.CB406_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=53,CBID:=404,Flow:=ADR(HMI1.Flow_404),Status:=ADR(HMI1.CB404_Closed),Vpu:=ADR(HMI1.CB404_Vpu),VLgood:=ADR(HMI1.CB404_VLgood)),</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2600,39 +2592,39 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D55" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B55)</f>
-        <v>HMI1.Flow_407</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_405</v>
       </c>
       <c r="E55" t="str">
-        <f>CONCATENATE("HMI1.CB",B55,"_Closed")</f>
-        <v>HMI1.CB407_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB405_Closed</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB407_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB405_Vpu</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB407_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB405_VLgood</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE("CB", B55, "_MODBUS")</f>
-        <v>CB407_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB405_MODBUS</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L55" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=54,CBID:=407,Flow:=ADR(HMI1.Flow_407),Status:=ADR(HMI1.CB407_Closed),Vpu:=ADR(HMI1.CB407_Vpu),VLgood:=ADR(HMI1.CB407_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=54,CBID:=405,Flow:=ADR(HMI1.Flow_405),Status:=ADR(HMI1.CB405_Closed),Vpu:=ADR(HMI1.CB405_Vpu),VLgood:=ADR(HMI1.CB405_VLgood)),</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -2640,39 +2632,39 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D56" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B56)</f>
-        <v>HMI1.Flow_408</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_406</v>
       </c>
       <c r="E56" t="str">
-        <f>CONCATENATE("HMI1.CB",B56,"_Closed")</f>
-        <v>HMI1.CB408_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB406_Closed</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB408_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB406_Vpu</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB408_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB406_VLgood</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE("CB", B56, "_MODBUS")</f>
-        <v>CB408_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB406_MODBUS</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K56" t="str">
-        <f t="shared" ref="K56:K61" si="7">IF(H56="","",CONCATENATE(",IOCCmd:=ADR(",H56,"),MBCmd:=ADR(",I56,".CMD),MBRst:=ADR(",I56,".RST)"))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L56" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=55,CBID:=408,Flow:=ADR(HMI1.Flow_408),Status:=ADR(HMI1.CB408_Closed),Vpu:=ADR(HMI1.CB408_Vpu),VLgood:=ADR(HMI1.CB408_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=55,CBID:=406,Flow:=ADR(HMI1.Flow_406),Status:=ADR(HMI1.CB406_Closed),Vpu:=ADR(HMI1.CB406_Vpu),VLgood:=ADR(HMI1.CB406_VLgood)),</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -2680,39 +2672,39 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D57" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B57)</f>
-        <v>HMI1.Flow_409</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_407</v>
       </c>
       <c r="E57" t="str">
-        <f>CONCATENATE("HMI1.CB",B57,"_Closed")</f>
-        <v>HMI1.CB409_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB407_Closed</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB409_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB407_Vpu</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB409_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB407_VLgood</v>
       </c>
       <c r="I57" t="str">
-        <f>CONCATENATE("CB", B57, "_MODBUS")</f>
-        <v>CB409_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB407_MODBUS</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L57" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=56,CBID:=409,Flow:=ADR(HMI1.Flow_409),Status:=ADR(HMI1.CB409_Closed),Vpu:=ADR(HMI1.CB409_Vpu),VLgood:=ADR(HMI1.CB409_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=56,CBID:=407,Flow:=ADR(HMI1.Flow_407),Status:=ADR(HMI1.CB407_Closed),Vpu:=ADR(HMI1.CB407_Vpu),VLgood:=ADR(HMI1.CB407_VLgood)),</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -2720,39 +2712,39 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D58" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B58)</f>
-        <v>HMI1.Flow_410</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_408</v>
       </c>
       <c r="E58" t="str">
-        <f>CONCATENATE("HMI1.CB",B58,"_Closed")</f>
-        <v>HMI1.CB410_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB408_Closed</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB410_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB408_Vpu</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB410_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB408_VLgood</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE("CB", B58, "_MODBUS")</f>
-        <v>CB410_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB408_MODBUS</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K58:K63" si="13">IF(H58="","",CONCATENATE(",IOCCmd:=ADR(",H58,"),MBCmd:=ADR(",I58,".CMD),MBRst:=ADR(",I58,".RST)"))</f>
         <v/>
       </c>
       <c r="L58" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=57,CBID:=410,Flow:=ADR(HMI1.Flow_410),Status:=ADR(HMI1.CB410_Closed),Vpu:=ADR(HMI1.CB410_Vpu),VLgood:=ADR(HMI1.CB410_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=57,CBID:=408,Flow:=ADR(HMI1.Flow_408),Status:=ADR(HMI1.CB408_Closed),Vpu:=ADR(HMI1.CB408_Vpu),VLgood:=ADR(HMI1.CB408_VLgood)),</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -2760,39 +2752,39 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D59" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B59)</f>
-        <v>HMI1.Flow_411</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_409</v>
       </c>
       <c r="E59" t="str">
-        <f>CONCATENATE("HMI1.CB",B59,"_Closed")</f>
-        <v>HMI1.CB411_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB409_Closed</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB411_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB409_Vpu</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB411_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB409_VLgood</v>
       </c>
       <c r="I59" t="str">
-        <f>CONCATENATE("CB", B59, "_MODBUS")</f>
-        <v>CB411_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB409_MODBUS</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="L59" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=58,CBID:=411,Flow:=ADR(HMI1.Flow_411),Status:=ADR(HMI1.CB411_Closed),Vpu:=ADR(HMI1.CB411_Vpu),VLgood:=ADR(HMI1.CB411_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=58,CBID:=409,Flow:=ADR(HMI1.Flow_409),Status:=ADR(HMI1.CB409_Closed),Vpu:=ADR(HMI1.CB409_Vpu),VLgood:=ADR(HMI1.CB409_VLgood)),</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2800,39 +2792,39 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D60" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B60)</f>
-        <v>HMI1.Flow_412</v>
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_410</v>
       </c>
       <c r="E60" t="str">
-        <f>CONCATENATE("HMI1.CB",B60,"_Closed")</f>
-        <v>HMI1.CB412_Closed</v>
+        <f t="shared" si="9"/>
+        <v>HMI1.CB410_Closed</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="2"/>
-        <v>HMI1.CB412_Vpu</v>
+        <f t="shared" si="5"/>
+        <v>HMI1.CB410_Vpu</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="3"/>
-        <v>HMI1.CB412_VLgood</v>
+        <f t="shared" si="6"/>
+        <v>HMI1.CB410_VLgood</v>
       </c>
       <c r="I60" t="str">
-        <f>CONCATENATE("CB", B60, "_MODBUS")</f>
-        <v>CB412_MODBUS</v>
+        <f t="shared" si="10"/>
+        <v>CB410_MODBUS</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="L60" t="str">
-        <f t="shared" si="1"/>
-        <v>(ID:=59,CBID:=412,Flow:=ADR(HMI1.Flow_412),Status:=ADR(HMI1.CB412_Closed),Vpu:=ADR(HMI1.CB412_Vpu),VLgood:=ADR(HMI1.CB412_VLgood)),</v>
+        <f t="shared" si="4"/>
+        <v>(ID:=59,CBID:=410,Flow:=ADR(HMI1.Flow_410),Status:=ADR(HMI1.CB410_Closed),Vpu:=ADR(HMI1.CB410_Vpu),VLgood:=ADR(HMI1.CB410_VLgood)),</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -2840,39 +2832,119 @@
         <v>60</v>
       </c>
       <c r="B61">
+        <v>411</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_411</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="9"/>
+        <v>HMI1.CB411_Closed</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="5"/>
+        <v>HMI1.CB411_Vpu</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.CB411_VLgood</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="10"/>
+        <v>CB411_MODBUS</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="4"/>
+        <v>(ID:=60,CBID:=411,Flow:=ADR(HMI1.Flow_411),Status:=ADR(HMI1.CB411_Closed),Vpu:=ADR(HMI1.CB411_Vpu),VLgood:=ADR(HMI1.CB411_VLgood)),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>412</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="8"/>
+        <v>HMI1.Flow_412</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="9"/>
+        <v>HMI1.CB412_Closed</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="5"/>
+        <v>HMI1.CB412_Vpu</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="6"/>
+        <v>HMI1.CB412_VLgood</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="10"/>
+        <v>CB412_MODBUS</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="4"/>
+        <v>(ID:=61,CBID:=412,Flow:=ADR(HMI1.Flow_412),Status:=ADR(HMI1.CB412_Closed),Vpu:=ADR(HMI1.CB412_Vpu),VLgood:=ADR(HMI1.CB412_VLgood)),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
         <v>413</v>
       </c>
-      <c r="D61" t="str">
-        <f>CONCATENATE("HMI1.Flow_",B61)</f>
+      <c r="D63" t="str">
+        <f t="shared" si="8"/>
         <v>HMI1.Flow_413</v>
       </c>
-      <c r="E61" t="str">
-        <f>CONCATENATE("HMI1.CB",B61,"_Closed")</f>
+      <c r="E63" t="str">
+        <f t="shared" si="9"/>
         <v>HMI1.CB413_Closed</v>
       </c>
-      <c r="F61" t="str">
-        <f t="shared" si="2"/>
+      <c r="F63" t="str">
+        <f t="shared" si="5"/>
         <v>HMI1.CB413_Vpu</v>
       </c>
-      <c r="G61" t="str">
-        <f t="shared" si="3"/>
+      <c r="G63" t="str">
+        <f t="shared" si="6"/>
         <v>HMI1.CB413_VLgood</v>
       </c>
-      <c r="I61" t="str">
-        <f>CONCATENATE("CB", B61, "_MODBUS")</f>
+      <c r="I63" t="str">
+        <f t="shared" si="10"/>
         <v>CB413_MODBUS</v>
       </c>
-      <c r="J61" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="K61" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L61" t="str">
-        <f>CONCATENATE("(ID:=",A61,",CBID:=",B61,",Flow:=ADR(HMI1.Flow_",B61,"),Status:=ADR(",E61,"),Vpu:=ADR(",F61,"),VLgood:=ADR(",G61,")",K61,"),")</f>
-        <v>(ID:=60,CBID:=413,Flow:=ADR(HMI1.Flow_413),Status:=ADR(HMI1.CB413_Closed),Vpu:=ADR(HMI1.CB413_Vpu),VLgood:=ADR(HMI1.CB413_VLgood)),</v>
+      <c r="J63" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="L63" t="str">
+        <f>CONCATENATE("(ID:=",A63,",CBID:=",B63,",Flow:=ADR(HMI1.Flow_",B63,"),Status:=ADR(",E63,"),Vpu:=ADR(",F63,"),VLgood:=ADR(",G63,")",K63,"),")</f>
+        <v>(ID:=62,CBID:=413,Flow:=ADR(HMI1.Flow_413),Status:=ADR(HMI1.CB413_Closed),Vpu:=ADR(HMI1.CB413_Vpu),VLgood:=ADR(HMI1.CB413_VLgood)),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MGC_SEL_programming.xlsx excel spreadsheet to add additonal CB for PV and ESS
</commit_message>
<xml_diff>
--- a/SimulationTools/RTAC/MGC_SEL_programming.xlsx
+++ b/SimulationTools/RTAC/MGC_SEL_programming.xlsx
@@ -375,8 +375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49:G50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated SEL project to new UDP frame
</commit_message>
<xml_diff>
--- a/SimulationTools/RTAC/MGC_SEL_programming.xlsx
+++ b/SimulationTools/RTAC/MGC_SEL_programming.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Structure initialisation string</t>
   </si>
@@ -373,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI63"/>
+  <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,7 +389,7 @@
     <col min="12" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -400,639 +400,636 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>301</v>
+        <v>101</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D33" si="0">CONCATENATE("HMI1.Flow_",B2)</f>
-        <v>HMI1.Flow_301</v>
+        <f>CONCATENATE("HMI1.Flow_",B2)</f>
+        <v>HMI1.Flow_101</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="1">CONCATENATE("HMI1.CB",B2,"_Closed")</f>
-        <v>HMI1.CB301_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B2,"_Closed")</f>
+        <v>HMI1.CB101_Closed</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE("HMI1.CB",B2,"_Vpu")</f>
-        <v>HMI1.CB301_Vpu</v>
+        <v>HMI1.CB101_Vpu</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE("HMI1.CB",B2,"_VLgood")</f>
-        <v>HMI1.CB301_VLgood</v>
+        <v>HMI1.CB101_VLgood</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE("HMI1.CB",B2,"_Cmd")</f>
-        <v>HMI1.CB301_Cmd</v>
+        <v>HMI1.CB101_Cmd</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I33" si="2">CONCATENATE("CB", B2, "_MODBUS")</f>
-        <v>CB301_MODBUS</v>
+        <f>CONCATENATE("CB", B2, "_MODBUS")</f>
+        <v>CB101_MODBUS</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J48" si="3">IF(C2="","",CONCATENATE("HMI1.BUS",C2,"_Stat"))</f>
+        <f>IF(C2="","",CONCATENATE("HMI1.BUS",C2,"_Stat"))</f>
         <v/>
       </c>
       <c r="K2" t="str">
         <f>IF(H2="","",CONCATENATE(",IOCCmd:=ADR(",H2,"),MBCmd:=ADR(",I2,".CMD),MBRst:=ADR(",I2,".RST)"))</f>
-        <v>,IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)</v>
+        <v>,IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)</v>
       </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L62" si="4">CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",E2,"),Vpu:=ADR(",F2,"),VLgood:=ADR(",G2,")",K2,"),")</f>
-        <v>(ID:=1,CBID:=301,Flow:=ADR(HMI1.Flow_301),Status:=ADR(HMI1.CB301_Closed),Vpu:=ADR(HMI1.CB301_Vpu),VLgood:=ADR(HMI1.CB301_VLgood),IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)),</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A2,",CBID:=",B2,",Flow:=ADR(HMI1.Flow_",B2,"),Status:=ADR(",E2,"),Vpu:=ADR(",F2,"),VLgood:=ADR(",G2,")",K2,"),")</f>
+        <v>(ID:=1,CBID:=101,Flow:=ADR(HMI1.Flow_101),Status:=ADR(HMI1.CB101_Closed),Vpu:=ADR(HMI1.CB101_Vpu),VLgood:=ADR(HMI1.CB101_VLgood),IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>302</v>
+        <v>102</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_302</v>
+        <f>CONCATENATE("HMI1.Flow_",B3)</f>
+        <v>HMI1.Flow_102</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB302_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B3,"_Closed")</f>
+        <v>HMI1.CB102_Closed</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F63" si="5">CONCATENATE("HMI1.CB",B3,"_Vpu")</f>
-        <v>HMI1.CB302_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B3,"_Vpu")</f>
+        <v>HMI1.CB102_Vpu</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G63" si="6">CONCATENATE("HMI1.CB",B3,"_VLgood")</f>
-        <v>HMI1.CB302_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B3,"_VLgood")</f>
+        <v>HMI1.CB102_VLgood</v>
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE("HMI1.CB",B3,"_Cmd")</f>
-        <v>HMI1.CB302_Cmd</v>
+        <v>HMI1.CB102_Cmd</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="2"/>
-        <v>CB302_MODBUS</v>
+        <f>CONCATENATE("CB", B3, "_MODBUS")</f>
+        <v>CB102_MODBUS</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C3="","",CONCATENATE("HMI1.BUS",C3,"_Stat"))</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K50" si="7">IF(H3="","",CONCATENATE(",IOCCmd:=ADR(",H3,"),MBCmd:=ADR(",I3,".CMD),MBRst:=ADR(",I3,".RST)"))</f>
-        <v>,IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)</v>
+        <f>IF(H3="","",CONCATENATE(",IOCCmd:=ADR(",H3,"),MBCmd:=ADR(",I3,".CMD),MBRst:=ADR(",I3,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=2,CBID:=302,Flow:=ADR(HMI1.Flow_302),Status:=ADR(HMI1.CB302_Closed),Vpu:=ADR(HMI1.CB302_Vpu),VLgood:=ADR(HMI1.CB302_VLgood),IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A3,",CBID:=",B3,",Flow:=ADR(HMI1.Flow_",B3,"),Status:=ADR(",E3,"),Vpu:=ADR(",F3,"),VLgood:=ADR(",G3,")",K3,"),")</f>
+        <v>(ID:=2,CBID:=102,Flow:=ADR(HMI1.Flow_102),Status:=ADR(HMI1.CB102_Closed),Vpu:=ADR(HMI1.CB102_Vpu),VLgood:=ADR(HMI1.CB102_VLgood),IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>303</v>
+        <v>103</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_303</v>
+        <f>CONCATENATE("HMI1.Flow_",B4)</f>
+        <v>HMI1.Flow_103</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB303_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B4,"_Closed")</f>
+        <v>HMI1.CB103_Closed</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB303_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B4,"_Vpu")</f>
+        <v>HMI1.CB103_Vpu</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB303_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B4,"_VLgood")</f>
+        <v>HMI1.CB103_VLgood</v>
       </c>
       <c r="H4" t="str">
         <f>CONCATENATE("HMI1.CB",B4,"_Cmd")</f>
-        <v>HMI1.CB303_Cmd</v>
+        <v>HMI1.CB103_Cmd</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="2"/>
-        <v>CB303_MODBUS</v>
+        <f>CONCATENATE("CB", B4, "_MODBUS")</f>
+        <v>CB103_MODBUS</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C4="","",CONCATENATE("HMI1.BUS",C4,"_Stat"))</f>
         <v/>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)</v>
+        <f>IF(H4="","",CONCATENATE(",IOCCmd:=ADR(",H4,"),MBCmd:=ADR(",I4,".CMD),MBRst:=ADR(",I4,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=3,CBID:=303,Flow:=ADR(HMI1.Flow_303),Status:=ADR(HMI1.CB303_Closed),Vpu:=ADR(HMI1.CB303_Vpu),VLgood:=ADR(HMI1.CB303_VLgood),IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A4,",CBID:=",B4,",Flow:=ADR(HMI1.Flow_",B4,"),Status:=ADR(",E4,"),Vpu:=ADR(",F4,"),VLgood:=ADR(",G4,")",K4,"),")</f>
+        <v>(ID:=3,CBID:=103,Flow:=ADR(HMI1.Flow_103),Status:=ADR(HMI1.CB103_Closed),Vpu:=ADR(HMI1.CB103_Vpu),VLgood:=ADR(HMI1.CB103_VLgood),IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>304</v>
+        <v>104</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_304</v>
+        <f>CONCATENATE("HMI1.Flow_",B5)</f>
+        <v>HMI1.Flow_104</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB304_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B5,"_Closed")</f>
+        <v>HMI1.CB104_Closed</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB304_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B5,"_Vpu")</f>
+        <v>HMI1.CB104_Vpu</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB304_VLgood</v>
-      </c>
-      <c r="H5" t="str">
-        <f>CONCATENATE("HMI1.CB",B5,"_Cmd")</f>
-        <v>HMI1.CB304_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B5,"_VLgood")</f>
+        <v>HMI1.CB104_VLgood</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="2"/>
-        <v>CB304_MODBUS</v>
+        <f>CONCATENATE("CB", B5, "_MODBUS")</f>
+        <v>CB104_MODBUS</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C5="","",CONCATENATE("HMI1.BUS",C5,"_Stat"))</f>
         <v/>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)</v>
+        <f>IF(H5="","",CONCATENATE(",IOCCmd:=ADR(",H5,"),MBCmd:=ADR(",I5,".CMD),MBRst:=ADR(",I5,".RST)"))</f>
+        <v/>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=4,CBID:=304,Flow:=ADR(HMI1.Flow_304),Status:=ADR(HMI1.CB304_Closed),Vpu:=ADR(HMI1.CB304_Vpu),VLgood:=ADR(HMI1.CB304_VLgood),IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A5,",CBID:=",B5,",Flow:=ADR(HMI1.Flow_",B5,"),Status:=ADR(",E5,"),Vpu:=ADR(",F5,"),VLgood:=ADR(",G5,")",K5,"),")</f>
+        <v>(ID:=4,CBID:=104,Flow:=ADR(HMI1.Flow_104),Status:=ADR(HMI1.CB104_Closed),Vpu:=ADR(HMI1.CB104_Vpu),VLgood:=ADR(HMI1.CB104_VLgood)),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>305</v>
+        <v>105</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_305</v>
+        <f>CONCATENATE("HMI1.Flow_",B6)</f>
+        <v>HMI1.Flow_105</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB305_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B6,"_Closed")</f>
+        <v>HMI1.CB105_Closed</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB305_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B6,"_Vpu")</f>
+        <v>HMI1.CB105_Vpu</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB305_VLgood</v>
-      </c>
-      <c r="H6" t="str">
-        <f>CONCATENATE("HMI1.CB",B6,"_Cmd")</f>
-        <v>HMI1.CB305_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B6,"_VLgood")</f>
+        <v>HMI1.CB105_VLgood</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="2"/>
-        <v>CB305_MODBUS</v>
+        <f>CONCATENATE("CB", B6, "_MODBUS")</f>
+        <v>CB105_MODBUS</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C6="","",CONCATENATE("HMI1.BUS",C6,"_Stat"))</f>
         <v/>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)</v>
+        <f>IF(H6="","",CONCATENATE(",IOCCmd:=ADR(",H6,"),MBCmd:=ADR(",I6,".CMD),MBRst:=ADR(",I6,".RST)"))</f>
+        <v/>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=5,CBID:=305,Flow:=ADR(HMI1.Flow_305),Status:=ADR(HMI1.CB305_Closed),Vpu:=ADR(HMI1.CB305_Vpu),VLgood:=ADR(HMI1.CB305_VLgood),IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A6,",CBID:=",B6,",Flow:=ADR(HMI1.Flow_",B6,"),Status:=ADR(",E6,"),Vpu:=ADR(",F6,"),VLgood:=ADR(",G6,")",K6,"),")</f>
+        <v>(ID:=5,CBID:=105,Flow:=ADR(HMI1.Flow_105),Status:=ADR(HMI1.CB105_Closed),Vpu:=ADR(HMI1.CB105_Vpu),VLgood:=ADR(HMI1.CB105_VLgood)),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>306</v>
+        <v>106</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_306</v>
+        <f>CONCATENATE("HMI1.Flow_",B7)</f>
+        <v>HMI1.Flow_106</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB306_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B7,"_Closed")</f>
+        <v>HMI1.CB106_Closed</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB306_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B7,"_Vpu")</f>
+        <v>HMI1.CB106_Vpu</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB306_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B7,"_VLgood")</f>
+        <v>HMI1.CB106_VLgood</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="2"/>
-        <v>CB306_MODBUS</v>
+        <f>CONCATENATE("CB", B7, "_MODBUS")</f>
+        <v>CB106_MODBUS</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C7="","",CONCATENATE("HMI1.BUS",C7,"_Stat"))</f>
         <v/>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H7="","",CONCATENATE(",IOCCmd:=ADR(",H7,"),MBCmd:=ADR(",I7,".CMD),MBRst:=ADR(",I7,".RST)"))</f>
         <v/>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=6,CBID:=306,Flow:=ADR(HMI1.Flow_306),Status:=ADR(HMI1.CB306_Closed),Vpu:=ADR(HMI1.CB306_Vpu),VLgood:=ADR(HMI1.CB306_VLgood)),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A7,",CBID:=",B7,",Flow:=ADR(HMI1.Flow_",B7,"),Status:=ADR(",E7,"),Vpu:=ADR(",F7,"),VLgood:=ADR(",G7,")",K7,"),")</f>
+        <v>(ID:=6,CBID:=106,Flow:=ADR(HMI1.Flow_106),Status:=ADR(HMI1.CB106_Closed),Vpu:=ADR(HMI1.CB106_Vpu),VLgood:=ADR(HMI1.CB106_VLgood)),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>307</v>
+        <v>107</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_307</v>
+        <f>CONCATENATE("HMI1.Flow_",B8)</f>
+        <v>HMI1.Flow_107</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB307_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B8,"_Closed")</f>
+        <v>HMI1.CB107_Closed</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB307_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B8,"_Vpu")</f>
+        <v>HMI1.CB107_Vpu</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB307_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B8,"_VLgood")</f>
+        <v>HMI1.CB107_VLgood</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>CB307_MODBUS</v>
+        <f>CONCATENATE("CB", B8, "_MODBUS")</f>
+        <v>CB107_MODBUS</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C8="","",CONCATENATE("HMI1.BUS",C8,"_Stat"))</f>
         <v/>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H8="","",CONCATENATE(",IOCCmd:=ADR(",H8,"),MBCmd:=ADR(",I8,".CMD),MBRst:=ADR(",I8,".RST)"))</f>
         <v/>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=7,CBID:=307,Flow:=ADR(HMI1.Flow_307),Status:=ADR(HMI1.CB307_Closed),Vpu:=ADR(HMI1.CB307_Vpu),VLgood:=ADR(HMI1.CB307_VLgood)),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A8,",CBID:=",B8,",Flow:=ADR(HMI1.Flow_",B8,"),Status:=ADR(",E8,"),Vpu:=ADR(",F8,"),VLgood:=ADR(",G8,")",K8,"),")</f>
+        <v>(ID:=7,CBID:=107,Flow:=ADR(HMI1.Flow_107),Status:=ADR(HMI1.CB107_Closed),Vpu:=ADR(HMI1.CB107_Vpu),VLgood:=ADR(HMI1.CB107_VLgood)),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>308</v>
+        <v>108</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_308</v>
+        <f>CONCATENATE("HMI1.Flow_",B9)</f>
+        <v>HMI1.Flow_108</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB308_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B9,"_Closed")</f>
+        <v>HMI1.CB108_Closed</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB308_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B9,"_Vpu")</f>
+        <v>HMI1.CB108_Vpu</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB308_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B9,"_VLgood")</f>
+        <v>HMI1.CB108_VLgood</v>
+      </c>
+      <c r="H9" t="str">
+        <f>CONCATENATE("HMI1.CB",B9,"_Cmd")</f>
+        <v>HMI1.CB108_Cmd</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="2"/>
-        <v>CB308_MODBUS</v>
+        <f>CONCATENATE("CB", B9, "_MODBUS")</f>
+        <v>CB108_MODBUS</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C9="","",CONCATENATE("HMI1.BUS",C9,"_Stat"))</f>
         <v/>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H9="","",CONCATENATE(",IOCCmd:=ADR(",H9,"),MBCmd:=ADR(",I9,".CMD),MBRst:=ADR(",I9,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=8,CBID:=308,Flow:=ADR(HMI1.Flow_308),Status:=ADR(HMI1.CB308_Closed),Vpu:=ADR(HMI1.CB308_Vpu),VLgood:=ADR(HMI1.CB308_VLgood)),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A9,",CBID:=",B9,",Flow:=ADR(HMI1.Flow_",B9,"),Status:=ADR(",E9,"),Vpu:=ADR(",F9,"),VLgood:=ADR(",G9,")",K9,"),")</f>
+        <v>(ID:=8,CBID:=108,Flow:=ADR(HMI1.Flow_108),Status:=ADR(HMI1.CB108_Closed),Vpu:=ADR(HMI1.CB108_Vpu),VLgood:=ADR(HMI1.CB108_VLgood),IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>309</v>
+        <v>109</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_309</v>
+        <f>CONCATENATE("HMI1.Flow_",B10)</f>
+        <v>HMI1.Flow_109</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB309_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B10,"_Closed")</f>
+        <v>HMI1.CB109_Closed</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB309_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B10,"_Vpu")</f>
+        <v>HMI1.CB109_Vpu</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB309_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B10,"_VLgood")</f>
+        <v>HMI1.CB109_VLgood</v>
+      </c>
+      <c r="H10" t="str">
+        <f>CONCATENATE("HMI1.CB",B10,"_Cmd")</f>
+        <v>HMI1.CB109_Cmd</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="2"/>
-        <v>CB309_MODBUS</v>
+        <f>CONCATENATE("CB", B10, "_MODBUS")</f>
+        <v>CB109_MODBUS</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C10="","",CONCATENATE("HMI1.BUS",C10,"_Stat"))</f>
         <v/>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H10="","",CONCATENATE(",IOCCmd:=ADR(",H10,"),MBCmd:=ADR(",I10,".CMD),MBRst:=ADR(",I10,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=9,CBID:=309,Flow:=ADR(HMI1.Flow_309),Status:=ADR(HMI1.CB309_Closed),Vpu:=ADR(HMI1.CB309_Vpu),VLgood:=ADR(HMI1.CB309_VLgood)),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A10,",CBID:=",B10,",Flow:=ADR(HMI1.Flow_",B10,"),Status:=ADR(",E10,"),Vpu:=ADR(",F10,"),VLgood:=ADR(",G10,")",K10,"),")</f>
+        <v>(ID:=9,CBID:=109,Flow:=ADR(HMI1.Flow_109),Status:=ADR(HMI1.CB109_Closed),Vpu:=ADR(HMI1.CB109_Vpu),VLgood:=ADR(HMI1.CB109_VLgood),IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>201</v>
+        <v>110</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_201</v>
+        <f>CONCATENATE("HMI1.Flow_",B11)</f>
+        <v>HMI1.Flow_110</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB201_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B11,"_Closed")</f>
+        <v>HMI1.CB110_Closed</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB201_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B11,"_Vpu")</f>
+        <v>HMI1.CB110_Vpu</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB201_VLgood</v>
-      </c>
-      <c r="H11" t="str">
-        <f>CONCATENATE("HMI1.CB",B11,"_Cmd")</f>
-        <v>HMI1.CB201_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B11,"_VLgood")</f>
+        <v>HMI1.CB110_VLgood</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="2"/>
-        <v>CB201_MODBUS</v>
+        <f>CONCATENATE("CB", B11, "_MODBUS")</f>
+        <v>CB110_MODBUS</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C11="","",CONCATENATE("HMI1.BUS",C11,"_Stat"))</f>
         <v/>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)</v>
+        <f>IF(H11="","",CONCATENATE(",IOCCmd:=ADR(",H11,"),MBCmd:=ADR(",I11,".CMD),MBRst:=ADR(",I11,".RST)"))</f>
+        <v/>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=10,CBID:=201,Flow:=ADR(HMI1.Flow_201),Status:=ADR(HMI1.CB201_Closed),Vpu:=ADR(HMI1.CB201_Vpu),VLgood:=ADR(HMI1.CB201_VLgood),IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A11,",CBID:=",B11,",Flow:=ADR(HMI1.Flow_",B11,"),Status:=ADR(",E11,"),Vpu:=ADR(",F11,"),VLgood:=ADR(",G11,")",K11,"),")</f>
+        <v>(ID:=10,CBID:=110,Flow:=ADR(HMI1.Flow_110),Status:=ADR(HMI1.CB110_Closed),Vpu:=ADR(HMI1.CB110_Vpu),VLgood:=ADR(HMI1.CB110_VLgood)),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>202</v>
+        <v>111</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_202</v>
+        <f>CONCATENATE("HMI1.Flow_",B12)</f>
+        <v>HMI1.Flow_111</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB202_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B12,"_Closed")</f>
+        <v>HMI1.CB111_Closed</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB202_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B12,"_Vpu")</f>
+        <v>HMI1.CB111_Vpu</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB202_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B12,"_VLgood")</f>
+        <v>HMI1.CB111_VLgood</v>
       </c>
       <c r="H12" t="str">
         <f>CONCATENATE("HMI1.CB",B12,"_Cmd")</f>
-        <v>HMI1.CB202_Cmd</v>
+        <v>HMI1.CB111_Cmd</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="2"/>
-        <v>CB202_MODBUS</v>
+        <f>CONCATENATE("CB", B12, "_MODBUS")</f>
+        <v>CB111_MODBUS</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C12="","",CONCATENATE("HMI1.BUS",C12,"_Stat"))</f>
         <v/>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)</v>
+        <f>IF(H12="","",CONCATENATE(",IOCCmd:=ADR(",H12,"),MBCmd:=ADR(",I12,".CMD),MBRst:=ADR(",I12,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=11,CBID:=202,Flow:=ADR(HMI1.Flow_202),Status:=ADR(HMI1.CB202_Closed),Vpu:=ADR(HMI1.CB202_Vpu),VLgood:=ADR(HMI1.CB202_VLgood),IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A12,",CBID:=",B12,",Flow:=ADR(HMI1.Flow_",B12,"),Status:=ADR(",E12,"),Vpu:=ADR(",F12,"),VLgood:=ADR(",G12,")",K12,"),")</f>
+        <v>(ID:=11,CBID:=111,Flow:=ADR(HMI1.Flow_111),Status:=ADR(HMI1.CB111_Closed),Vpu:=ADR(HMI1.CB111_Vpu),VLgood:=ADR(HMI1.CB111_VLgood),IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>203</v>
+        <v>112</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_203</v>
+        <f>CONCATENATE("HMI1.Flow_",B13)</f>
+        <v>HMI1.Flow_112</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB203_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B13,"_Closed")</f>
+        <v>HMI1.CB112_Closed</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB203_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B13,"_Vpu")</f>
+        <v>HMI1.CB112_Vpu</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB203_VLgood</v>
-      </c>
-      <c r="H13" t="str">
-        <f>CONCATENATE("HMI1.CB",B13,"_Cmd")</f>
-        <v>HMI1.CB203_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B13,"_VLgood")</f>
+        <v>HMI1.CB112_VLgood</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="2"/>
-        <v>CB203_MODBUS</v>
+        <f>CONCATENATE("CB", B13, "_MODBUS")</f>
+        <v>CB112_MODBUS</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C13="","",CONCATENATE("HMI1.BUS",C13,"_Stat"))</f>
         <v/>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)</v>
+        <f>IF(H13="","",CONCATENATE(",IOCCmd:=ADR(",H13,"),MBCmd:=ADR(",I13,".CMD),MBRst:=ADR(",I13,".RST)"))</f>
+        <v/>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=12,CBID:=203,Flow:=ADR(HMI1.Flow_203),Status:=ADR(HMI1.CB203_Closed),Vpu:=ADR(HMI1.CB203_Vpu),VLgood:=ADR(HMI1.CB203_VLgood),IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A13,",CBID:=",B13,",Flow:=ADR(HMI1.Flow_",B13,"),Status:=ADR(",E13,"),Vpu:=ADR(",F13,"),VLgood:=ADR(",G13,")",K13,"),")</f>
+        <v>(ID:=12,CBID:=112,Flow:=ADR(HMI1.Flow_112),Status:=ADR(HMI1.CB112_Closed),Vpu:=ADR(HMI1.CB112_Vpu),VLgood:=ADR(HMI1.CB112_VLgood)),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>204</v>
+        <v>113</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_204</v>
+        <f>CONCATENATE("HMI1.Flow_",B14)</f>
+        <v>HMI1.Flow_113</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB204_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B14,"_Closed")</f>
+        <v>HMI1.CB113_Closed</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB204_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B14,"_Vpu")</f>
+        <v>HMI1.CB113_Vpu</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB204_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B14,"_VLgood")</f>
+        <v>HMI1.CB113_VLgood</v>
+      </c>
+      <c r="H14" t="str">
+        <f>CONCATENATE("HMI1.CB",B14,"_Cmd")</f>
+        <v>HMI1.CB113_Cmd</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="2"/>
-        <v>CB204_MODBUS</v>
+        <f>CONCATENATE("CB", B14, "_MODBUS")</f>
+        <v>CB113_MODBUS</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C14="","",CONCATENATE("HMI1.BUS",C14,"_Stat"))</f>
         <v/>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H14="","",CONCATENATE(",IOCCmd:=ADR(",H14,"),MBCmd:=ADR(",I14,".CMD),MBRst:=ADR(",I14,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=13,CBID:=204,Flow:=ADR(HMI1.Flow_204),Status:=ADR(HMI1.CB204_Closed),Vpu:=ADR(HMI1.CB204_Vpu),VLgood:=ADR(HMI1.CB204_VLgood)),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A14,",CBID:=",B14,",Flow:=ADR(HMI1.Flow_",B14,"),Status:=ADR(",E14,"),Vpu:=ADR(",F14,"),VLgood:=ADR(",G14,")",K14,"),")</f>
+        <v>(ID:=13,CBID:=113,Flow:=ADR(HMI1.Flow_113),Status:=ADR(HMI1.CB113_Closed),Vpu:=ADR(HMI1.CB113_Vpu),VLgood:=ADR(HMI1.CB113_VLgood),IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>205</v>
+        <v>114</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_205</v>
+        <f>CONCATENATE("HMI1.Flow_",B15)</f>
+        <v>HMI1.Flow_114</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB205_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B15,"_Closed")</f>
+        <v>HMI1.CB114_Closed</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB205_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B15,"_Vpu")</f>
+        <v>HMI1.CB114_Vpu</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB205_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B15,"_VLgood")</f>
+        <v>HMI1.CB114_VLgood</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="2"/>
-        <v>CB205_MODBUS</v>
+        <f>CONCATENATE("CB", B15, "_MODBUS")</f>
+        <v>CB114_MODBUS</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C15="","",CONCATENATE("HMI1.BUS",C15,"_Stat"))</f>
         <v/>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H15="","",CONCATENATE(",IOCCmd:=ADR(",H15,"),MBCmd:=ADR(",I15,".CMD),MBRst:=ADR(",I15,".RST)"))</f>
         <v/>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=14,CBID:=205,Flow:=ADR(HMI1.Flow_205),Status:=ADR(HMI1.CB205_Closed),Vpu:=ADR(HMI1.CB205_Vpu),VLgood:=ADR(HMI1.CB205_VLgood)),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A15,",CBID:=",B15,",Flow:=ADR(HMI1.Flow_",B15,"),Status:=ADR(",E15,"),Vpu:=ADR(",F15,"),VLgood:=ADR(",G15,")",K15,"),")</f>
+        <v>(ID:=14,CBID:=114,Flow:=ADR(HMI1.Flow_114),Status:=ADR(HMI1.CB114_Closed),Vpu:=ADR(HMI1.CB114_Vpu),VLgood:=ADR(HMI1.CB114_VLgood)),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_206</v>
+        <f>CONCATENATE("HMI1.Flow_",B16)</f>
+        <v>HMI1.Flow_201</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB206_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B16,"_Closed")</f>
+        <v>HMI1.CB201_Closed</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB206_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B16,"_Vpu")</f>
+        <v>HMI1.CB201_Vpu</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB206_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B16,"_VLgood")</f>
+        <v>HMI1.CB201_VLgood</v>
+      </c>
+      <c r="H16" t="str">
+        <f>CONCATENATE("HMI1.CB",B16,"_Cmd")</f>
+        <v>HMI1.CB201_Cmd</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="2"/>
-        <v>CB206_MODBUS</v>
+        <f>CONCATENATE("CB", B16, "_MODBUS")</f>
+        <v>CB201_MODBUS</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C16="","",CONCATENATE("HMI1.BUS",C16,"_Stat"))</f>
         <v/>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H16="","",CONCATENATE(",IOCCmd:=ADR(",H16,"),MBCmd:=ADR(",I16,".CMD),MBRst:=ADR(",I16,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=15,CBID:=206,Flow:=ADR(HMI1.Flow_206),Status:=ADR(HMI1.CB206_Closed),Vpu:=ADR(HMI1.CB206_Vpu),VLgood:=ADR(HMI1.CB206_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A16,",CBID:=",B16,",Flow:=ADR(HMI1.Flow_",B16,"),Status:=ADR(",E16,"),Vpu:=ADR(",F16,"),VLgood:=ADR(",G16,")",K16,"),")</f>
+        <v>(ID:=15,CBID:=201,Flow:=ADR(HMI1.Flow_201),Status:=ADR(HMI1.CB201_Closed),Vpu:=ADR(HMI1.CB201_Vpu),VLgood:=ADR(HMI1.CB201_VLgood),IOCCmd:=ADR(HMI1.CB201_Cmd),MBCmd:=ADR(CB201_MODBUS.CMD),MBRst:=ADR(CB201_MODBUS.RST)),</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1040,39 +1037,43 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_207</v>
+        <f>CONCATENATE("HMI1.Flow_",B17)</f>
+        <v>HMI1.Flow_202</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB207_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B17,"_Closed")</f>
+        <v>HMI1.CB202_Closed</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB207_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B17,"_Vpu")</f>
+        <v>HMI1.CB202_Vpu</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB207_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B17,"_VLgood")</f>
+        <v>HMI1.CB202_VLgood</v>
+      </c>
+      <c r="H17" t="str">
+        <f>CONCATENATE("HMI1.CB",B17,"_Cmd")</f>
+        <v>HMI1.CB202_Cmd</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="2"/>
-        <v>CB207_MODBUS</v>
+        <f>CONCATENATE("CB", B17, "_MODBUS")</f>
+        <v>CB202_MODBUS</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C17="","",CONCATENATE("HMI1.BUS",C17,"_Stat"))</f>
         <v/>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H17="","",CONCATENATE(",IOCCmd:=ADR(",H17,"),MBCmd:=ADR(",I17,".CMD),MBRst:=ADR(",I17,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=16,CBID:=207,Flow:=ADR(HMI1.Flow_207),Status:=ADR(HMI1.CB207_Closed),Vpu:=ADR(HMI1.CB207_Vpu),VLgood:=ADR(HMI1.CB207_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A17,",CBID:=",B17,",Flow:=ADR(HMI1.Flow_",B17,"),Status:=ADR(",E17,"),Vpu:=ADR(",F17,"),VLgood:=ADR(",G17,")",K17,"),")</f>
+        <v>(ID:=16,CBID:=202,Flow:=ADR(HMI1.Flow_202),Status:=ADR(HMI1.CB202_Closed),Vpu:=ADR(HMI1.CB202_Vpu),VLgood:=ADR(HMI1.CB202_VLgood),IOCCmd:=ADR(HMI1.CB202_Cmd),MBCmd:=ADR(CB202_MODBUS.CMD),MBRst:=ADR(CB202_MODBUS.RST)),</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1080,39 +1081,43 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_208</v>
+        <f>CONCATENATE("HMI1.Flow_",B18)</f>
+        <v>HMI1.Flow_203</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB208_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B18,"_Closed")</f>
+        <v>HMI1.CB203_Closed</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB208_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B18,"_Vpu")</f>
+        <v>HMI1.CB203_Vpu</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB208_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B18,"_VLgood")</f>
+        <v>HMI1.CB203_VLgood</v>
+      </c>
+      <c r="H18" t="str">
+        <f>CONCATENATE("HMI1.CB",B18,"_Cmd")</f>
+        <v>HMI1.CB203_Cmd</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="2"/>
-        <v>CB208_MODBUS</v>
+        <f>CONCATENATE("CB", B18, "_MODBUS")</f>
+        <v>CB203_MODBUS</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C18="","",CONCATENATE("HMI1.BUS",C18,"_Stat"))</f>
         <v/>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H18="","",CONCATENATE(",IOCCmd:=ADR(",H18,"),MBCmd:=ADR(",I18,".CMD),MBRst:=ADR(",I18,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=17,CBID:=208,Flow:=ADR(HMI1.Flow_208),Status:=ADR(HMI1.CB208_Closed),Vpu:=ADR(HMI1.CB208_Vpu),VLgood:=ADR(HMI1.CB208_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A18,",CBID:=",B18,",Flow:=ADR(HMI1.Flow_",B18,"),Status:=ADR(",E18,"),Vpu:=ADR(",F18,"),VLgood:=ADR(",G18,")",K18,"),")</f>
+        <v>(ID:=17,CBID:=203,Flow:=ADR(HMI1.Flow_203),Status:=ADR(HMI1.CB203_Closed),Vpu:=ADR(HMI1.CB203_Vpu),VLgood:=ADR(HMI1.CB203_VLgood),IOCCmd:=ADR(HMI1.CB203_Cmd),MBCmd:=ADR(CB203_MODBUS.CMD),MBRst:=ADR(CB203_MODBUS.RST)),</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1120,39 +1125,39 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_209</v>
+        <f>CONCATENATE("HMI1.Flow_",B19)</f>
+        <v>HMI1.Flow_204</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB209_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B19,"_Closed")</f>
+        <v>HMI1.CB204_Closed</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB209_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B19,"_Vpu")</f>
+        <v>HMI1.CB204_Vpu</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB209_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B19,"_VLgood")</f>
+        <v>HMI1.CB204_VLgood</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="2"/>
-        <v>CB209_MODBUS</v>
+        <f>CONCATENATE("CB", B19, "_MODBUS")</f>
+        <v>CB204_MODBUS</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C19="","",CONCATENATE("HMI1.BUS",C19,"_Stat"))</f>
         <v/>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H19="","",CONCATENATE(",IOCCmd:=ADR(",H19,"),MBCmd:=ADR(",I19,".CMD),MBRst:=ADR(",I19,".RST)"))</f>
         <v/>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=18,CBID:=209,Flow:=ADR(HMI1.Flow_209),Status:=ADR(HMI1.CB209_Closed),Vpu:=ADR(HMI1.CB209_Vpu),VLgood:=ADR(HMI1.CB209_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A19,",CBID:=",B19,",Flow:=ADR(HMI1.Flow_",B19,"),Status:=ADR(",E19,"),Vpu:=ADR(",F19,"),VLgood:=ADR(",G19,")",K19,"),")</f>
+        <v>(ID:=18,CBID:=204,Flow:=ADR(HMI1.Flow_204),Status:=ADR(HMI1.CB204_Closed),Vpu:=ADR(HMI1.CB204_Vpu),VLgood:=ADR(HMI1.CB204_VLgood)),</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1160,39 +1165,39 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_210</v>
+        <f>CONCATENATE("HMI1.Flow_",B20)</f>
+        <v>HMI1.Flow_205</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB210_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B20,"_Closed")</f>
+        <v>HMI1.CB205_Closed</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB210_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B20,"_Vpu")</f>
+        <v>HMI1.CB205_Vpu</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB210_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B20,"_VLgood")</f>
+        <v>HMI1.CB205_VLgood</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="2"/>
-        <v>CB210_MODBUS</v>
+        <f>CONCATENATE("CB", B20, "_MODBUS")</f>
+        <v>CB205_MODBUS</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C20="","",CONCATENATE("HMI1.BUS",C20,"_Stat"))</f>
         <v/>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H20="","",CONCATENATE(",IOCCmd:=ADR(",H20,"),MBCmd:=ADR(",I20,".CMD),MBRst:=ADR(",I20,".RST)"))</f>
         <v/>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=19,CBID:=210,Flow:=ADR(HMI1.Flow_210),Status:=ADR(HMI1.CB210_Closed),Vpu:=ADR(HMI1.CB210_Vpu),VLgood:=ADR(HMI1.CB210_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A20,",CBID:=",B20,",Flow:=ADR(HMI1.Flow_",B20,"),Status:=ADR(",E20,"),Vpu:=ADR(",F20,"),VLgood:=ADR(",G20,")",K20,"),")</f>
+        <v>(ID:=19,CBID:=205,Flow:=ADR(HMI1.Flow_205),Status:=ADR(HMI1.CB205_Closed),Vpu:=ADR(HMI1.CB205_Vpu),VLgood:=ADR(HMI1.CB205_VLgood)),</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1200,39 +1205,39 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_211</v>
+        <f>CONCATENATE("HMI1.Flow_",B21)</f>
+        <v>HMI1.Flow_206</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB211_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B21,"_Closed")</f>
+        <v>HMI1.CB206_Closed</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB211_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B21,"_Vpu")</f>
+        <v>HMI1.CB206_Vpu</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB211_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B21,"_VLgood")</f>
+        <v>HMI1.CB206_VLgood</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="2"/>
-        <v>CB211_MODBUS</v>
+        <f>CONCATENATE("CB", B21, "_MODBUS")</f>
+        <v>CB206_MODBUS</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C21="","",CONCATENATE("HMI1.BUS",C21,"_Stat"))</f>
         <v/>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H21="","",CONCATENATE(",IOCCmd:=ADR(",H21,"),MBCmd:=ADR(",I21,".CMD),MBRst:=ADR(",I21,".RST)"))</f>
         <v/>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=20,CBID:=211,Flow:=ADR(HMI1.Flow_211),Status:=ADR(HMI1.CB211_Closed),Vpu:=ADR(HMI1.CB211_Vpu),VLgood:=ADR(HMI1.CB211_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A21,",CBID:=",B21,",Flow:=ADR(HMI1.Flow_",B21,"),Status:=ADR(",E21,"),Vpu:=ADR(",F21,"),VLgood:=ADR(",G21,")",K21,"),")</f>
+        <v>(ID:=20,CBID:=206,Flow:=ADR(HMI1.Flow_206),Status:=ADR(HMI1.CB206_Closed),Vpu:=ADR(HMI1.CB206_Vpu),VLgood:=ADR(HMI1.CB206_VLgood)),</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -1240,39 +1245,39 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_212</v>
+        <f>CONCATENATE("HMI1.Flow_",B22)</f>
+        <v>HMI1.Flow_207</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB212_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B22,"_Closed")</f>
+        <v>HMI1.CB207_Closed</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB212_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B22,"_Vpu")</f>
+        <v>HMI1.CB207_Vpu</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB212_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B22,"_VLgood")</f>
+        <v>HMI1.CB207_VLgood</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="2"/>
-        <v>CB212_MODBUS</v>
+        <f>CONCATENATE("CB", B22, "_MODBUS")</f>
+        <v>CB207_MODBUS</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C22="","",CONCATENATE("HMI1.BUS",C22,"_Stat"))</f>
         <v/>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H22="","",CONCATENATE(",IOCCmd:=ADR(",H22,"),MBCmd:=ADR(",I22,".CMD),MBRst:=ADR(",I22,".RST)"))</f>
         <v/>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=21,CBID:=212,Flow:=ADR(HMI1.Flow_212),Status:=ADR(HMI1.CB212_Closed),Vpu:=ADR(HMI1.CB212_Vpu),VLgood:=ADR(HMI1.CB212_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A22,",CBID:=",B22,",Flow:=ADR(HMI1.Flow_",B22,"),Status:=ADR(",E22,"),Vpu:=ADR(",F22,"),VLgood:=ADR(",G22,")",K22,"),")</f>
+        <v>(ID:=21,CBID:=207,Flow:=ADR(HMI1.Flow_207),Status:=ADR(HMI1.CB207_Closed),Vpu:=ADR(HMI1.CB207_Vpu),VLgood:=ADR(HMI1.CB207_VLgood)),</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1280,43 +1285,39 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_213</v>
+        <f>CONCATENATE("HMI1.Flow_",B23)</f>
+        <v>HMI1.Flow_208</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB213_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B23,"_Closed")</f>
+        <v>HMI1.CB208_Closed</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB213_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B23,"_Vpu")</f>
+        <v>HMI1.CB208_Vpu</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB213_VLgood</v>
-      </c>
-      <c r="H23" t="str">
-        <f>CONCATENATE("HMI1.CB",B23,"_Cmd")</f>
-        <v>HMI1.CB213_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B23,"_VLgood")</f>
+        <v>HMI1.CB208_VLgood</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="2"/>
-        <v>CB213_MODBUS</v>
+        <f>CONCATENATE("CB", B23, "_MODBUS")</f>
+        <v>CB208_MODBUS</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C23="","",CONCATENATE("HMI1.BUS",C23,"_Stat"))</f>
         <v/>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)</v>
+        <f>IF(H23="","",CONCATENATE(",IOCCmd:=ADR(",H23,"),MBCmd:=ADR(",I23,".CMD),MBRst:=ADR(",I23,".RST)"))</f>
+        <v/>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=22,CBID:=213,Flow:=ADR(HMI1.Flow_213),Status:=ADR(HMI1.CB213_Closed),Vpu:=ADR(HMI1.CB213_Vpu),VLgood:=ADR(HMI1.CB213_VLgood),IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)),</v>
+        <f>CONCATENATE("(ID:=",A23,",CBID:=",B23,",Flow:=ADR(HMI1.Flow_",B23,"),Status:=ADR(",E23,"),Vpu:=ADR(",F23,"),VLgood:=ADR(",G23,")",K23,"),")</f>
+        <v>(ID:=22,CBID:=208,Flow:=ADR(HMI1.Flow_208),Status:=ADR(HMI1.CB208_Closed),Vpu:=ADR(HMI1.CB208_Vpu),VLgood:=ADR(HMI1.CB208_VLgood)),</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -1324,39 +1325,39 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_214</v>
+        <f>CONCATENATE("HMI1.Flow_",B24)</f>
+        <v>HMI1.Flow_209</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB214_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B24,"_Closed")</f>
+        <v>HMI1.CB209_Closed</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB214_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B24,"_Vpu")</f>
+        <v>HMI1.CB209_Vpu</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB214_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B24,"_VLgood")</f>
+        <v>HMI1.CB209_VLgood</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="2"/>
-        <v>CB214_MODBUS</v>
+        <f>CONCATENATE("CB", B24, "_MODBUS")</f>
+        <v>CB209_MODBUS</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C24="","",CONCATENATE("HMI1.BUS",C24,"_Stat"))</f>
         <v/>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H24="","",CONCATENATE(",IOCCmd:=ADR(",H24,"),MBCmd:=ADR(",I24,".CMD),MBRst:=ADR(",I24,".RST)"))</f>
         <v/>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=23,CBID:=214,Flow:=ADR(HMI1.Flow_214),Status:=ADR(HMI1.CB214_Closed),Vpu:=ADR(HMI1.CB214_Vpu),VLgood:=ADR(HMI1.CB214_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A24,",CBID:=",B24,",Flow:=ADR(HMI1.Flow_",B24,"),Status:=ADR(",E24,"),Vpu:=ADR(",F24,"),VLgood:=ADR(",G24,")",K24,"),")</f>
+        <v>(ID:=23,CBID:=209,Flow:=ADR(HMI1.Flow_209),Status:=ADR(HMI1.CB209_Closed),Vpu:=ADR(HMI1.CB209_Vpu),VLgood:=ADR(HMI1.CB209_VLgood)),</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1364,39 +1365,39 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_215</v>
+        <f>CONCATENATE("HMI1.Flow_",B25)</f>
+        <v>HMI1.Flow_210</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB215_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B25,"_Closed")</f>
+        <v>HMI1.CB210_Closed</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB215_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B25,"_Vpu")</f>
+        <v>HMI1.CB210_Vpu</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB215_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B25,"_VLgood")</f>
+        <v>HMI1.CB210_VLgood</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="2"/>
-        <v>CB215_MODBUS</v>
+        <f>CONCATENATE("CB", B25, "_MODBUS")</f>
+        <v>CB210_MODBUS</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C25="","",CONCATENATE("HMI1.BUS",C25,"_Stat"))</f>
         <v/>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H25="","",CONCATENATE(",IOCCmd:=ADR(",H25,"),MBCmd:=ADR(",I25,".CMD),MBRst:=ADR(",I25,".RST)"))</f>
         <v/>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=24,CBID:=215,Flow:=ADR(HMI1.Flow_215),Status:=ADR(HMI1.CB215_Closed),Vpu:=ADR(HMI1.CB215_Vpu),VLgood:=ADR(HMI1.CB215_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A25,",CBID:=",B25,",Flow:=ADR(HMI1.Flow_",B25,"),Status:=ADR(",E25,"),Vpu:=ADR(",F25,"),VLgood:=ADR(",G25,")",K25,"),")</f>
+        <v>(ID:=24,CBID:=210,Flow:=ADR(HMI1.Flow_210),Status:=ADR(HMI1.CB210_Closed),Vpu:=ADR(HMI1.CB210_Vpu),VLgood:=ADR(HMI1.CB210_VLgood)),</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -1404,43 +1405,39 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_216</v>
+        <f>CONCATENATE("HMI1.Flow_",B26)</f>
+        <v>HMI1.Flow_211</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB216_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B26,"_Closed")</f>
+        <v>HMI1.CB211_Closed</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB216_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B26,"_Vpu")</f>
+        <v>HMI1.CB211_Vpu</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB216_VLgood</v>
-      </c>
-      <c r="H26" t="str">
-        <f>CONCATENATE("HMI1.CB",B26,"_Cmd")</f>
-        <v>HMI1.CB216_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B26,"_VLgood")</f>
+        <v>HMI1.CB211_VLgood</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="2"/>
-        <v>CB216_MODBUS</v>
+        <f>CONCATENATE("CB", B26, "_MODBUS")</f>
+        <v>CB211_MODBUS</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C26="","",CONCATENATE("HMI1.BUS",C26,"_Stat"))</f>
         <v/>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)</v>
+        <f>IF(H26="","",CONCATENATE(",IOCCmd:=ADR(",H26,"),MBCmd:=ADR(",I26,".CMD),MBRst:=ADR(",I26,".RST)"))</f>
+        <v/>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=25,CBID:=216,Flow:=ADR(HMI1.Flow_216),Status:=ADR(HMI1.CB216_Closed),Vpu:=ADR(HMI1.CB216_Vpu),VLgood:=ADR(HMI1.CB216_VLgood),IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)),</v>
+        <f>CONCATENATE("(ID:=",A26,",CBID:=",B26,",Flow:=ADR(HMI1.Flow_",B26,"),Status:=ADR(",E26,"),Vpu:=ADR(",F26,"),VLgood:=ADR(",G26,")",K26,"),")</f>
+        <v>(ID:=25,CBID:=211,Flow:=ADR(HMI1.Flow_211),Status:=ADR(HMI1.CB211_Closed),Vpu:=ADR(HMI1.CB211_Vpu),VLgood:=ADR(HMI1.CB211_VLgood)),</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -1448,43 +1445,39 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_217</v>
+        <f>CONCATENATE("HMI1.Flow_",B27)</f>
+        <v>HMI1.Flow_212</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB217_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B27,"_Closed")</f>
+        <v>HMI1.CB212_Closed</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB217_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B27,"_Vpu")</f>
+        <v>HMI1.CB212_Vpu</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB217_VLgood</v>
-      </c>
-      <c r="H27" t="str">
-        <f>CONCATENATE("HMI1.CB",B27,"_Cmd")</f>
-        <v>HMI1.CB217_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B27,"_VLgood")</f>
+        <v>HMI1.CB212_VLgood</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="2"/>
-        <v>CB217_MODBUS</v>
+        <f>CONCATENATE("CB", B27, "_MODBUS")</f>
+        <v>CB212_MODBUS</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C27="","",CONCATENATE("HMI1.BUS",C27,"_Stat"))</f>
         <v/>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)</v>
+        <f>IF(H27="","",CONCATENATE(",IOCCmd:=ADR(",H27,"),MBCmd:=ADR(",I27,".CMD),MBRst:=ADR(",I27,".RST)"))</f>
+        <v/>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=26,CBID:=217,Flow:=ADR(HMI1.Flow_217),Status:=ADR(HMI1.CB217_Closed),Vpu:=ADR(HMI1.CB217_Vpu),VLgood:=ADR(HMI1.CB217_VLgood),IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)),</v>
+        <f>CONCATENATE("(ID:=",A27,",CBID:=",B27,",Flow:=ADR(HMI1.Flow_",B27,"),Status:=ADR(",E27,"),Vpu:=ADR(",F27,"),VLgood:=ADR(",G27,")",K27,"),")</f>
+        <v>(ID:=26,CBID:=212,Flow:=ADR(HMI1.Flow_212),Status:=ADR(HMI1.CB212_Closed),Vpu:=ADR(HMI1.CB212_Vpu),VLgood:=ADR(HMI1.CB212_VLgood)),</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -1492,39 +1485,43 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_218</v>
+        <f>CONCATENATE("HMI1.Flow_",B28)</f>
+        <v>HMI1.Flow_213</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB218_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B28,"_Closed")</f>
+        <v>HMI1.CB213_Closed</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB218_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B28,"_Vpu")</f>
+        <v>HMI1.CB213_Vpu</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB218_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B28,"_VLgood")</f>
+        <v>HMI1.CB213_VLgood</v>
+      </c>
+      <c r="H28" t="str">
+        <f>CONCATENATE("HMI1.CB",B28,"_Cmd")</f>
+        <v>HMI1.CB213_Cmd</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" si="2"/>
-        <v>CB218_MODBUS</v>
+        <f>CONCATENATE("CB", B28, "_MODBUS")</f>
+        <v>CB213_MODBUS</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C28="","",CONCATENATE("HMI1.BUS",C28,"_Stat"))</f>
         <v/>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H28="","",CONCATENATE(",IOCCmd:=ADR(",H28,"),MBCmd:=ADR(",I28,".CMD),MBRst:=ADR(",I28,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=27,CBID:=218,Flow:=ADR(HMI1.Flow_218),Status:=ADR(HMI1.CB218_Closed),Vpu:=ADR(HMI1.CB218_Vpu),VLgood:=ADR(HMI1.CB218_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A28,",CBID:=",B28,",Flow:=ADR(HMI1.Flow_",B28,"),Status:=ADR(",E28,"),Vpu:=ADR(",F28,"),VLgood:=ADR(",G28,")",K28,"),")</f>
+        <v>(ID:=27,CBID:=213,Flow:=ADR(HMI1.Flow_213),Status:=ADR(HMI1.CB213_Closed),Vpu:=ADR(HMI1.CB213_Vpu),VLgood:=ADR(HMI1.CB213_VLgood),IOCCmd:=ADR(HMI1.CB213_Cmd),MBCmd:=ADR(CB213_MODBUS.CMD),MBRst:=ADR(CB213_MODBUS.RST)),</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -1532,39 +1529,39 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_219</v>
+        <f>CONCATENATE("HMI1.Flow_",B29)</f>
+        <v>HMI1.Flow_214</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB219_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B29,"_Closed")</f>
+        <v>HMI1.CB214_Closed</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB219_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B29,"_Vpu")</f>
+        <v>HMI1.CB214_Vpu</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB219_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B29,"_VLgood")</f>
+        <v>HMI1.CB214_VLgood</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" si="2"/>
-        <v>CB219_MODBUS</v>
+        <f>CONCATENATE("CB", B29, "_MODBUS")</f>
+        <v>CB214_MODBUS</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C29="","",CONCATENATE("HMI1.BUS",C29,"_Stat"))</f>
         <v/>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H29="","",CONCATENATE(",IOCCmd:=ADR(",H29,"),MBCmd:=ADR(",I29,".CMD),MBRst:=ADR(",I29,".RST)"))</f>
         <v/>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=28,CBID:=219,Flow:=ADR(HMI1.Flow_219),Status:=ADR(HMI1.CB219_Closed),Vpu:=ADR(HMI1.CB219_Vpu),VLgood:=ADR(HMI1.CB219_VLgood)),</v>
+        <f>CONCATENATE("(ID:=",A29,",CBID:=",B29,",Flow:=ADR(HMI1.Flow_",B29,"),Status:=ADR(",E29,"),Vpu:=ADR(",F29,"),VLgood:=ADR(",G29,")",K29,"),")</f>
+        <v>(ID:=28,CBID:=214,Flow:=ADR(HMI1.Flow_214),Status:=ADR(HMI1.CB214_Closed),Vpu:=ADR(HMI1.CB214_Vpu),VLgood:=ADR(HMI1.CB214_VLgood)),</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1572,43 +1569,39 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>101</v>
+        <v>215</v>
       </c>
       <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_101</v>
+        <f>CONCATENATE("HMI1.Flow_",B30)</f>
+        <v>HMI1.Flow_215</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB101_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B30,"_Closed")</f>
+        <v>HMI1.CB215_Closed</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB101_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B30,"_Vpu")</f>
+        <v>HMI1.CB215_Vpu</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB101_VLgood</v>
-      </c>
-      <c r="H30" t="str">
-        <f>CONCATENATE("HMI1.CB",B30,"_Cmd")</f>
-        <v>HMI1.CB101_Cmd</v>
+        <f>CONCATENATE("HMI1.CB",B30,"_VLgood")</f>
+        <v>HMI1.CB215_VLgood</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="2"/>
-        <v>CB101_MODBUS</v>
+        <f>CONCATENATE("CB", B30, "_MODBUS")</f>
+        <v>CB215_MODBUS</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C30="","",CONCATENATE("HMI1.BUS",C30,"_Stat"))</f>
         <v/>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)</v>
+        <f>IF(H30="","",CONCATENATE(",IOCCmd:=ADR(",H30,"),MBCmd:=ADR(",I30,".CMD),MBRst:=ADR(",I30,".RST)"))</f>
+        <v/>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=29,CBID:=101,Flow:=ADR(HMI1.Flow_101),Status:=ADR(HMI1.CB101_Closed),Vpu:=ADR(HMI1.CB101_Vpu),VLgood:=ADR(HMI1.CB101_VLgood),IOCCmd:=ADR(HMI1.CB101_Cmd),MBCmd:=ADR(CB101_MODBUS.CMD),MBRst:=ADR(CB101_MODBUS.RST)),</v>
+        <f>CONCATENATE("(ID:=",A30,",CBID:=",B30,",Flow:=ADR(HMI1.Flow_",B30,"),Status:=ADR(",E30,"),Vpu:=ADR(",F30,"),VLgood:=ADR(",G30,")",K30,"),")</f>
+        <v>(ID:=29,CBID:=215,Flow:=ADR(HMI1.Flow_215),Status:=ADR(HMI1.CB215_Closed),Vpu:=ADR(HMI1.CB215_Vpu),VLgood:=ADR(HMI1.CB215_VLgood)),</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1616,43 +1609,43 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>102</v>
+        <v>216</v>
       </c>
       <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_102</v>
+        <f>CONCATENATE("HMI1.Flow_",B31)</f>
+        <v>HMI1.Flow_216</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB102_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B31,"_Closed")</f>
+        <v>HMI1.CB216_Closed</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB102_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B31,"_Vpu")</f>
+        <v>HMI1.CB216_Vpu</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB102_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B31,"_VLgood")</f>
+        <v>HMI1.CB216_VLgood</v>
       </c>
       <c r="H31" t="str">
         <f>CONCATENATE("HMI1.CB",B31,"_Cmd")</f>
-        <v>HMI1.CB102_Cmd</v>
+        <v>HMI1.CB216_Cmd</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="2"/>
-        <v>CB102_MODBUS</v>
+        <f>CONCATENATE("CB", B31, "_MODBUS")</f>
+        <v>CB216_MODBUS</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C31="","",CONCATENATE("HMI1.BUS",C31,"_Stat"))</f>
         <v/>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)</v>
+        <f>IF(H31="","",CONCATENATE(",IOCCmd:=ADR(",H31,"),MBCmd:=ADR(",I31,".CMD),MBRst:=ADR(",I31,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=30,CBID:=102,Flow:=ADR(HMI1.Flow_102),Status:=ADR(HMI1.CB102_Closed),Vpu:=ADR(HMI1.CB102_Vpu),VLgood:=ADR(HMI1.CB102_VLgood),IOCCmd:=ADR(HMI1.CB102_Cmd),MBCmd:=ADR(CB102_MODBUS.CMD),MBRst:=ADR(CB102_MODBUS.RST)),</v>
+        <f>CONCATENATE("(ID:=",A31,",CBID:=",B31,",Flow:=ADR(HMI1.Flow_",B31,"),Status:=ADR(",E31,"),Vpu:=ADR(",F31,"),VLgood:=ADR(",G31,")",K31,"),")</f>
+        <v>(ID:=30,CBID:=216,Flow:=ADR(HMI1.Flow_216),Status:=ADR(HMI1.CB216_Closed),Vpu:=ADR(HMI1.CB216_Vpu),VLgood:=ADR(HMI1.CB216_VLgood),IOCCmd:=ADR(HMI1.CB216_Cmd),MBCmd:=ADR(CB216_MODBUS.CMD),MBRst:=ADR(CB216_MODBUS.RST)),</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -1660,235 +1653,246 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>103</v>
+        <v>217</v>
       </c>
       <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_103</v>
+        <f>CONCATENATE("HMI1.Flow_",B32)</f>
+        <v>HMI1.Flow_217</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB103_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B32,"_Closed")</f>
+        <v>HMI1.CB217_Closed</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB103_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B32,"_Vpu")</f>
+        <v>HMI1.CB217_Vpu</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB103_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B32,"_VLgood")</f>
+        <v>HMI1.CB217_VLgood</v>
       </c>
       <c r="H32" t="str">
         <f>CONCATENATE("HMI1.CB",B32,"_Cmd")</f>
-        <v>HMI1.CB103_Cmd</v>
+        <v>HMI1.CB217_Cmd</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="2"/>
-        <v>CB103_MODBUS</v>
+        <f>CONCATENATE("CB", B32, "_MODBUS")</f>
+        <v>CB217_MODBUS</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C32="","",CONCATENATE("HMI1.BUS",C32,"_Stat"))</f>
         <v/>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)</v>
+        <f>IF(H32="","",CONCATENATE(",IOCCmd:=ADR(",H32,"),MBCmd:=ADR(",I32,".CMD),MBRst:=ADR(",I32,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=31,CBID:=103,Flow:=ADR(HMI1.Flow_103),Status:=ADR(HMI1.CB103_Closed),Vpu:=ADR(HMI1.CB103_Vpu),VLgood:=ADR(HMI1.CB103_VLgood),IOCCmd:=ADR(HMI1.CB103_Cmd),MBCmd:=ADR(CB103_MODBUS.CMD),MBRst:=ADR(CB103_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A32,",CBID:=",B32,",Flow:=ADR(HMI1.Flow_",B32,"),Status:=ADR(",E32,"),Vpu:=ADR(",F32,"),VLgood:=ADR(",G32,")",K32,"),")</f>
+        <v>(ID:=31,CBID:=217,Flow:=ADR(HMI1.Flow_217),Status:=ADR(HMI1.CB217_Closed),Vpu:=ADR(HMI1.CB217_Vpu),VLgood:=ADR(HMI1.CB217_VLgood),IOCCmd:=ADR(HMI1.CB217_Cmd),MBCmd:=ADR(CB217_MODBUS.CMD),MBRst:=ADR(CB217_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <v>104</v>
+        <v>218</v>
       </c>
       <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>HMI1.Flow_104</v>
+        <f>CONCATENATE("HMI1.Flow_",B33)</f>
+        <v>HMI1.Flow_218</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>HMI1.CB104_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B33,"_Closed")</f>
+        <v>HMI1.CB218_Closed</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB104_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B33,"_Vpu")</f>
+        <v>HMI1.CB218_Vpu</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB104_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B33,"_VLgood")</f>
+        <v>HMI1.CB218_VLgood</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="2"/>
-        <v>CB104_MODBUS</v>
+        <f>CONCATENATE("CB", B33, "_MODBUS")</f>
+        <v>CB218_MODBUS</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C33="","",CONCATENATE("HMI1.BUS",C33,"_Stat"))</f>
         <v/>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H33="","",CONCATENATE(",IOCCmd:=ADR(",H33,"),MBCmd:=ADR(",I33,".CMD),MBRst:=ADR(",I33,".RST)"))</f>
         <v/>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=32,CBID:=104,Flow:=ADR(HMI1.Flow_104),Status:=ADR(HMI1.CB104_Closed),Vpu:=ADR(HMI1.CB104_Vpu),VLgood:=ADR(HMI1.CB104_VLgood)),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A33,",CBID:=",B33,",Flow:=ADR(HMI1.Flow_",B33,"),Status:=ADR(",E33,"),Vpu:=ADR(",F33,"),VLgood:=ADR(",G33,")",K33,"),")</f>
+        <v>(ID:=32,CBID:=218,Flow:=ADR(HMI1.Flow_218),Status:=ADR(HMI1.CB218_Closed),Vpu:=ADR(HMI1.CB218_Vpu),VLgood:=ADR(HMI1.CB218_VLgood)),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>105</v>
+        <v>219</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" ref="D34:D63" si="8">CONCATENATE("HMI1.Flow_",B34)</f>
-        <v>HMI1.Flow_105</v>
+        <f>CONCATENATE("HMI1.Flow_",B34)</f>
+        <v>HMI1.Flow_219</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E63" si="9">CONCATENATE("HMI1.CB",B34,"_Closed")</f>
-        <v>HMI1.CB105_Closed</v>
+        <f>CONCATENATE("HMI1.CB",B34,"_Closed")</f>
+        <v>HMI1.CB219_Closed</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB105_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B34,"_Vpu")</f>
+        <v>HMI1.CB219_Vpu</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB105_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B34,"_VLgood")</f>
+        <v>HMI1.CB219_VLgood</v>
       </c>
       <c r="I34" t="str">
-        <f t="shared" ref="I34:I63" si="10">CONCATENATE("CB", B34, "_MODBUS")</f>
-        <v>CB105_MODBUS</v>
+        <f>CONCATENATE("CB", B34, "_MODBUS")</f>
+        <v>CB219_MODBUS</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C34="","",CONCATENATE("HMI1.BUS",C34,"_Stat"))</f>
         <v/>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H34="","",CONCATENATE(",IOCCmd:=ADR(",H34,"),MBCmd:=ADR(",I34,".CMD),MBRst:=ADR(",I34,".RST)"))</f>
         <v/>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=33,CBID:=105,Flow:=ADR(HMI1.Flow_105),Status:=ADR(HMI1.CB105_Closed),Vpu:=ADR(HMI1.CB105_Vpu),VLgood:=ADR(HMI1.CB105_VLgood)),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <f>CONCATENATE("(ID:=",A34,",CBID:=",B34,",Flow:=ADR(HMI1.Flow_",B34,"),Status:=ADR(",E34,"),Vpu:=ADR(",F34,"),VLgood:=ADR(",G34,")",K34,"),")</f>
+        <v>(ID:=33,CBID:=219,Flow:=ADR(HMI1.Flow_219),Status:=ADR(HMI1.CB219_Closed),Vpu:=ADR(HMI1.CB219_Vpu),VLgood:=ADR(HMI1.CB219_VLgood)),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>106</v>
+        <v>301</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_106</v>
+        <f t="shared" ref="D35:D44" si="0">CONCATENATE("HMI1.Flow_",B35)</f>
+        <v>HMI1.Flow_301</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB106_Closed</v>
+        <f t="shared" ref="E35:E44" si="1">CONCATENATE("HMI1.CB",B35,"_Closed")</f>
+        <v>HMI1.CB301_Closed</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB106_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B35,"_Vpu")</f>
+        <v>HMI1.CB301_Vpu</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB106_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B35,"_VLgood")</f>
+        <v>HMI1.CB301_VLgood</v>
+      </c>
+      <c r="H35" t="str">
+        <f>CONCATENATE("HMI1.CB",B35,"_Cmd")</f>
+        <v>HMI1.CB301_Cmd</v>
       </c>
       <c r="I35" t="str">
-        <f t="shared" si="10"/>
-        <v>CB106_MODBUS</v>
+        <f t="shared" ref="I35:I44" si="2">CONCATENATE("CB", B35, "_MODBUS")</f>
+        <v>CB301_MODBUS</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J35:J55" si="3">IF(C35="","",CONCATENATE("HMI1.BUS",C35,"_Stat"))</f>
         <v/>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(H35="","",CONCATENATE(",IOCCmd:=ADR(",H35,"),MBCmd:=ADR(",I35,".CMD),MBRst:=ADR(",I35,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=34,CBID:=106,Flow:=ADR(HMI1.Flow_106),Status:=ADR(HMI1.CB106_Closed),Vpu:=ADR(HMI1.CB106_Vpu),VLgood:=ADR(HMI1.CB106_VLgood)),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="L35:L60" si="4">CONCATENATE("(ID:=",A35,",CBID:=",B35,",Flow:=ADR(HMI1.Flow_",B35,"),Status:=ADR(",E35,"),Vpu:=ADR(",F35,"),VLgood:=ADR(",G35,")",K35,"),")</f>
+        <v>(ID:=34,CBID:=301,Flow:=ADR(HMI1.Flow_301),Status:=ADR(HMI1.CB301_Closed),Vpu:=ADR(HMI1.CB301_Vpu),VLgood:=ADR(HMI1.CB301_VLgood),IOCCmd:=ADR(HMI1.CB301_Cmd),MBCmd:=ADR(CB301_MODBUS.CMD),MBRst:=ADR(CB301_MODBUS.RST)),</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <v>107</v>
+        <v>302</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_107</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_302</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB107_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB302_Closed</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB107_Vpu</v>
+        <f t="shared" ref="F36:F60" si="5">CONCATENATE("HMI1.CB",B36,"_Vpu")</f>
+        <v>HMI1.CB302_Vpu</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB107_VLgood</v>
+        <f t="shared" ref="G36:G60" si="6">CONCATENATE("HMI1.CB",B36,"_VLgood")</f>
+        <v>HMI1.CB302_VLgood</v>
+      </c>
+      <c r="H36" t="str">
+        <f>CONCATENATE("HMI1.CB",B36,"_Cmd")</f>
+        <v>HMI1.CB302_Cmd</v>
       </c>
       <c r="I36" t="str">
-        <f t="shared" si="10"/>
-        <v>CB107_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB302_MODBUS</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f t="shared" ref="K36:K60" si="7">IF(H36="","",CONCATENATE(",IOCCmd:=ADR(",H36,"),MBCmd:=ADR(",I36,".CMD),MBRst:=ADR(",I36,".RST)"))</f>
+        <v>,IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=35,CBID:=107,Flow:=ADR(HMI1.Flow_107),Status:=ADR(HMI1.CB107_Closed),Vpu:=ADR(HMI1.CB107_Vpu),VLgood:=ADR(HMI1.CB107_VLgood)),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=35,CBID:=302,Flow:=ADR(HMI1.Flow_302),Status:=ADR(HMI1.CB302_Closed),Vpu:=ADR(HMI1.CB302_Vpu),VLgood:=ADR(HMI1.CB302_VLgood),IOCCmd:=ADR(HMI1.CB302_Cmd),MBCmd:=ADR(CB302_MODBUS.CMD),MBRst:=ADR(CB302_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>108</v>
+        <v>303</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_108</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_303</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB108_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB303_Closed</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB108_Vpu</v>
+        <v>HMI1.CB303_Vpu</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB108_VLgood</v>
+        <v>HMI1.CB303_VLgood</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("HMI1.CB",B37,"_Cmd")</f>
-        <v>HMI1.CB108_Cmd</v>
+        <v>HMI1.CB303_Cmd</v>
       </c>
       <c r="I37" t="str">
-        <f t="shared" si="10"/>
-        <v>CB108_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB303_MODBUS</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="3"/>
@@ -1896,43 +1900,43 @@
       </c>
       <c r="K37" t="str">
         <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)</v>
+        <v>,IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=36,CBID:=108,Flow:=ADR(HMI1.Flow_108),Status:=ADR(HMI1.CB108_Closed),Vpu:=ADR(HMI1.CB108_Vpu),VLgood:=ADR(HMI1.CB108_VLgood),IOCCmd:=ADR(HMI1.CB108_Cmd),MBCmd:=ADR(CB108_MODBUS.CMD),MBRst:=ADR(CB108_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=36,CBID:=303,Flow:=ADR(HMI1.Flow_303),Status:=ADR(HMI1.CB303_Closed),Vpu:=ADR(HMI1.CB303_Vpu),VLgood:=ADR(HMI1.CB303_VLgood),IOCCmd:=ADR(HMI1.CB303_Cmd),MBCmd:=ADR(CB303_MODBUS.CMD),MBRst:=ADR(CB303_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>109</v>
+        <v>304</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_109</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_304</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB109_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB304_Closed</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB109_Vpu</v>
+        <v>HMI1.CB304_Vpu</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB109_VLgood</v>
+        <v>HMI1.CB304_VLgood</v>
       </c>
       <c r="H38" t="str">
         <f>CONCATENATE("HMI1.CB",B38,"_Cmd")</f>
-        <v>HMI1.CB109_Cmd</v>
+        <v>HMI1.CB304_Cmd</v>
       </c>
       <c r="I38" t="str">
-        <f t="shared" si="10"/>
-        <v>CB109_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB304_MODBUS</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
@@ -1940,39 +1944,43 @@
       </c>
       <c r="K38" t="str">
         <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)</v>
+        <v>,IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=37,CBID:=109,Flow:=ADR(HMI1.Flow_109),Status:=ADR(HMI1.CB109_Closed),Vpu:=ADR(HMI1.CB109_Vpu),VLgood:=ADR(HMI1.CB109_VLgood),IOCCmd:=ADR(HMI1.CB109_Cmd),MBCmd:=ADR(CB109_MODBUS.CMD),MBRst:=ADR(CB109_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=37,CBID:=304,Flow:=ADR(HMI1.Flow_304),Status:=ADR(HMI1.CB304_Closed),Vpu:=ADR(HMI1.CB304_Vpu),VLgood:=ADR(HMI1.CB304_VLgood),IOCCmd:=ADR(HMI1.CB304_Cmd),MBCmd:=ADR(CB304_MODBUS.CMD),MBRst:=ADR(CB304_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <v>110</v>
+        <v>305</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_110</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_305</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB110_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB305_Closed</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB110_Vpu</v>
+        <v>HMI1.CB305_Vpu</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB110_VLgood</v>
+        <v>HMI1.CB305_VLgood</v>
+      </c>
+      <c r="H39" t="str">
+        <f>CONCATENATE("HMI1.CB",B39,"_Cmd")</f>
+        <v>HMI1.CB305_Cmd</v>
       </c>
       <c r="I39" t="str">
-        <f t="shared" si="10"/>
-        <v>CB110_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB305_MODBUS</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="3"/>
@@ -1980,43 +1988,39 @@
       </c>
       <c r="K39" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>,IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=38,CBID:=110,Flow:=ADR(HMI1.Flow_110),Status:=ADR(HMI1.CB110_Closed),Vpu:=ADR(HMI1.CB110_Vpu),VLgood:=ADR(HMI1.CB110_VLgood)),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=38,CBID:=305,Flow:=ADR(HMI1.Flow_305),Status:=ADR(HMI1.CB305_Closed),Vpu:=ADR(HMI1.CB305_Vpu),VLgood:=ADR(HMI1.CB305_VLgood),IOCCmd:=ADR(HMI1.CB305_Cmd),MBCmd:=ADR(CB305_MODBUS.CMD),MBRst:=ADR(CB305_MODBUS.RST)),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <v>111</v>
+        <v>306</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_111</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_306</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB111_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB306_Closed</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB111_Vpu</v>
+        <v>HMI1.CB306_Vpu</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB111_VLgood</v>
-      </c>
-      <c r="H40" t="str">
-        <f>CONCATENATE("HMI1.CB",B40,"_Cmd")</f>
-        <v>HMI1.CB111_Cmd</v>
+        <v>HMI1.CB306_VLgood</v>
       </c>
       <c r="I40" t="str">
-        <f t="shared" si="10"/>
-        <v>CB111_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB306_MODBUS</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="3"/>
@@ -2024,39 +2028,39 @@
       </c>
       <c r="K40" t="str">
         <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)</v>
+        <v/>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=39,CBID:=111,Flow:=ADR(HMI1.Flow_111),Status:=ADR(HMI1.CB111_Closed),Vpu:=ADR(HMI1.CB111_Vpu),VLgood:=ADR(HMI1.CB111_VLgood),IOCCmd:=ADR(HMI1.CB111_Cmd),MBCmd:=ADR(CB111_MODBUS.CMD),MBRst:=ADR(CB111_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=39,CBID:=306,Flow:=ADR(HMI1.Flow_306),Status:=ADR(HMI1.CB306_Closed),Vpu:=ADR(HMI1.CB306_Vpu),VLgood:=ADR(HMI1.CB306_VLgood)),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>112</v>
+        <v>307</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_112</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_307</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB112_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB307_Closed</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB112_Vpu</v>
+        <v>HMI1.CB307_Vpu</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB112_VLgood</v>
+        <v>HMI1.CB307_VLgood</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" si="10"/>
-        <v>CB112_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB307_MODBUS</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="3"/>
@@ -2068,39 +2072,35 @@
       </c>
       <c r="L41" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=40,CBID:=112,Flow:=ADR(HMI1.Flow_112),Status:=ADR(HMI1.CB112_Closed),Vpu:=ADR(HMI1.CB112_Vpu),VLgood:=ADR(HMI1.CB112_VLgood)),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=40,CBID:=307,Flow:=ADR(HMI1.Flow_307),Status:=ADR(HMI1.CB307_Closed),Vpu:=ADR(HMI1.CB307_Vpu),VLgood:=ADR(HMI1.CB307_VLgood)),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
-        <v>113</v>
+        <v>308</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_113</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_308</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB113_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB308_Closed</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB113_Vpu</v>
+        <v>HMI1.CB308_Vpu</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB113_VLgood</v>
-      </c>
-      <c r="H42" t="str">
-        <f>CONCATENATE("HMI1.CB",B42,"_Cmd")</f>
-        <v>HMI1.CB113_Cmd</v>
+        <v>HMI1.CB308_VLgood</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="10"/>
-        <v>CB113_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB308_MODBUS</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="3"/>
@@ -2108,39 +2108,39 @@
       </c>
       <c r="K42" t="str">
         <f t="shared" si="7"/>
-        <v>,IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)</v>
+        <v/>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=41,CBID:=113,Flow:=ADR(HMI1.Flow_113),Status:=ADR(HMI1.CB113_Closed),Vpu:=ADR(HMI1.CB113_Vpu),VLgood:=ADR(HMI1.CB113_VLgood),IOCCmd:=ADR(HMI1.CB113_Cmd),MBCmd:=ADR(CB113_MODBUS.CMD),MBRst:=ADR(CB113_MODBUS.RST)),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=41,CBID:=308,Flow:=ADR(HMI1.Flow_308),Status:=ADR(HMI1.CB308_Closed),Vpu:=ADR(HMI1.CB308_Vpu),VLgood:=ADR(HMI1.CB308_VLgood)),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
-        <v>114</v>
+        <v>309</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_114</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_309</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB114_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB309_Closed</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB114_Vpu</v>
+        <v>HMI1.CB309_Vpu</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB114_VLgood</v>
+        <v>HMI1.CB309_VLgood</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="10"/>
-        <v>CB114_MODBUS</v>
+        <f t="shared" si="2"/>
+        <v>CB309_MODBUS</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="3"/>
@@ -2152,39 +2152,35 @@
       </c>
       <c r="L43" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=42,CBID:=114,Flow:=ADR(HMI1.Flow_114),Status:=ADR(HMI1.CB114_Closed),Vpu:=ADR(HMI1.CB114_Vpu),VLgood:=ADR(HMI1.CB114_VLgood)),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=42,CBID:=309,Flow:=ADR(HMI1.Flow_309),Status:=ADR(HMI1.CB309_Closed),Vpu:=ADR(HMI1.CB309_Vpu),VLgood:=ADR(HMI1.CB309_VLgood)),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_300</v>
+        <f t="shared" si="0"/>
+        <v>HMI1.Flow_310</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB300_Closed</v>
+        <f t="shared" si="1"/>
+        <v>HMI1.CB310_Closed</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB300_Vpu</v>
+        <v>HMI1.CB310_Vpu</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB300_VLgood</v>
+        <v>HMI1.CB310_VLgood</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="10"/>
-        <v>CB300_MODBUS</v>
-      </c>
-      <c r="J44" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>CB310_MODBUS</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="7"/>
@@ -2192,167 +2188,170 @@
       </c>
       <c r="L44" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=43,CBID:=300,Flow:=ADR(HMI1.Flow_300),Status:=ADR(HMI1.CB300_Closed),Vpu:=ADR(HMI1.CB300_Vpu),VLgood:=ADR(HMI1.CB300_VLgood)),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+        <v>(ID:=43,CBID:=310,Flow:=ADR(HMI1.Flow_310),Status:=ADR(HMI1.CB310_Closed),Vpu:=ADR(HMI1.CB310_Vpu),VLgood:=ADR(HMI1.CB310_VLgood)),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
-        <v>200</v>
+        <v>401</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_200</v>
+        <f t="shared" ref="D45:D50" si="8">CONCATENATE("HMI1.Flow_",B45)</f>
+        <v>HMI1.Flow_401</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB200_Closed</v>
+        <f t="shared" ref="E45:E50" si="9">CONCATENATE("HMI1.CB",B45,"_Closed")</f>
+        <v>HMI1.CB401_Closed</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB200_Vpu</v>
+        <f>CONCATENATE("HMI1.CB",B45,"_Vpu")</f>
+        <v>HMI1.CB401_Vpu</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB200_VLgood</v>
+        <f>CONCATENATE("HMI1.CB",B45,"_VLgood")</f>
+        <v>HMI1.CB401_VLgood</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="10"/>
-        <v>CB200_MODBUS</v>
+        <f t="shared" ref="I45:I50" si="10">CONCATENATE("CB", B45, "_MODBUS")</f>
+        <v>CB401_MODBUS</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J45:J50" si="11">IF(C45="","",CONCATENATE("HMI1.BUS",C45,"_Stat"))</f>
         <v/>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(H45="","",CONCATENATE(",IOCCmd:=ADR(",H45,"),MBCmd:=ADR(",I45,".CMD),MBRst:=ADR(",I45,".RST)"))</f>
         <v/>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=44,CBID:=200,Flow:=ADR(HMI1.Flow_200),Status:=ADR(HMI1.CB200_Closed),Vpu:=ADR(HMI1.CB200_Vpu),VLgood:=ADR(HMI1.CB200_VLgood)),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="L45:L50" si="12">CONCATENATE("(ID:=",A45,",CBID:=",B45,",Flow:=ADR(HMI1.Flow_",B45,"),Status:=ADR(",E45,"),Vpu:=ADR(",F45,"),VLgood:=ADR(",G45,")",K45,"),")</f>
+        <v>(ID:=44,CBID:=401,Flow:=ADR(HMI1.Flow_401),Status:=ADR(HMI1.CB401_Closed),Vpu:=ADR(HMI1.CB401_Vpu),VLgood:=ADR(HMI1.CB401_VLgood)),</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
-        <v>100</v>
+        <v>402</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="8"/>
-        <v>HMI1.Flow_100</v>
+        <v>HMI1.Flow_402</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="9"/>
-        <v>HMI1.CB100_Closed</v>
+        <v>HMI1.CB402_Closed</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB100_Vpu</v>
+        <f t="shared" ref="F46:F50" si="13">CONCATENATE("HMI1.CB",B46,"_Vpu")</f>
+        <v>HMI1.CB402_Vpu</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB100_VLgood</v>
+        <f t="shared" ref="G46:G50" si="14">CONCATENATE("HMI1.CB",B46,"_VLgood")</f>
+        <v>HMI1.CB402_VLgood</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="10"/>
-        <v>CB100_MODBUS</v>
+        <v>CB402_MODBUS</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K46:K50" si="15">IF(H46="","",CONCATENATE(",IOCCmd:=ADR(",H46,"),MBCmd:=ADR(",I46,".CMD),MBRst:=ADR(",I46,".RST)"))</f>
         <v/>
       </c>
       <c r="L46" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=45,CBID:=100,Flow:=ADR(HMI1.Flow_100),Status:=ADR(HMI1.CB100_Closed),Vpu:=ADR(HMI1.CB100_Vpu),VLgood:=ADR(HMI1.CB100_VLgood)),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="12"/>
+        <v>(ID:=45,CBID:=402,Flow:=ADR(HMI1.Flow_402),Status:=ADR(HMI1.CB402_Closed),Vpu:=ADR(HMI1.CB402_Vpu),VLgood:=ADR(HMI1.CB402_VLgood)),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
-        <v>351</v>
+        <v>403</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="8"/>
-        <v>HMI1.Flow_351</v>
+        <v>HMI1.Flow_403</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="9"/>
-        <v>HMI1.CB351_Closed</v>
+        <v>HMI1.CB403_Closed</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB351_Vpu</v>
+        <f t="shared" si="13"/>
+        <v>HMI1.CB403_Vpu</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB351_VLgood</v>
+        <f t="shared" si="14"/>
+        <v>HMI1.CB403_VLgood</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="10"/>
-        <v>CB351_MODBUS</v>
+        <v>CB403_MODBUS</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L47" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=46,CBID:=351,Flow:=ADR(HMI1.Flow_351),Status:=ADR(HMI1.CB351_Closed),Vpu:=ADR(HMI1.CB351_Vpu),VLgood:=ADR(HMI1.CB351_VLgood)),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="12"/>
+        <v>(ID:=46,CBID:=403,Flow:=ADR(HMI1.Flow_403),Status:=ADR(HMI1.CB403_Closed),Vpu:=ADR(HMI1.CB403_Vpu),VLgood:=ADR(HMI1.CB403_VLgood)),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
-        <v>151</v>
+        <v>404</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="8"/>
-        <v>HMI1.Flow_151</v>
+        <v>HMI1.Flow_404</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="9"/>
-        <v>HMI1.CB151_Closed</v>
+        <v>HMI1.CB404_Closed</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB151_Vpu</v>
+        <f t="shared" si="13"/>
+        <v>HMI1.CB404_Vpu</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB151_VLgood</v>
+        <f t="shared" si="14"/>
+        <v>HMI1.CB404_VLgood</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="10"/>
-        <v>CB151_MODBUS</v>
+        <v>CB404_MODBUS</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L48" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=47,CBID:=151,Flow:=ADR(HMI1.Flow_151),Status:=ADR(HMI1.CB151_Closed),Vpu:=ADR(HMI1.CB151_Vpu),VLgood:=ADR(HMI1.CB151_VLgood)),</v>
+        <f t="shared" si="12"/>
+        <v>(ID:=47,CBID:=404,Flow:=ADR(HMI1.Flow_404),Status:=ADR(HMI1.CB404_Closed),Vpu:=ADR(HMI1.CB404_Vpu),VLgood:=ADR(HMI1.CB404_VLgood)),</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -2360,35 +2359,39 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>261</v>
+        <v>405</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="8"/>
-        <v>HMI1.Flow_261</v>
+        <v>HMI1.Flow_405</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="9"/>
-        <v>HMI1.CB261_Closed</v>
+        <v>HMI1.CB405_Closed</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB261_Vpu</v>
+        <f t="shared" si="13"/>
+        <v>HMI1.CB405_Vpu</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB261_VLgood</v>
+        <f t="shared" si="14"/>
+        <v>HMI1.CB405_VLgood</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="10"/>
-        <v>CB261_MODBUS</v>
+        <v>CB405_MODBUS</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L49" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=48,CBID:=261,Flow:=ADR(HMI1.Flow_261),Status:=ADR(HMI1.CB261_Closed),Vpu:=ADR(HMI1.CB261_Vpu),VLgood:=ADR(HMI1.CB261_VLgood)),</v>
+        <f t="shared" si="12"/>
+        <v>(ID:=48,CBID:=405,Flow:=ADR(HMI1.Flow_405),Status:=ADR(HMI1.CB405_Closed),Vpu:=ADR(HMI1.CB405_Vpu),VLgood:=ADR(HMI1.CB405_VLgood)),</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -2396,35 +2399,39 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>271</v>
+        <v>406</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="8"/>
-        <v>HMI1.Flow_271</v>
+        <v>HMI1.Flow_406</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="9"/>
-        <v>HMI1.CB271_Closed</v>
+        <v>HMI1.CB406_Closed</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB271_Vpu</v>
+        <f t="shared" si="13"/>
+        <v>HMI1.CB406_Vpu</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB271_VLgood</v>
+        <f t="shared" si="14"/>
+        <v>HMI1.CB406_VLgood</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="10"/>
-        <v>CB271_MODBUS</v>
+        <v>CB406_MODBUS</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L50" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=49,CBID:=271,Flow:=ADR(HMI1.Flow_271),Status:=ADR(HMI1.CB271_Closed),Vpu:=ADR(HMI1.CB271_Vpu),VLgood:=ADR(HMI1.CB271_VLgood)),</v>
+        <f t="shared" si="12"/>
+        <v>(ID:=49,CBID:=406,Flow:=ADR(HMI1.Flow_406),Status:=ADR(HMI1.CB406_Closed),Vpu:=ADR(HMI1.CB406_Vpu),VLgood:=ADR(HMI1.CB406_VLgood)),</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -2432,39 +2439,39 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>401</v>
+        <v>100</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_401</v>
+        <f t="shared" ref="D51:D60" si="16">CONCATENATE("HMI1.Flow_",B51)</f>
+        <v>HMI1.Flow_100</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB401_Closed</v>
+        <f t="shared" ref="E51:E60" si="17">CONCATENATE("HMI1.CB",B51,"_Closed")</f>
+        <v>HMI1.CB100_Closed</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB401_Vpu</v>
+        <v>HMI1.CB100_Vpu</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB401_VLgood</v>
+        <v>HMI1.CB100_VLgood</v>
       </c>
       <c r="I51" t="str">
-        <f t="shared" si="10"/>
-        <v>CB401_MODBUS</v>
+        <f t="shared" ref="I51:I60" si="18">CONCATENATE("CB", B51, "_MODBUS")</f>
+        <v>CB100_MODBUS</v>
       </c>
       <c r="J51" t="str">
-        <f>IF(C51="","",CONCATENATE("HMI1.BUS",C51,"_Stat"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K51" t="str">
-        <f t="shared" ref="K51:K57" si="11">IF(H51="","",CONCATENATE(",IOCCmd:=ADR(",H51,"),MBCmd:=ADR(",I51,".CMD),MBRst:=ADR(",I51,".RST)"))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=50,CBID:=401,Flow:=ADR(HMI1.Flow_401),Status:=ADR(HMI1.CB401_Closed),Vpu:=ADR(HMI1.CB401_Vpu),VLgood:=ADR(HMI1.CB401_VLgood)),</v>
+        <v>(ID:=50,CBID:=100,Flow:=ADR(HMI1.Flow_100),Status:=ADR(HMI1.CB100_Closed),Vpu:=ADR(HMI1.CB100_Vpu),VLgood:=ADR(HMI1.CB100_VLgood)),</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -2472,39 +2479,39 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>402</v>
+        <v>200</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_402</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_200</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB402_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB200_Closed</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB402_Vpu</v>
+        <v>HMI1.CB200_Vpu</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB402_VLgood</v>
+        <v>HMI1.CB200_VLgood</v>
       </c>
       <c r="I52" t="str">
-        <f t="shared" si="10"/>
-        <v>CB402_MODBUS</v>
+        <f t="shared" si="18"/>
+        <v>CB200_MODBUS</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" ref="J52:J63" si="12">IF(C52="","",CONCATENATE("HMI1.BUS",C52,"_Stat"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=51,CBID:=402,Flow:=ADR(HMI1.Flow_402),Status:=ADR(HMI1.CB402_Closed),Vpu:=ADR(HMI1.CB402_Vpu),VLgood:=ADR(HMI1.CB402_VLgood)),</v>
+        <v>(ID:=51,CBID:=200,Flow:=ADR(HMI1.Flow_200),Status:=ADR(HMI1.CB200_Closed),Vpu:=ADR(HMI1.CB200_Vpu),VLgood:=ADR(HMI1.CB200_VLgood)),</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -2512,39 +2519,39 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>403</v>
+        <v>300</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_403</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_300</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB403_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB300_Closed</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB403_Vpu</v>
+        <v>HMI1.CB300_Vpu</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB403_VLgood</v>
+        <v>HMI1.CB300_VLgood</v>
       </c>
       <c r="I53" t="str">
-        <f t="shared" si="10"/>
-        <v>CB403_MODBUS</v>
+        <f t="shared" si="18"/>
+        <v>CB300_MODBUS</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L53" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=52,CBID:=403,Flow:=ADR(HMI1.Flow_403),Status:=ADR(HMI1.CB403_Closed),Vpu:=ADR(HMI1.CB403_Vpu),VLgood:=ADR(HMI1.CB403_VLgood)),</v>
+        <v>(ID:=52,CBID:=300,Flow:=ADR(HMI1.Flow_300),Status:=ADR(HMI1.CB300_Closed),Vpu:=ADR(HMI1.CB300_Vpu),VLgood:=ADR(HMI1.CB300_VLgood)),</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -2552,39 +2559,39 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>404</v>
+        <v>151</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_404</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_151</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB404_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB151_Closed</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB404_Vpu</v>
+        <v>HMI1.CB151_Vpu</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB404_VLgood</v>
+        <v>HMI1.CB151_VLgood</v>
       </c>
       <c r="I54" t="str">
-        <f t="shared" si="10"/>
-        <v>CB404_MODBUS</v>
+        <f t="shared" si="18"/>
+        <v>CB151_MODBUS</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L54" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=53,CBID:=404,Flow:=ADR(HMI1.Flow_404),Status:=ADR(HMI1.CB404_Closed),Vpu:=ADR(HMI1.CB404_Vpu),VLgood:=ADR(HMI1.CB404_VLgood)),</v>
+        <v>(ID:=53,CBID:=151,Flow:=ADR(HMI1.Flow_151),Status:=ADR(HMI1.CB151_Closed),Vpu:=ADR(HMI1.CB151_Vpu),VLgood:=ADR(HMI1.CB151_VLgood)),</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -2592,39 +2599,39 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>405</v>
+        <v>251</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_405</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_251</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB405_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB251_Closed</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB405_Vpu</v>
+        <v>HMI1.CB251_Vpu</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB405_VLgood</v>
+        <v>HMI1.CB251_VLgood</v>
       </c>
       <c r="I55" t="str">
-        <f t="shared" si="10"/>
-        <v>CB405_MODBUS</v>
+        <f t="shared" si="18"/>
+        <v>CB251_MODBUS</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=54,CBID:=405,Flow:=ADR(HMI1.Flow_405),Status:=ADR(HMI1.CB405_Closed),Vpu:=ADR(HMI1.CB405_Vpu),VLgood:=ADR(HMI1.CB405_VLgood)),</v>
+        <v>(ID:=54,CBID:=251,Flow:=ADR(HMI1.Flow_251),Status:=ADR(HMI1.CB251_Closed),Vpu:=ADR(HMI1.CB251_Vpu),VLgood:=ADR(HMI1.CB251_VLgood)),</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -2632,39 +2639,35 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>406</v>
+        <v>252</v>
       </c>
       <c r="D56" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_406</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_252</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB406_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB252_Closed</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB406_Vpu</v>
+        <v>HMI1.CB252_Vpu</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB406_VLgood</v>
+        <v>HMI1.CB252_VLgood</v>
       </c>
       <c r="I56" t="str">
-        <f t="shared" si="10"/>
-        <v>CB406_MODBUS</v>
-      </c>
-      <c r="J56" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>CB252_MODBUS</v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=55,CBID:=406,Flow:=ADR(HMI1.Flow_406),Status:=ADR(HMI1.CB406_Closed),Vpu:=ADR(HMI1.CB406_Vpu),VLgood:=ADR(HMI1.CB406_VLgood)),</v>
+        <v>(ID:=55,CBID:=252,Flow:=ADR(HMI1.Flow_252),Status:=ADR(HMI1.CB252_Closed),Vpu:=ADR(HMI1.CB252_Vpu),VLgood:=ADR(HMI1.CB252_VLgood)),</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -2672,39 +2675,35 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>407</v>
+        <v>351</v>
       </c>
       <c r="D57" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_407</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_351</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB407_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB351_Closed</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB407_Vpu</v>
+        <v>HMI1.CB351_Vpu</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB407_VLgood</v>
+        <v>HMI1.CB351_VLgood</v>
       </c>
       <c r="I57" t="str">
-        <f t="shared" si="10"/>
-        <v>CB407_MODBUS</v>
-      </c>
-      <c r="J57" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>CB351_MODBUS</v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=56,CBID:=407,Flow:=ADR(HMI1.Flow_407),Status:=ADR(HMI1.CB407_Closed),Vpu:=ADR(HMI1.CB407_Vpu),VLgood:=ADR(HMI1.CB407_VLgood)),</v>
+        <v>(ID:=56,CBID:=351,Flow:=ADR(HMI1.Flow_351),Status:=ADR(HMI1.CB351_Closed),Vpu:=ADR(HMI1.CB351_Vpu),VLgood:=ADR(HMI1.CB351_VLgood)),</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -2712,39 +2711,35 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>408</v>
+        <v>451</v>
       </c>
       <c r="D58" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_408</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_451</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB408_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB451_Closed</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB408_Vpu</v>
+        <v>HMI1.CB451_Vpu</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB408_VLgood</v>
+        <v>HMI1.CB451_VLgood</v>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="10"/>
-        <v>CB408_MODBUS</v>
-      </c>
-      <c r="J58" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>CB451_MODBUS</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" ref="K58:K63" si="13">IF(H58="","",CONCATENATE(",IOCCmd:=ADR(",H58,"),MBCmd:=ADR(",I58,".CMD),MBRst:=ADR(",I58,".RST)"))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=57,CBID:=408,Flow:=ADR(HMI1.Flow_408),Status:=ADR(HMI1.CB408_Closed),Vpu:=ADR(HMI1.CB408_Vpu),VLgood:=ADR(HMI1.CB408_VLgood)),</v>
+        <v>(ID:=57,CBID:=451,Flow:=ADR(HMI1.Flow_451),Status:=ADR(HMI1.CB451_Closed),Vpu:=ADR(HMI1.CB451_Vpu),VLgood:=ADR(HMI1.CB451_VLgood)),</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -2752,39 +2747,35 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>409</v>
+        <v>452</v>
       </c>
       <c r="D59" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_409</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_452</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB409_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB452_Closed</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB409_Vpu</v>
+        <v>HMI1.CB452_Vpu</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB409_VLgood</v>
+        <v>HMI1.CB452_VLgood</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="10"/>
-        <v>CB409_MODBUS</v>
-      </c>
-      <c r="J59" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>CB452_MODBUS</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L59" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=58,CBID:=409,Flow:=ADR(HMI1.Flow_409),Status:=ADR(HMI1.CB409_Closed),Vpu:=ADR(HMI1.CB409_Vpu),VLgood:=ADR(HMI1.CB409_VLgood)),</v>
+        <v>(ID:=58,CBID:=452,Flow:=ADR(HMI1.Flow_452),Status:=ADR(HMI1.CB452_Closed),Vpu:=ADR(HMI1.CB452_Vpu),VLgood:=ADR(HMI1.CB452_VLgood)),</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -2792,159 +2783,35 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>410</v>
+        <v>453</v>
       </c>
       <c r="D60" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_410</v>
+        <f t="shared" si="16"/>
+        <v>HMI1.Flow_453</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB410_Closed</v>
+        <f t="shared" si="17"/>
+        <v>HMI1.CB453_Closed</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="5"/>
-        <v>HMI1.CB410_Vpu</v>
+        <v>HMI1.CB453_Vpu</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="6"/>
-        <v>HMI1.CB410_VLgood</v>
+        <v>HMI1.CB453_VLgood</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="10"/>
-        <v>CB410_MODBUS</v>
-      </c>
-      <c r="J60" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>CB453_MODBUS</v>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="4"/>
-        <v>(ID:=59,CBID:=410,Flow:=ADR(HMI1.Flow_410),Status:=ADR(HMI1.CB410_Closed),Vpu:=ADR(HMI1.CB410_Vpu),VLgood:=ADR(HMI1.CB410_VLgood)),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>411</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_411</v>
-      </c>
-      <c r="E61" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB411_Closed</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB411_Vpu</v>
-      </c>
-      <c r="G61" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB411_VLgood</v>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" si="10"/>
-        <v>CB411_MODBUS</v>
-      </c>
-      <c r="J61" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="K61" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="L61" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=60,CBID:=411,Flow:=ADR(HMI1.Flow_411),Status:=ADR(HMI1.CB411_Closed),Vpu:=ADR(HMI1.CB411_Vpu),VLgood:=ADR(HMI1.CB411_VLgood)),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>412</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_412</v>
-      </c>
-      <c r="E62" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB412_Closed</v>
-      </c>
-      <c r="F62" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB412_Vpu</v>
-      </c>
-      <c r="G62" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB412_VLgood</v>
-      </c>
-      <c r="I62" t="str">
-        <f t="shared" si="10"/>
-        <v>CB412_MODBUS</v>
-      </c>
-      <c r="J62" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="K62" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="L62" t="str">
-        <f t="shared" si="4"/>
-        <v>(ID:=61,CBID:=412,Flow:=ADR(HMI1.Flow_412),Status:=ADR(HMI1.CB412_Closed),Vpu:=ADR(HMI1.CB412_Vpu),VLgood:=ADR(HMI1.CB412_VLgood)),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>413</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="8"/>
-        <v>HMI1.Flow_413</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="9"/>
-        <v>HMI1.CB413_Closed</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="5"/>
-        <v>HMI1.CB413_Vpu</v>
-      </c>
-      <c r="G63" t="str">
-        <f t="shared" si="6"/>
-        <v>HMI1.CB413_VLgood</v>
-      </c>
-      <c r="I63" t="str">
-        <f t="shared" si="10"/>
-        <v>CB413_MODBUS</v>
-      </c>
-      <c r="J63" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="K63" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="L63" t="str">
-        <f>CONCATENATE("(ID:=",A63,",CBID:=",B63,",Flow:=ADR(HMI1.Flow_",B63,"),Status:=ADR(",E63,"),Vpu:=ADR(",F63,"),VLgood:=ADR(",G63,")",K63,"),")</f>
-        <v>(ID:=62,CBID:=413,Flow:=ADR(HMI1.Flow_413),Status:=ADR(HMI1.CB413_Closed),Vpu:=ADR(HMI1.CB413_Vpu),VLgood:=ADR(HMI1.CB413_VLgood)),</v>
+        <v>(ID:=59,CBID:=453,Flow:=ADR(HMI1.Flow_453),Status:=ADR(HMI1.CB453_Closed),Vpu:=ADR(HMI1.CB453_Vpu),VLgood:=ADR(HMI1.CB453_VLgood)),</v>
       </c>
     </row>
   </sheetData>
@@ -2978,7 +2845,7 @@
       </c>
       <c r="C2" t="str">
         <f>INDEX(HMI_signals!H:H,B2+1)</f>
-        <v>HMI1.CB301_Cmd</v>
+        <v>HMI1.CB101_Cmd</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2991,7 +2858,7 @@
       </c>
       <c r="C3" t="str">
         <f>INDEX(HMI_signals!H:H,B3+1)</f>
-        <v>HMI1.CB301_Cmd</v>
+        <v>HMI1.CB101_Cmd</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3004,7 +2871,7 @@
       </c>
       <c r="C4" t="str">
         <f>INDEX(HMI_signals!H:H,B4+1)</f>
-        <v>HMI1.CB301_Cmd</v>
+        <v>HMI1.CB101_Cmd</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3017,7 +2884,7 @@
       </c>
       <c r="C5" t="str">
         <f>INDEX(HMI_signals!H:H,B5+1)</f>
-        <v>HMI1.CB301_Cmd</v>
+        <v>HMI1.CB101_Cmd</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3030,7 +2897,7 @@
       </c>
       <c r="C6" t="str">
         <f>INDEX(HMI_signals!H:H,B6+1)</f>
-        <v>HMI1.CB302_Cmd</v>
+        <v>HMI1.CB102_Cmd</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3043,7 +2910,7 @@
       </c>
       <c r="C7" t="str">
         <f>INDEX(HMI_signals!H:H,B7+1)</f>
-        <v>HMI1.CB302_Cmd</v>
+        <v>HMI1.CB102_Cmd</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3056,7 +2923,7 @@
       </c>
       <c r="C8" t="str">
         <f>INDEX(HMI_signals!H:H,B8+1)</f>
-        <v>HMI1.CB302_Cmd</v>
+        <v>HMI1.CB102_Cmd</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -3069,7 +2936,7 @@
       </c>
       <c r="C9" t="str">
         <f>INDEX(HMI_signals!H:H,B9+1)</f>
-        <v>HMI1.CB302_Cmd</v>
+        <v>HMI1.CB102_Cmd</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -3082,7 +2949,7 @@
       </c>
       <c r="C10" t="str">
         <f>INDEX(HMI_signals!H:H,B10+1)</f>
-        <v>HMI1.CB303_Cmd</v>
+        <v>HMI1.CB103_Cmd</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -3095,7 +2962,7 @@
       </c>
       <c r="C11" t="str">
         <f>INDEX(HMI_signals!H:H,B11+1)</f>
-        <v>HMI1.CB303_Cmd</v>
+        <v>HMI1.CB103_Cmd</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -3108,7 +2975,7 @@
       </c>
       <c r="C12" t="str">
         <f>INDEX(HMI_signals!H:H,B12+1)</f>
-        <v>HMI1.CB303_Cmd</v>
+        <v>HMI1.CB103_Cmd</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -3121,7 +2988,7 @@
       </c>
       <c r="C13" t="str">
         <f>INDEX(HMI_signals!H:H,B13+1)</f>
-        <v>HMI1.CB303_Cmd</v>
+        <v>HMI1.CB103_Cmd</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -3132,9 +2999,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14">
         <f>INDEX(HMI_signals!H:H,B14+1)</f>
-        <v>HMI1.CB304_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -3145,9 +3012,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15">
         <f>INDEX(HMI_signals!H:H,B15+1)</f>
-        <v>HMI1.CB304_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -3158,9 +3025,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16">
         <f>INDEX(HMI_signals!H:H,B16+1)</f>
-        <v>HMI1.CB304_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3171,9 +3038,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17">
         <f>INDEX(HMI_signals!H:H,B17+1)</f>
-        <v>HMI1.CB304_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -3184,9 +3051,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18">
         <f>INDEX(HMI_signals!H:H,B18+1)</f>
-        <v>HMI1.CB305_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3197,9 +3064,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19">
         <f>INDEX(HMI_signals!H:H,B19+1)</f>
-        <v>HMI1.CB305_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3210,9 +3077,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20">
         <f>INDEX(HMI_signals!H:H,B20+1)</f>
-        <v>HMI1.CB305_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3223,9 +3090,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21">
         <f>INDEX(HMI_signals!H:H,B21+1)</f>
-        <v>HMI1.CB305_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3340,9 +3207,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="str">
         <f>INDEX(HMI_signals!H:H,B30+1)</f>
-        <v>0</v>
+        <v>HMI1.CB108_Cmd</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -3353,9 +3220,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="str">
         <f>INDEX(HMI_signals!H:H,B31+1)</f>
-        <v>0</v>
+        <v>HMI1.CB108_Cmd</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -3366,9 +3233,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="str">
         <f>INDEX(HMI_signals!H:H,B32+1)</f>
-        <v>0</v>
+        <v>HMI1.CB108_Cmd</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -3379,9 +3246,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="str">
         <f>INDEX(HMI_signals!H:H,B33+1)</f>
-        <v>0</v>
+        <v>HMI1.CB108_Cmd</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -3392,9 +3259,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="str">
         <f>INDEX(HMI_signals!H:H,B34+1)</f>
-        <v>0</v>
+        <v>HMI1.CB109_Cmd</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -3405,9 +3272,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="str">
         <f>INDEX(HMI_signals!H:H,B35+1)</f>
-        <v>0</v>
+        <v>HMI1.CB109_Cmd</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -3418,9 +3285,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="str">
         <f>INDEX(HMI_signals!H:H,B36+1)</f>
-        <v>0</v>
+        <v>HMI1.CB109_Cmd</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -3431,9 +3298,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="str">
         <f>INDEX(HMI_signals!H:H,B37+1)</f>
-        <v>0</v>
+        <v>HMI1.CB109_Cmd</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -3444,9 +3311,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C38">
         <f>INDEX(HMI_signals!H:H,B38+1)</f>
-        <v>HMI1.CB201_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -3457,9 +3324,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39">
         <f>INDEX(HMI_signals!H:H,B39+1)</f>
-        <v>HMI1.CB201_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -3470,9 +3337,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C40">
         <f>INDEX(HMI_signals!H:H,B40+1)</f>
-        <v>HMI1.CB201_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -3483,9 +3350,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41">
         <f>INDEX(HMI_signals!H:H,B41+1)</f>
-        <v>HMI1.CB201_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -3498,7 +3365,7 @@
       </c>
       <c r="C42" t="str">
         <f>INDEX(HMI_signals!H:H,B42+1)</f>
-        <v>HMI1.CB202_Cmd</v>
+        <v>HMI1.CB111_Cmd</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -3511,7 +3378,7 @@
       </c>
       <c r="C43" t="str">
         <f>INDEX(HMI_signals!H:H,B43+1)</f>
-        <v>HMI1.CB202_Cmd</v>
+        <v>HMI1.CB111_Cmd</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -3524,7 +3391,7 @@
       </c>
       <c r="C44" t="str">
         <f>INDEX(HMI_signals!H:H,B44+1)</f>
-        <v>HMI1.CB202_Cmd</v>
+        <v>HMI1.CB111_Cmd</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -3537,7 +3404,7 @@
       </c>
       <c r="C45" t="str">
         <f>INDEX(HMI_signals!H:H,B45+1)</f>
-        <v>HMI1.CB202_Cmd</v>
+        <v>HMI1.CB111_Cmd</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -3548,9 +3415,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C46">
         <f>INDEX(HMI_signals!H:H,B46+1)</f>
-        <v>HMI1.CB203_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -3561,9 +3428,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47">
         <f>INDEX(HMI_signals!H:H,B47+1)</f>
-        <v>HMI1.CB203_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -3574,9 +3441,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C48">
         <f>INDEX(HMI_signals!H:H,B48+1)</f>
-        <v>HMI1.CB203_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -3587,9 +3454,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49">
         <f>INDEX(HMI_signals!H:H,B49+1)</f>
-        <v>HMI1.CB203_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -3600,9 +3467,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="str">
         <f>INDEX(HMI_signals!H:H,B50+1)</f>
-        <v>0</v>
+        <v>HMI1.CB113_Cmd</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -3613,9 +3480,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="str">
         <f>INDEX(HMI_signals!H:H,B51+1)</f>
-        <v>0</v>
+        <v>HMI1.CB113_Cmd</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -3626,9 +3493,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="str">
         <f>INDEX(HMI_signals!H:H,B52+1)</f>
-        <v>0</v>
+        <v>HMI1.CB113_Cmd</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -3639,9 +3506,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="str">
         <f>INDEX(HMI_signals!H:H,B53+1)</f>
-        <v>0</v>
+        <v>HMI1.CB113_Cmd</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -3704,9 +3571,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="str">
         <f>INDEX(HMI_signals!H:H,B58+1)</f>
-        <v>0</v>
+        <v>HMI1.CB201_Cmd</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -3717,9 +3584,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="str">
         <f>INDEX(HMI_signals!H:H,B59+1)</f>
-        <v>0</v>
+        <v>HMI1.CB201_Cmd</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -3730,9 +3597,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="str">
         <f>INDEX(HMI_signals!H:H,B60+1)</f>
-        <v>0</v>
+        <v>HMI1.CB201_Cmd</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -3743,9 +3610,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="str">
         <f>INDEX(HMI_signals!H:H,B61+1)</f>
-        <v>0</v>
+        <v>HMI1.CB201_Cmd</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -3756,9 +3623,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="str">
         <f>INDEX(HMI_signals!H:H,B62+1)</f>
-        <v>0</v>
+        <v>HMI1.CB202_Cmd</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -3769,9 +3636,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="str">
         <f>INDEX(HMI_signals!H:H,B63+1)</f>
-        <v>0</v>
+        <v>HMI1.CB202_Cmd</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -3782,9 +3649,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C64">
+      <c r="C64" t="str">
         <f>INDEX(HMI_signals!H:H,B64+1)</f>
-        <v>0</v>
+        <v>HMI1.CB202_Cmd</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -3795,9 +3662,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C65">
+      <c r="C65" t="str">
         <f>INDEX(HMI_signals!H:H,B65+1)</f>
-        <v>0</v>
+        <v>HMI1.CB202_Cmd</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -3808,9 +3675,9 @@
         <f t="shared" ref="B66:B129" si="1">CEILING(A66/4,1)</f>
         <v>17</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="str">
         <f>INDEX(HMI_signals!H:H,B66+1)</f>
-        <v>0</v>
+        <v>HMI1.CB203_Cmd</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -3821,9 +3688,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="str">
         <f>INDEX(HMI_signals!H:H,B67+1)</f>
-        <v>0</v>
+        <v>HMI1.CB203_Cmd</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -3834,9 +3701,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="str">
         <f>INDEX(HMI_signals!H:H,B68+1)</f>
-        <v>0</v>
+        <v>HMI1.CB203_Cmd</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -3847,9 +3714,9 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="str">
         <f>INDEX(HMI_signals!H:H,B69+1)</f>
-        <v>0</v>
+        <v>HMI1.CB203_Cmd</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -4068,9 +3935,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C86">
         <f>INDEX(HMI_signals!H:H,B86+1)</f>
-        <v>HMI1.CB213_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -4081,9 +3948,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C87">
         <f>INDEX(HMI_signals!H:H,B87+1)</f>
-        <v>HMI1.CB213_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -4094,9 +3961,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C88" t="str">
+      <c r="C88">
         <f>INDEX(HMI_signals!H:H,B88+1)</f>
-        <v>HMI1.CB213_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -4107,9 +3974,9 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C89" t="str">
+      <c r="C89">
         <f>INDEX(HMI_signals!H:H,B89+1)</f>
-        <v>HMI1.CB213_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -4224,9 +4091,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C98" t="str">
+      <c r="C98">
         <f>INDEX(HMI_signals!H:H,B98+1)</f>
-        <v>HMI1.CB216_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -4237,9 +4104,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C99" t="str">
+      <c r="C99">
         <f>INDEX(HMI_signals!H:H,B99+1)</f>
-        <v>HMI1.CB216_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -4250,9 +4117,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C100" t="str">
+      <c r="C100">
         <f>INDEX(HMI_signals!H:H,B100+1)</f>
-        <v>HMI1.CB216_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -4263,9 +4130,9 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C101" t="str">
+      <c r="C101">
         <f>INDEX(HMI_signals!H:H,B101+1)</f>
-        <v>HMI1.CB216_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -4276,9 +4143,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C102" t="str">
+      <c r="C102">
         <f>INDEX(HMI_signals!H:H,B102+1)</f>
-        <v>HMI1.CB217_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -4289,9 +4156,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C103" t="str">
+      <c r="C103">
         <f>INDEX(HMI_signals!H:H,B103+1)</f>
-        <v>HMI1.CB217_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -4302,9 +4169,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C104" t="str">
+      <c r="C104">
         <f>INDEX(HMI_signals!H:H,B104+1)</f>
-        <v>HMI1.CB217_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -4315,9 +4182,9 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C105" t="str">
+      <c r="C105">
         <f>INDEX(HMI_signals!H:H,B105+1)</f>
-        <v>HMI1.CB217_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -4328,9 +4195,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C106">
+      <c r="C106" t="str">
         <f>INDEX(HMI_signals!H:H,B106+1)</f>
-        <v>0</v>
+        <v>HMI1.CB213_Cmd</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -4341,9 +4208,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C107">
+      <c r="C107" t="str">
         <f>INDEX(HMI_signals!H:H,B107+1)</f>
-        <v>0</v>
+        <v>HMI1.CB213_Cmd</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -4354,9 +4221,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C108">
+      <c r="C108" t="str">
         <f>INDEX(HMI_signals!H:H,B108+1)</f>
-        <v>0</v>
+        <v>HMI1.CB213_Cmd</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -4367,9 +4234,9 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C109">
+      <c r="C109" t="str">
         <f>INDEX(HMI_signals!H:H,B109+1)</f>
-        <v>0</v>
+        <v>HMI1.CB213_Cmd</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -4432,9 +4299,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C114" t="str">
+      <c r="C114">
         <f>INDEX(HMI_signals!H:H,B114+1)</f>
-        <v>HMI1.CB101_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -4445,9 +4312,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C115" t="str">
+      <c r="C115">
         <f>INDEX(HMI_signals!H:H,B115+1)</f>
-        <v>HMI1.CB101_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -4458,9 +4325,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C116" t="str">
+      <c r="C116">
         <f>INDEX(HMI_signals!H:H,B116+1)</f>
-        <v>HMI1.CB101_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -4471,9 +4338,9 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C117" t="str">
+      <c r="C117">
         <f>INDEX(HMI_signals!H:H,B117+1)</f>
-        <v>HMI1.CB101_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -4486,7 +4353,7 @@
       </c>
       <c r="C118" t="str">
         <f>INDEX(HMI_signals!H:H,B118+1)</f>
-        <v>HMI1.CB102_Cmd</v>
+        <v>HMI1.CB216_Cmd</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -4499,7 +4366,7 @@
       </c>
       <c r="C119" t="str">
         <f>INDEX(HMI_signals!H:H,B119+1)</f>
-        <v>HMI1.CB102_Cmd</v>
+        <v>HMI1.CB216_Cmd</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -4512,7 +4379,7 @@
       </c>
       <c r="C120" t="str">
         <f>INDEX(HMI_signals!H:H,B120+1)</f>
-        <v>HMI1.CB102_Cmd</v>
+        <v>HMI1.CB216_Cmd</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -4525,7 +4392,7 @@
       </c>
       <c r="C121" t="str">
         <f>INDEX(HMI_signals!H:H,B121+1)</f>
-        <v>HMI1.CB102_Cmd</v>
+        <v>HMI1.CB216_Cmd</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -4538,7 +4405,7 @@
       </c>
       <c r="C122" t="str">
         <f>INDEX(HMI_signals!H:H,B122+1)</f>
-        <v>HMI1.CB103_Cmd</v>
+        <v>HMI1.CB217_Cmd</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -4551,7 +4418,7 @@
       </c>
       <c r="C123" t="str">
         <f>INDEX(HMI_signals!H:H,B123+1)</f>
-        <v>HMI1.CB103_Cmd</v>
+        <v>HMI1.CB217_Cmd</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -4564,7 +4431,7 @@
       </c>
       <c r="C124" t="str">
         <f>INDEX(HMI_signals!H:H,B124+1)</f>
-        <v>HMI1.CB103_Cmd</v>
+        <v>HMI1.CB217_Cmd</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -4577,7 +4444,7 @@
       </c>
       <c r="C125" t="str">
         <f>INDEX(HMI_signals!H:H,B125+1)</f>
-        <v>HMI1.CB103_Cmd</v>
+        <v>HMI1.CB217_Cmd</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -4692,9 +4559,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="C134">
+      <c r="C134" t="str">
         <f>INDEX(HMI_signals!H:H,B134+1)</f>
-        <v>0</v>
+        <v>HMI1.CB301_Cmd</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -4705,9 +4572,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="C135">
+      <c r="C135" t="str">
         <f>INDEX(HMI_signals!H:H,B135+1)</f>
-        <v>0</v>
+        <v>HMI1.CB301_Cmd</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -4718,9 +4585,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="C136">
+      <c r="C136" t="str">
         <f>INDEX(HMI_signals!H:H,B136+1)</f>
-        <v>0</v>
+        <v>HMI1.CB301_Cmd</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -4731,9 +4598,9 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="C137">
+      <c r="C137" t="str">
         <f>INDEX(HMI_signals!H:H,B137+1)</f>
-        <v>0</v>
+        <v>HMI1.CB301_Cmd</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -4744,9 +4611,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="C138">
+      <c r="C138" t="str">
         <f>INDEX(HMI_signals!H:H,B138+1)</f>
-        <v>0</v>
+        <v>HMI1.CB302_Cmd</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -4757,9 +4624,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="C139">
+      <c r="C139" t="str">
         <f>INDEX(HMI_signals!H:H,B139+1)</f>
-        <v>0</v>
+        <v>HMI1.CB302_Cmd</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -4770,9 +4637,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="C140">
+      <c r="C140" t="str">
         <f>INDEX(HMI_signals!H:H,B140+1)</f>
-        <v>0</v>
+        <v>HMI1.CB302_Cmd</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -4783,9 +4650,9 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="C141">
+      <c r="C141" t="str">
         <f>INDEX(HMI_signals!H:H,B141+1)</f>
-        <v>0</v>
+        <v>HMI1.CB302_Cmd</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -4798,7 +4665,7 @@
       </c>
       <c r="C142" t="str">
         <f>INDEX(HMI_signals!H:H,B142+1)</f>
-        <v>HMI1.CB108_Cmd</v>
+        <v>HMI1.CB303_Cmd</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
@@ -4811,7 +4678,7 @@
       </c>
       <c r="C143" t="str">
         <f>INDEX(HMI_signals!H:H,B143+1)</f>
-        <v>HMI1.CB108_Cmd</v>
+        <v>HMI1.CB303_Cmd</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -4824,7 +4691,7 @@
       </c>
       <c r="C144" t="str">
         <f>INDEX(HMI_signals!H:H,B144+1)</f>
-        <v>HMI1.CB108_Cmd</v>
+        <v>HMI1.CB303_Cmd</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -4837,7 +4704,7 @@
       </c>
       <c r="C145" t="str">
         <f>INDEX(HMI_signals!H:H,B145+1)</f>
-        <v>HMI1.CB108_Cmd</v>
+        <v>HMI1.CB303_Cmd</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -4850,7 +4717,7 @@
       </c>
       <c r="C146" t="str">
         <f>INDEX(HMI_signals!H:H,B146+1)</f>
-        <v>HMI1.CB109_Cmd</v>
+        <v>HMI1.CB304_Cmd</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -4863,7 +4730,7 @@
       </c>
       <c r="C147" t="str">
         <f>INDEX(HMI_signals!H:H,B147+1)</f>
-        <v>HMI1.CB109_Cmd</v>
+        <v>HMI1.CB304_Cmd</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -4876,7 +4743,7 @@
       </c>
       <c r="C148" t="str">
         <f>INDEX(HMI_signals!H:H,B148+1)</f>
-        <v>HMI1.CB109_Cmd</v>
+        <v>HMI1.CB304_Cmd</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -4889,7 +4756,7 @@
       </c>
       <c r="C149" t="str">
         <f>INDEX(HMI_signals!H:H,B149+1)</f>
-        <v>HMI1.CB109_Cmd</v>
+        <v>HMI1.CB304_Cmd</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -4900,9 +4767,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="C150">
+      <c r="C150" t="str">
         <f>INDEX(HMI_signals!H:H,B150+1)</f>
-        <v>0</v>
+        <v>HMI1.CB305_Cmd</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -4913,9 +4780,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="C151">
+      <c r="C151" t="str">
         <f>INDEX(HMI_signals!H:H,B151+1)</f>
-        <v>0</v>
+        <v>HMI1.CB305_Cmd</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -4926,9 +4793,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="C152">
+      <c r="C152" t="str">
         <f>INDEX(HMI_signals!H:H,B152+1)</f>
-        <v>0</v>
+        <v>HMI1.CB305_Cmd</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -4939,9 +4806,9 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="C153">
+      <c r="C153" t="str">
         <f>INDEX(HMI_signals!H:H,B153+1)</f>
-        <v>0</v>
+        <v>HMI1.CB305_Cmd</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -4952,9 +4819,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="C154" t="str">
+      <c r="C154">
         <f>INDEX(HMI_signals!H:H,B154+1)</f>
-        <v>HMI1.CB111_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -4965,9 +4832,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="C155" t="str">
+      <c r="C155">
         <f>INDEX(HMI_signals!H:H,B155+1)</f>
-        <v>HMI1.CB111_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -4978,9 +4845,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="C156" t="str">
+      <c r="C156">
         <f>INDEX(HMI_signals!H:H,B156+1)</f>
-        <v>HMI1.CB111_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -4991,9 +4858,9 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="C157" t="str">
+      <c r="C157">
         <f>INDEX(HMI_signals!H:H,B157+1)</f>
-        <v>HMI1.CB111_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -5056,9 +4923,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="C162" t="str">
+      <c r="C162">
         <f>INDEX(HMI_signals!H:H,B162+1)</f>
-        <v>HMI1.CB113_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -5069,9 +4936,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="C163" t="str">
+      <c r="C163">
         <f>INDEX(HMI_signals!H:H,B163+1)</f>
-        <v>HMI1.CB113_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -5082,9 +4949,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="C164" t="str">
+      <c r="C164">
         <f>INDEX(HMI_signals!H:H,B164+1)</f>
-        <v>HMI1.CB113_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -5095,9 +4962,9 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="C165" t="str">
+      <c r="C165">
         <f>INDEX(HMI_signals!H:H,B165+1)</f>
-        <v>HMI1.CB113_Cmd</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated HMI with SoC display Corrected CB310 flow scaling Changed UDP mapping to reflect new frame structure
</commit_message>
<xml_diff>
--- a/SimulationTools/RTAC/MGC_SEL_programming.xlsx
+++ b/SimulationTools/RTAC/MGC_SEL_programming.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="312" windowWidth="11016" windowHeight="8736" activeTab="2"/>
+    <workbookView xWindow="288" yWindow="312" windowWidth="11016" windowHeight="8736"/>
   </bookViews>
   <sheets>
     <sheet name="HMI_signals" sheetId="1" r:id="rId1"/>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ60"/>
   <sheetViews>
-    <sheetView topLeftCell="C21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M60"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2234,7 +2234,7 @@
         <v>CB310_MODBUS</v>
       </c>
       <c r="K44">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="12"/>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="6"/>
-        <v>(ID:=43,CBID:=310,Flow:=ADR(HMI1.Flow_310),Pscale:=20,Status:=ADR(HMI1.CB310_Closed),Vpu:=ADR(HMI1.CB310_Vpu),VLgood:=ADR(HMI1.CB310_VLgood)),</v>
+        <v>(ID:=43,CBID:=310,Flow:=ADR(HMI1.Flow_310),Pscale:=1,Status:=ADR(HMI1.CB310_Closed),Vpu:=ADR(HMI1.CB310_Vpu),VLgood:=ADR(HMI1.CB310_VLgood)),</v>
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.3">
@@ -7761,7 +7761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>